<commit_message>
Beginning of UTF-32 parser.
</commit_message>
<xml_diff>
--- a/doc/unicode.xlsx
+++ b/doc/unicode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="16515" windowHeight="7995" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="16515" windowHeight="7995" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="UTF-8 Errors" sheetId="7" r:id="rId1"/>
@@ -1224,14 +1224,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1239,14 +1245,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1750,28 +1750,28 @@
       <c r="I2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="24" t="s">
+      <c r="J2" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
       <c r="M2" s="8" t="s">
         <v>59</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="O2" s="24" t="s">
+      <c r="O2" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24" t="s">
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="T2" s="24"/>
-      <c r="U2" s="24"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="26"/>
       <c r="V2" s="8" t="s">
         <v>63</v>
       </c>
@@ -1861,11 +1861,11 @@
       <c r="I9" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J9" s="22" t="s">
+      <c r="J9" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
       <c r="M9" s="8" t="s">
         <v>119</v>
       </c>
@@ -1913,30 +1913,30 @@
       <c r="B10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I10" s="23" t="s">
+      <c r="I10" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="J10" s="22" t="s">
+      <c r="J10" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="23" t="s">
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="23"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="23"/>
-      <c r="U10" s="23"/>
-      <c r="V10" s="23"/>
-      <c r="W10" s="23"/>
-      <c r="X10" s="23"/>
-      <c r="Y10" s="23"/>
-      <c r="Z10" s="21" t="s">
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="24"/>
+      <c r="S10" s="24"/>
+      <c r="T10" s="24"/>
+      <c r="U10" s="24"/>
+      <c r="V10" s="24"/>
+      <c r="W10" s="24"/>
+      <c r="X10" s="24"/>
+      <c r="Y10" s="24"/>
+      <c r="Z10" s="28" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1944,81 +1944,81 @@
       <c r="B11" t="s">
         <v>3</v>
       </c>
-      <c r="I11" s="23"/>
-      <c r="J11" s="25" t="s">
+      <c r="I11" s="24"/>
+      <c r="J11" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="23"/>
-      <c r="U11" s="23"/>
-      <c r="V11" s="23"/>
-      <c r="W11" s="23"/>
-      <c r="X11" s="23"/>
-      <c r="Y11" s="23"/>
-      <c r="Z11" s="21"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="24"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24"/>
+      <c r="U11" s="24"/>
+      <c r="V11" s="24"/>
+      <c r="W11" s="24"/>
+      <c r="X11" s="24"/>
+      <c r="Y11" s="24"/>
+      <c r="Z11" s="28"/>
     </row>
     <row r="12" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>4</v>
       </c>
-      <c r="I12" s="23"/>
-      <c r="J12" s="22" t="s">
+      <c r="I12" s="24"/>
+      <c r="J12" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="K12" s="22"/>
+      <c r="K12" s="21"/>
       <c r="L12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="23"/>
-      <c r="U12" s="23"/>
-      <c r="V12" s="23"/>
-      <c r="W12" s="23"/>
-      <c r="X12" s="23"/>
-      <c r="Y12" s="23"/>
-      <c r="Z12" s="21"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="24"/>
+      <c r="R12" s="24"/>
+      <c r="S12" s="24"/>
+      <c r="T12" s="24"/>
+      <c r="U12" s="24"/>
+      <c r="V12" s="24"/>
+      <c r="W12" s="24"/>
+      <c r="X12" s="24"/>
+      <c r="Y12" s="24"/>
+      <c r="Z12" s="28"/>
     </row>
     <row r="13" spans="2:26" x14ac:dyDescent="0.25">
       <c r="C13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="23" t="s">
+      <c r="I13" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="J13" s="22" t="s">
+      <c r="J13" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="23" t="s">
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="23"/>
-      <c r="R13" s="23"/>
-      <c r="S13" s="23"/>
-      <c r="T13" s="23"/>
-      <c r="U13" s="23"/>
-      <c r="V13" s="23"/>
-      <c r="W13" s="23"/>
-      <c r="X13" s="23"/>
-      <c r="Y13" s="23"/>
+      <c r="N13" s="24"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="24"/>
+      <c r="Q13" s="24"/>
+      <c r="R13" s="24"/>
+      <c r="S13" s="24"/>
+      <c r="T13" s="24"/>
+      <c r="U13" s="24"/>
+      <c r="V13" s="24"/>
+      <c r="W13" s="24"/>
+      <c r="X13" s="24"/>
+      <c r="Y13" s="24"/>
       <c r="Z13" s="12" t="s">
         <v>127</v>
       </c>
@@ -2027,27 +2027,27 @@
       <c r="C14" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="23"/>
-      <c r="J14" s="25" t="s">
+      <c r="I14" s="24"/>
+      <c r="J14" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="23" t="s">
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="N14" s="23"/>
-      <c r="O14" s="23"/>
-      <c r="P14" s="23"/>
-      <c r="Q14" s="23"/>
-      <c r="R14" s="23"/>
-      <c r="S14" s="23"/>
-      <c r="T14" s="23"/>
-      <c r="U14" s="23"/>
-      <c r="V14" s="23"/>
-      <c r="W14" s="23"/>
-      <c r="X14" s="23"/>
-      <c r="Y14" s="23"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="24"/>
+      <c r="S14" s="24"/>
+      <c r="T14" s="24"/>
+      <c r="U14" s="24"/>
+      <c r="V14" s="24"/>
+      <c r="W14" s="24"/>
+      <c r="X14" s="24"/>
+      <c r="Y14" s="24"/>
       <c r="Z14" s="12" t="s">
         <v>127</v>
       </c>
@@ -2059,26 +2059,26 @@
       <c r="I15" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J15" s="24" t="s">
+      <c r="J15" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="22" t="s">
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="N15" s="22"/>
-      <c r="O15" s="22"/>
-      <c r="P15" s="22"/>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="22"/>
-      <c r="S15" s="22"/>
-      <c r="T15" s="22"/>
-      <c r="U15" s="22"/>
-      <c r="V15" s="22"/>
-      <c r="W15" s="22"/>
-      <c r="X15" s="22"/>
-      <c r="Y15" s="22"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="21"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="21"/>
+      <c r="T15" s="21"/>
+      <c r="U15" s="21"/>
+      <c r="V15" s="21"/>
+      <c r="W15" s="21"/>
+      <c r="X15" s="21"/>
+      <c r="Y15" s="21"/>
       <c r="Z15" s="14" t="s">
         <v>126</v>
       </c>
@@ -2090,26 +2090,26 @@
       <c r="I16" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J16" s="25" t="s">
+      <c r="J16" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
-      <c r="M16" s="23" t="s">
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="23"/>
-      <c r="S16" s="23"/>
-      <c r="T16" s="23"/>
-      <c r="U16" s="23"/>
-      <c r="V16" s="23"/>
-      <c r="W16" s="23"/>
-      <c r="X16" s="23"/>
-      <c r="Y16" s="23"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="24"/>
+      <c r="S16" s="24"/>
+      <c r="T16" s="24"/>
+      <c r="U16" s="24"/>
+      <c r="V16" s="24"/>
+      <c r="W16" s="24"/>
+      <c r="X16" s="24"/>
+      <c r="Y16" s="24"/>
       <c r="Z16" s="12" t="s">
         <v>127</v>
       </c>
@@ -2121,28 +2121,28 @@
       <c r="I17" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J17" s="24" t="s">
+      <c r="J17" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="K17" s="24"/>
+      <c r="K17" s="26"/>
       <c r="L17" t="s">
         <v>55</v>
       </c>
-      <c r="M17" s="22" t="s">
+      <c r="M17" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="N17" s="22"/>
-      <c r="O17" s="22"/>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="22"/>
-      <c r="R17" s="22"/>
-      <c r="S17" s="22"/>
-      <c r="T17" s="22"/>
-      <c r="U17" s="22"/>
-      <c r="V17" s="22"/>
-      <c r="W17" s="22"/>
-      <c r="X17" s="22"/>
-      <c r="Y17" s="22"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="21"/>
+      <c r="Q17" s="21"/>
+      <c r="R17" s="21"/>
+      <c r="S17" s="21"/>
+      <c r="T17" s="21"/>
+      <c r="U17" s="21"/>
+      <c r="V17" s="21"/>
+      <c r="W17" s="21"/>
+      <c r="X17" s="21"/>
+      <c r="Y17" s="21"/>
       <c r="Z17" s="14" t="s">
         <v>126</v>
       </c>
@@ -2154,26 +2154,26 @@
       <c r="I18" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J18" s="25" t="s">
+      <c r="J18" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="23" t="s">
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="N18" s="23"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="23"/>
-      <c r="R18" s="23"/>
-      <c r="S18" s="23"/>
-      <c r="T18" s="23"/>
-      <c r="U18" s="23"/>
-      <c r="V18" s="23"/>
-      <c r="W18" s="23"/>
-      <c r="X18" s="23"/>
-      <c r="Y18" s="23"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="24"/>
+      <c r="S18" s="24"/>
+      <c r="T18" s="24"/>
+      <c r="U18" s="24"/>
+      <c r="V18" s="24"/>
+      <c r="W18" s="24"/>
+      <c r="X18" s="24"/>
+      <c r="Y18" s="24"/>
       <c r="Z18" s="12" t="s">
         <v>127</v>
       </c>
@@ -2185,26 +2185,26 @@
       <c r="I19" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J19" s="27" t="s">
+      <c r="J19" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="K19" s="27"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="23" t="s">
+      <c r="K19" s="25"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="N19" s="23"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="23"/>
-      <c r="Q19" s="23"/>
-      <c r="R19" s="23"/>
-      <c r="S19" s="23"/>
-      <c r="T19" s="23"/>
-      <c r="U19" s="23"/>
-      <c r="V19" s="23"/>
-      <c r="W19" s="23"/>
-      <c r="X19" s="23"/>
-      <c r="Y19" s="23"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="24"/>
+      <c r="Q19" s="24"/>
+      <c r="R19" s="24"/>
+      <c r="S19" s="24"/>
+      <c r="T19" s="24"/>
+      <c r="U19" s="24"/>
+      <c r="V19" s="24"/>
+      <c r="W19" s="24"/>
+      <c r="X19" s="24"/>
+      <c r="Y19" s="24"/>
       <c r="Z19" s="12" t="s">
         <v>127</v>
       </c>
@@ -2216,26 +2216,26 @@
       <c r="I20" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J20" s="24" t="s">
+      <c r="J20" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="22" t="s">
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="N20" s="22"/>
-      <c r="O20" s="22"/>
-      <c r="P20" s="22"/>
-      <c r="Q20" s="22"/>
-      <c r="R20" s="22"/>
-      <c r="S20" s="22"/>
-      <c r="T20" s="22"/>
-      <c r="U20" s="22"/>
-      <c r="V20" s="22"/>
-      <c r="W20" s="22"/>
-      <c r="X20" s="22"/>
-      <c r="Y20" s="22"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="21"/>
+      <c r="Q20" s="21"/>
+      <c r="R20" s="21"/>
+      <c r="S20" s="21"/>
+      <c r="T20" s="21"/>
+      <c r="U20" s="21"/>
+      <c r="V20" s="21"/>
+      <c r="W20" s="21"/>
+      <c r="X20" s="21"/>
+      <c r="Y20" s="21"/>
       <c r="Z20" s="14" t="s">
         <v>126</v>
       </c>
@@ -2247,26 +2247,26 @@
       <c r="I21" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J21" s="25" t="s">
+      <c r="J21" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="23" t="s">
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="N21" s="23"/>
-      <c r="O21" s="23"/>
-      <c r="P21" s="23"/>
-      <c r="Q21" s="23"/>
-      <c r="R21" s="23"/>
-      <c r="S21" s="23"/>
-      <c r="T21" s="23"/>
-      <c r="U21" s="23"/>
-      <c r="V21" s="23"/>
-      <c r="W21" s="23"/>
-      <c r="X21" s="23"/>
-      <c r="Y21" s="23"/>
+      <c r="N21" s="24"/>
+      <c r="O21" s="24"/>
+      <c r="P21" s="24"/>
+      <c r="Q21" s="24"/>
+      <c r="R21" s="24"/>
+      <c r="S21" s="24"/>
+      <c r="T21" s="24"/>
+      <c r="U21" s="24"/>
+      <c r="V21" s="24"/>
+      <c r="W21" s="24"/>
+      <c r="X21" s="24"/>
+      <c r="Y21" s="24"/>
       <c r="Z21" s="12" t="s">
         <v>127</v>
       </c>
@@ -2281,25 +2281,25 @@
       <c r="J22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K22" s="24" t="s">
+      <c r="K22" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="L22" s="24"/>
-      <c r="M22" s="22" t="s">
+      <c r="L22" s="26"/>
+      <c r="M22" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="N22" s="22"/>
-      <c r="O22" s="22"/>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="22"/>
-      <c r="R22" s="22"/>
-      <c r="S22" s="22"/>
-      <c r="T22" s="22"/>
-      <c r="U22" s="22"/>
-      <c r="V22" s="22"/>
-      <c r="W22" s="22"/>
-      <c r="X22" s="22"/>
-      <c r="Y22" s="22"/>
+      <c r="N22" s="21"/>
+      <c r="O22" s="21"/>
+      <c r="P22" s="21"/>
+      <c r="Q22" s="21"/>
+      <c r="R22" s="21"/>
+      <c r="S22" s="21"/>
+      <c r="T22" s="21"/>
+      <c r="U22" s="21"/>
+      <c r="V22" s="21"/>
+      <c r="W22" s="21"/>
+      <c r="X22" s="21"/>
+      <c r="Y22" s="21"/>
       <c r="Z22" s="14" t="s">
         <v>126</v>
       </c>
@@ -2311,26 +2311,26 @@
       <c r="I23" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J23" s="26" t="s">
+      <c r="J23" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="K23" s="26"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="23" t="s">
+      <c r="K23" s="22"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="N23" s="23"/>
-      <c r="O23" s="23"/>
-      <c r="P23" s="23"/>
-      <c r="Q23" s="23"/>
-      <c r="R23" s="23"/>
-      <c r="S23" s="23"/>
-      <c r="T23" s="23"/>
-      <c r="U23" s="23"/>
-      <c r="V23" s="23"/>
-      <c r="W23" s="23"/>
-      <c r="X23" s="23"/>
-      <c r="Y23" s="23"/>
+      <c r="N23" s="24"/>
+      <c r="O23" s="24"/>
+      <c r="P23" s="24"/>
+      <c r="Q23" s="24"/>
+      <c r="R23" s="24"/>
+      <c r="S23" s="24"/>
+      <c r="T23" s="24"/>
+      <c r="U23" s="24"/>
+      <c r="V23" s="24"/>
+      <c r="W23" s="24"/>
+      <c r="X23" s="24"/>
+      <c r="Y23" s="24"/>
       <c r="Z23" s="12" t="s">
         <v>127</v>
       </c>
@@ -2343,26 +2343,26 @@
       <c r="I24" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="J24" s="22" t="s">
+      <c r="J24" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="K24" s="22"/>
-      <c r="L24" s="22"/>
-      <c r="M24" s="22" t="s">
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="N24" s="22"/>
-      <c r="O24" s="22"/>
-      <c r="P24" s="22"/>
-      <c r="Q24" s="22"/>
-      <c r="R24" s="22"/>
-      <c r="S24" s="22"/>
-      <c r="T24" s="22"/>
-      <c r="U24" s="22"/>
-      <c r="V24" s="22"/>
-      <c r="W24" s="22"/>
-      <c r="X24" s="22"/>
-      <c r="Y24" s="22"/>
+      <c r="N24" s="21"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="21"/>
+      <c r="Q24" s="21"/>
+      <c r="R24" s="21"/>
+      <c r="S24" s="21"/>
+      <c r="T24" s="21"/>
+      <c r="U24" s="21"/>
+      <c r="V24" s="21"/>
+      <c r="W24" s="21"/>
+      <c r="X24" s="21"/>
+      <c r="Y24" s="21"/>
       <c r="Z24" s="10" t="s">
         <v>130</v>
       </c>
@@ -2374,26 +2374,26 @@
       <c r="I25" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J25" s="24" t="s">
+      <c r="J25" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="K25" s="24"/>
-      <c r="L25" s="24"/>
-      <c r="M25" s="23" t="s">
+      <c r="K25" s="26"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="N25" s="23"/>
-      <c r="O25" s="23"/>
-      <c r="P25" s="23"/>
-      <c r="Q25" s="23"/>
-      <c r="R25" s="23"/>
-      <c r="S25" s="23"/>
-      <c r="T25" s="23"/>
-      <c r="U25" s="23"/>
-      <c r="V25" s="23"/>
-      <c r="W25" s="23"/>
-      <c r="X25" s="23"/>
-      <c r="Y25" s="23"/>
+      <c r="N25" s="24"/>
+      <c r="O25" s="24"/>
+      <c r="P25" s="24"/>
+      <c r="Q25" s="24"/>
+      <c r="R25" s="24"/>
+      <c r="S25" s="24"/>
+      <c r="T25" s="24"/>
+      <c r="U25" s="24"/>
+      <c r="V25" s="24"/>
+      <c r="W25" s="24"/>
+      <c r="X25" s="24"/>
+      <c r="Y25" s="24"/>
       <c r="Z25" s="12" t="s">
         <v>127</v>
       </c>
@@ -2405,26 +2405,26 @@
       <c r="I26" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="J26" s="25" t="s">
+      <c r="J26" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="K26" s="25"/>
-      <c r="L26" s="25"/>
-      <c r="M26" s="22" t="s">
+      <c r="K26" s="27"/>
+      <c r="L26" s="27"/>
+      <c r="M26" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="N26" s="22"/>
-      <c r="O26" s="22"/>
-      <c r="P26" s="22"/>
-      <c r="Q26" s="22"/>
-      <c r="R26" s="22"/>
-      <c r="S26" s="22"/>
-      <c r="T26" s="22"/>
-      <c r="U26" s="22"/>
-      <c r="V26" s="22"/>
-      <c r="W26" s="22"/>
-      <c r="X26" s="22"/>
-      <c r="Y26" s="22"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="21"/>
+      <c r="P26" s="21"/>
+      <c r="Q26" s="21"/>
+      <c r="R26" s="21"/>
+      <c r="S26" s="21"/>
+      <c r="T26" s="21"/>
+      <c r="U26" s="21"/>
+      <c r="V26" s="21"/>
+      <c r="W26" s="21"/>
+      <c r="X26" s="21"/>
+      <c r="Y26" s="21"/>
       <c r="Z26" s="10" t="s">
         <v>130</v>
       </c>
@@ -2436,26 +2436,26 @@
       <c r="I27" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J27" s="24" t="s">
+      <c r="J27" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="K27" s="24"/>
-      <c r="L27" s="24"/>
-      <c r="M27" s="22" t="s">
+      <c r="K27" s="26"/>
+      <c r="L27" s="26"/>
+      <c r="M27" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="N27" s="22"/>
-      <c r="O27" s="22"/>
-      <c r="P27" s="22"/>
-      <c r="Q27" s="22"/>
-      <c r="R27" s="22"/>
-      <c r="S27" s="22"/>
-      <c r="T27" s="22"/>
-      <c r="U27" s="22"/>
-      <c r="V27" s="22"/>
-      <c r="W27" s="22"/>
-      <c r="X27" s="22"/>
-      <c r="Y27" s="22"/>
+      <c r="N27" s="21"/>
+      <c r="O27" s="21"/>
+      <c r="P27" s="21"/>
+      <c r="Q27" s="21"/>
+      <c r="R27" s="21"/>
+      <c r="S27" s="21"/>
+      <c r="T27" s="21"/>
+      <c r="U27" s="21"/>
+      <c r="V27" s="21"/>
+      <c r="W27" s="21"/>
+      <c r="X27" s="21"/>
+      <c r="Y27" s="21"/>
       <c r="Z27" s="14" t="s">
         <v>126</v>
       </c>
@@ -2467,26 +2467,26 @@
       <c r="I28" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J28" s="24" t="s">
+      <c r="J28" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="K28" s="24"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="23" t="s">
+      <c r="K28" s="26"/>
+      <c r="L28" s="26"/>
+      <c r="M28" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="N28" s="23"/>
-      <c r="O28" s="23"/>
-      <c r="P28" s="23"/>
-      <c r="Q28" s="23"/>
-      <c r="R28" s="23"/>
-      <c r="S28" s="23"/>
-      <c r="T28" s="23"/>
-      <c r="U28" s="23"/>
-      <c r="V28" s="23"/>
-      <c r="W28" s="23"/>
-      <c r="X28" s="23"/>
-      <c r="Y28" s="23"/>
+      <c r="N28" s="24"/>
+      <c r="O28" s="24"/>
+      <c r="P28" s="24"/>
+      <c r="Q28" s="24"/>
+      <c r="R28" s="24"/>
+      <c r="S28" s="24"/>
+      <c r="T28" s="24"/>
+      <c r="U28" s="24"/>
+      <c r="V28" s="24"/>
+      <c r="W28" s="24"/>
+      <c r="X28" s="24"/>
+      <c r="Y28" s="24"/>
       <c r="Z28" s="12" t="s">
         <v>127</v>
       </c>
@@ -2498,26 +2498,26 @@
       <c r="I29" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="J29" s="25" t="s">
+      <c r="J29" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="K29" s="25"/>
-      <c r="L29" s="25"/>
-      <c r="M29" s="22" t="s">
+      <c r="K29" s="27"/>
+      <c r="L29" s="27"/>
+      <c r="M29" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="N29" s="22"/>
-      <c r="O29" s="22"/>
-      <c r="P29" s="22"/>
-      <c r="Q29" s="22"/>
-      <c r="R29" s="22"/>
-      <c r="S29" s="22"/>
-      <c r="T29" s="22"/>
-      <c r="U29" s="22"/>
-      <c r="V29" s="22"/>
-      <c r="W29" s="22"/>
-      <c r="X29" s="22"/>
-      <c r="Y29" s="22"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="21"/>
+      <c r="Q29" s="21"/>
+      <c r="R29" s="21"/>
+      <c r="S29" s="21"/>
+      <c r="T29" s="21"/>
+      <c r="U29" s="21"/>
+      <c r="V29" s="21"/>
+      <c r="W29" s="21"/>
+      <c r="X29" s="21"/>
+      <c r="Y29" s="21"/>
       <c r="Z29" s="10" t="s">
         <v>130</v>
       </c>
@@ -2532,25 +2532,25 @@
       <c r="J30" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K30" s="28" t="s">
+      <c r="K30" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="L30" s="28"/>
-      <c r="M30" s="22" t="s">
+      <c r="L30" s="23"/>
+      <c r="M30" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="N30" s="22"/>
-      <c r="O30" s="22"/>
-      <c r="P30" s="22"/>
-      <c r="Q30" s="22"/>
-      <c r="R30" s="22"/>
-      <c r="S30" s="22"/>
-      <c r="T30" s="22"/>
-      <c r="U30" s="22"/>
-      <c r="V30" s="22"/>
-      <c r="W30" s="22"/>
-      <c r="X30" s="22"/>
-      <c r="Y30" s="22"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="21"/>
+      <c r="Q30" s="21"/>
+      <c r="R30" s="21"/>
+      <c r="S30" s="21"/>
+      <c r="T30" s="21"/>
+      <c r="U30" s="21"/>
+      <c r="V30" s="21"/>
+      <c r="W30" s="21"/>
+      <c r="X30" s="21"/>
+      <c r="Y30" s="21"/>
       <c r="Z30" s="14" t="s">
         <v>126</v>
       </c>
@@ -2562,26 +2562,26 @@
       <c r="I31" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J31" s="24" t="s">
+      <c r="J31" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="23" t="s">
+      <c r="K31" s="26"/>
+      <c r="L31" s="26"/>
+      <c r="M31" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="N31" s="23"/>
-      <c r="O31" s="23"/>
-      <c r="P31" s="23"/>
-      <c r="Q31" s="23"/>
-      <c r="R31" s="23"/>
-      <c r="S31" s="23"/>
-      <c r="T31" s="23"/>
-      <c r="U31" s="23"/>
-      <c r="V31" s="23"/>
-      <c r="W31" s="23"/>
-      <c r="X31" s="23"/>
-      <c r="Y31" s="23"/>
+      <c r="N31" s="24"/>
+      <c r="O31" s="24"/>
+      <c r="P31" s="24"/>
+      <c r="Q31" s="24"/>
+      <c r="R31" s="24"/>
+      <c r="S31" s="24"/>
+      <c r="T31" s="24"/>
+      <c r="U31" s="24"/>
+      <c r="V31" s="24"/>
+      <c r="W31" s="24"/>
+      <c r="X31" s="24"/>
+      <c r="Y31" s="24"/>
       <c r="Z31" s="12" t="s">
         <v>127</v>
       </c>
@@ -2593,26 +2593,26 @@
       <c r="I32" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="J32" s="25" t="s">
+      <c r="J32" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="K32" s="25"/>
-      <c r="L32" s="25"/>
-      <c r="M32" s="22" t="s">
+      <c r="K32" s="27"/>
+      <c r="L32" s="27"/>
+      <c r="M32" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="N32" s="22"/>
-      <c r="O32" s="22"/>
-      <c r="P32" s="22"/>
-      <c r="Q32" s="22"/>
-      <c r="R32" s="22"/>
-      <c r="S32" s="22"/>
-      <c r="T32" s="22"/>
-      <c r="U32" s="22"/>
-      <c r="V32" s="22"/>
-      <c r="W32" s="22"/>
-      <c r="X32" s="22"/>
-      <c r="Y32" s="22"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="21"/>
+      <c r="P32" s="21"/>
+      <c r="Q32" s="21"/>
+      <c r="R32" s="21"/>
+      <c r="S32" s="21"/>
+      <c r="T32" s="21"/>
+      <c r="U32" s="21"/>
+      <c r="V32" s="21"/>
+      <c r="W32" s="21"/>
+      <c r="X32" s="21"/>
+      <c r="Y32" s="21"/>
       <c r="Z32" s="10" t="s">
         <v>130</v>
       </c>
@@ -2624,26 +2624,26 @@
       <c r="I33" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="J33" s="28" t="s">
+      <c r="J33" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="K33" s="28"/>
-      <c r="L33" s="28"/>
-      <c r="M33" s="23" t="s">
+      <c r="K33" s="23"/>
+      <c r="L33" s="23"/>
+      <c r="M33" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="N33" s="23"/>
-      <c r="O33" s="23"/>
-      <c r="P33" s="23"/>
-      <c r="Q33" s="23"/>
-      <c r="R33" s="23"/>
-      <c r="S33" s="23"/>
-      <c r="T33" s="23"/>
-      <c r="U33" s="23"/>
-      <c r="V33" s="23"/>
-      <c r="W33" s="23"/>
-      <c r="X33" s="23"/>
-      <c r="Y33" s="23"/>
+      <c r="N33" s="24"/>
+      <c r="O33" s="24"/>
+      <c r="P33" s="24"/>
+      <c r="Q33" s="24"/>
+      <c r="R33" s="24"/>
+      <c r="S33" s="24"/>
+      <c r="T33" s="24"/>
+      <c r="U33" s="24"/>
+      <c r="V33" s="24"/>
+      <c r="W33" s="24"/>
+      <c r="X33" s="24"/>
+      <c r="Y33" s="24"/>
       <c r="Z33" s="12" t="s">
         <v>127</v>
       </c>
@@ -2656,26 +2656,26 @@
       <c r="I34" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="J34" s="27" t="s">
+      <c r="J34" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="K34" s="27"/>
-      <c r="L34" s="27"/>
-      <c r="M34" s="22" t="s">
+      <c r="K34" s="25"/>
+      <c r="L34" s="25"/>
+      <c r="M34" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="N34" s="22"/>
-      <c r="O34" s="22"/>
-      <c r="P34" s="22"/>
-      <c r="Q34" s="22"/>
-      <c r="R34" s="22"/>
-      <c r="S34" s="22"/>
-      <c r="T34" s="22"/>
-      <c r="U34" s="22"/>
-      <c r="V34" s="22"/>
-      <c r="W34" s="22"/>
-      <c r="X34" s="22"/>
-      <c r="Y34" s="22"/>
+      <c r="N34" s="21"/>
+      <c r="O34" s="21"/>
+      <c r="P34" s="21"/>
+      <c r="Q34" s="21"/>
+      <c r="R34" s="21"/>
+      <c r="S34" s="21"/>
+      <c r="T34" s="21"/>
+      <c r="U34" s="21"/>
+      <c r="V34" s="21"/>
+      <c r="W34" s="21"/>
+      <c r="X34" s="21"/>
+      <c r="Y34" s="21"/>
       <c r="Z34" s="10" t="s">
         <v>130</v>
       </c>
@@ -2691,26 +2691,26 @@
       <c r="I35" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J35" s="26" t="s">
+      <c r="J35" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="K35" s="26"/>
-      <c r="L35" s="26"/>
-      <c r="M35" s="22" t="s">
+      <c r="K35" s="22"/>
+      <c r="L35" s="22"/>
+      <c r="M35" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="N35" s="22"/>
-      <c r="O35" s="22"/>
-      <c r="P35" s="22"/>
-      <c r="Q35" s="22"/>
-      <c r="R35" s="22"/>
-      <c r="S35" s="22"/>
-      <c r="T35" s="22"/>
-      <c r="U35" s="22"/>
-      <c r="V35" s="22"/>
-      <c r="W35" s="22"/>
-      <c r="X35" s="22"/>
-      <c r="Y35" s="22"/>
+      <c r="N35" s="21"/>
+      <c r="O35" s="21"/>
+      <c r="P35" s="21"/>
+      <c r="Q35" s="21"/>
+      <c r="R35" s="21"/>
+      <c r="S35" s="21"/>
+      <c r="T35" s="21"/>
+      <c r="U35" s="21"/>
+      <c r="V35" s="21"/>
+      <c r="W35" s="21"/>
+      <c r="X35" s="21"/>
+      <c r="Y35" s="21"/>
       <c r="Z35" s="14" t="s">
         <v>126</v>
       </c>
@@ -2726,26 +2726,26 @@
       <c r="I36" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J36" s="26" t="s">
+      <c r="J36" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="K36" s="26"/>
-      <c r="L36" s="26"/>
-      <c r="M36" s="23" t="s">
+      <c r="K36" s="22"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="N36" s="23"/>
-      <c r="O36" s="23"/>
-      <c r="P36" s="23"/>
-      <c r="Q36" s="23"/>
-      <c r="R36" s="23"/>
-      <c r="S36" s="23"/>
-      <c r="T36" s="23"/>
-      <c r="U36" s="23"/>
-      <c r="V36" s="23"/>
-      <c r="W36" s="23"/>
-      <c r="X36" s="23"/>
-      <c r="Y36" s="23"/>
+      <c r="N36" s="24"/>
+      <c r="O36" s="24"/>
+      <c r="P36" s="24"/>
+      <c r="Q36" s="24"/>
+      <c r="R36" s="24"/>
+      <c r="S36" s="24"/>
+      <c r="T36" s="24"/>
+      <c r="U36" s="24"/>
+      <c r="V36" s="24"/>
+      <c r="W36" s="24"/>
+      <c r="X36" s="24"/>
+      <c r="Y36" s="24"/>
       <c r="Z36" s="12" t="s">
         <v>127</v>
       </c>
@@ -2761,26 +2761,26 @@
       <c r="I37" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="J37" s="22" t="s">
+      <c r="J37" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="K37" s="22"/>
-      <c r="L37" s="22"/>
-      <c r="M37" s="22" t="s">
+      <c r="K37" s="21"/>
+      <c r="L37" s="21"/>
+      <c r="M37" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="N37" s="22"/>
-      <c r="O37" s="22"/>
-      <c r="P37" s="22"/>
-      <c r="Q37" s="22"/>
-      <c r="R37" s="22"/>
-      <c r="S37" s="22"/>
-      <c r="T37" s="22"/>
-      <c r="U37" s="22"/>
-      <c r="V37" s="22"/>
-      <c r="W37" s="22"/>
-      <c r="X37" s="22"/>
-      <c r="Y37" s="22"/>
+      <c r="N37" s="21"/>
+      <c r="O37" s="21"/>
+      <c r="P37" s="21"/>
+      <c r="Q37" s="21"/>
+      <c r="R37" s="21"/>
+      <c r="S37" s="21"/>
+      <c r="T37" s="21"/>
+      <c r="U37" s="21"/>
+      <c r="V37" s="21"/>
+      <c r="W37" s="21"/>
+      <c r="X37" s="21"/>
+      <c r="Y37" s="21"/>
       <c r="Z37" s="10" t="s">
         <v>130</v>
       </c>
@@ -2796,26 +2796,26 @@
       <c r="I38" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J38" s="26" t="s">
+      <c r="J38" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="K38" s="26"/>
-      <c r="L38" s="26"/>
-      <c r="M38" s="22" t="s">
+      <c r="K38" s="22"/>
+      <c r="L38" s="22"/>
+      <c r="M38" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="N38" s="22"/>
-      <c r="O38" s="22"/>
-      <c r="P38" s="22"/>
-      <c r="Q38" s="22"/>
-      <c r="R38" s="22"/>
-      <c r="S38" s="22"/>
-      <c r="T38" s="22"/>
-      <c r="U38" s="22"/>
-      <c r="V38" s="22"/>
-      <c r="W38" s="22"/>
-      <c r="X38" s="22"/>
-      <c r="Y38" s="22"/>
+      <c r="N38" s="21"/>
+      <c r="O38" s="21"/>
+      <c r="P38" s="21"/>
+      <c r="Q38" s="21"/>
+      <c r="R38" s="21"/>
+      <c r="S38" s="21"/>
+      <c r="T38" s="21"/>
+      <c r="U38" s="21"/>
+      <c r="V38" s="21"/>
+      <c r="W38" s="21"/>
+      <c r="X38" s="21"/>
+      <c r="Y38" s="21"/>
       <c r="Z38" s="14" t="s">
         <v>126</v>
       </c>
@@ -2831,26 +2831,26 @@
       <c r="I39" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J39" s="26" t="s">
+      <c r="J39" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="K39" s="26"/>
-      <c r="L39" s="26"/>
-      <c r="M39" s="23" t="s">
+      <c r="K39" s="22"/>
+      <c r="L39" s="22"/>
+      <c r="M39" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="N39" s="23"/>
-      <c r="O39" s="23"/>
-      <c r="P39" s="23"/>
-      <c r="Q39" s="23"/>
-      <c r="R39" s="23"/>
-      <c r="S39" s="23"/>
-      <c r="T39" s="23"/>
-      <c r="U39" s="23"/>
-      <c r="V39" s="23"/>
-      <c r="W39" s="23"/>
-      <c r="X39" s="23"/>
-      <c r="Y39" s="23"/>
+      <c r="N39" s="24"/>
+      <c r="O39" s="24"/>
+      <c r="P39" s="24"/>
+      <c r="Q39" s="24"/>
+      <c r="R39" s="24"/>
+      <c r="S39" s="24"/>
+      <c r="T39" s="24"/>
+      <c r="U39" s="24"/>
+      <c r="V39" s="24"/>
+      <c r="W39" s="24"/>
+      <c r="X39" s="24"/>
+      <c r="Y39" s="24"/>
       <c r="Z39" s="12" t="s">
         <v>127</v>
       </c>
@@ -2866,26 +2866,26 @@
       <c r="I40" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="J40" s="26" t="s">
+      <c r="J40" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="K40" s="26"/>
-      <c r="L40" s="26"/>
-      <c r="M40" s="22" t="s">
+      <c r="K40" s="22"/>
+      <c r="L40" s="22"/>
+      <c r="M40" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="N40" s="22"/>
-      <c r="O40" s="22"/>
-      <c r="P40" s="22"/>
-      <c r="Q40" s="22"/>
-      <c r="R40" s="22"/>
-      <c r="S40" s="22"/>
-      <c r="T40" s="22"/>
-      <c r="U40" s="22"/>
-      <c r="V40" s="22"/>
-      <c r="W40" s="22"/>
-      <c r="X40" s="22"/>
-      <c r="Y40" s="22"/>
+      <c r="N40" s="21"/>
+      <c r="O40" s="21"/>
+      <c r="P40" s="21"/>
+      <c r="Q40" s="21"/>
+      <c r="R40" s="21"/>
+      <c r="S40" s="21"/>
+      <c r="T40" s="21"/>
+      <c r="U40" s="21"/>
+      <c r="V40" s="21"/>
+      <c r="W40" s="21"/>
+      <c r="X40" s="21"/>
+      <c r="Y40" s="21"/>
       <c r="Z40" s="10" t="s">
         <v>130</v>
       </c>
@@ -2901,26 +2901,26 @@
       <c r="I41" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="J41" s="22" t="s">
+      <c r="J41" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="K41" s="22"/>
-      <c r="L41" s="22"/>
-      <c r="M41" s="22" t="s">
+      <c r="K41" s="21"/>
+      <c r="L41" s="21"/>
+      <c r="M41" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="N41" s="22"/>
-      <c r="O41" s="22"/>
-      <c r="P41" s="22"/>
-      <c r="Q41" s="22"/>
-      <c r="R41" s="22"/>
-      <c r="S41" s="22"/>
-      <c r="T41" s="22"/>
-      <c r="U41" s="22"/>
-      <c r="V41" s="22"/>
-      <c r="W41" s="22"/>
-      <c r="X41" s="22"/>
-      <c r="Y41" s="22"/>
+      <c r="N41" s="21"/>
+      <c r="O41" s="21"/>
+      <c r="P41" s="21"/>
+      <c r="Q41" s="21"/>
+      <c r="R41" s="21"/>
+      <c r="S41" s="21"/>
+      <c r="T41" s="21"/>
+      <c r="U41" s="21"/>
+      <c r="V41" s="21"/>
+      <c r="W41" s="21"/>
+      <c r="X41" s="21"/>
+      <c r="Y41" s="21"/>
       <c r="Z41" s="10" t="s">
         <v>129</v>
       </c>
@@ -2936,26 +2936,26 @@
       <c r="I42" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J42" s="26" t="s">
+      <c r="J42" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="K42" s="26"/>
-      <c r="L42" s="26"/>
-      <c r="M42" s="22" t="s">
+      <c r="K42" s="22"/>
+      <c r="L42" s="22"/>
+      <c r="M42" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="N42" s="22"/>
-      <c r="O42" s="22"/>
-      <c r="P42" s="22"/>
-      <c r="Q42" s="22"/>
-      <c r="R42" s="22"/>
-      <c r="S42" s="22"/>
-      <c r="T42" s="22"/>
-      <c r="U42" s="22"/>
-      <c r="V42" s="22"/>
-      <c r="W42" s="22"/>
-      <c r="X42" s="22"/>
-      <c r="Y42" s="22"/>
+      <c r="N42" s="21"/>
+      <c r="O42" s="21"/>
+      <c r="P42" s="21"/>
+      <c r="Q42" s="21"/>
+      <c r="R42" s="21"/>
+      <c r="S42" s="21"/>
+      <c r="T42" s="21"/>
+      <c r="U42" s="21"/>
+      <c r="V42" s="21"/>
+      <c r="W42" s="21"/>
+      <c r="X42" s="21"/>
+      <c r="Y42" s="21"/>
       <c r="Z42" s="14" t="s">
         <v>126</v>
       </c>
@@ -2971,26 +2971,26 @@
       <c r="I43" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J43" s="26" t="s">
+      <c r="J43" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="K43" s="26"/>
-      <c r="L43" s="26"/>
-      <c r="M43" s="23" t="s">
+      <c r="K43" s="22"/>
+      <c r="L43" s="22"/>
+      <c r="M43" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="N43" s="23"/>
-      <c r="O43" s="23"/>
-      <c r="P43" s="23"/>
-      <c r="Q43" s="23"/>
-      <c r="R43" s="23"/>
-      <c r="S43" s="23"/>
-      <c r="T43" s="23"/>
-      <c r="U43" s="23"/>
-      <c r="V43" s="23"/>
-      <c r="W43" s="23"/>
-      <c r="X43" s="23"/>
-      <c r="Y43" s="23"/>
+      <c r="N43" s="24"/>
+      <c r="O43" s="24"/>
+      <c r="P43" s="24"/>
+      <c r="Q43" s="24"/>
+      <c r="R43" s="24"/>
+      <c r="S43" s="24"/>
+      <c r="T43" s="24"/>
+      <c r="U43" s="24"/>
+      <c r="V43" s="24"/>
+      <c r="W43" s="24"/>
+      <c r="X43" s="24"/>
+      <c r="Y43" s="24"/>
       <c r="Z43" s="12" t="s">
         <v>127</v>
       </c>
@@ -3006,26 +3006,26 @@
       <c r="I44" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="J44" s="26" t="s">
+      <c r="J44" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="K44" s="26"/>
-      <c r="L44" s="26"/>
-      <c r="M44" s="22" t="s">
+      <c r="K44" s="22"/>
+      <c r="L44" s="22"/>
+      <c r="M44" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="N44" s="22"/>
-      <c r="O44" s="22"/>
-      <c r="P44" s="22"/>
-      <c r="Q44" s="22"/>
-      <c r="R44" s="22"/>
-      <c r="S44" s="22"/>
-      <c r="T44" s="22"/>
-      <c r="U44" s="22"/>
-      <c r="V44" s="22"/>
-      <c r="W44" s="22"/>
-      <c r="X44" s="22"/>
-      <c r="Y44" s="22"/>
+      <c r="N44" s="21"/>
+      <c r="O44" s="21"/>
+      <c r="P44" s="21"/>
+      <c r="Q44" s="21"/>
+      <c r="R44" s="21"/>
+      <c r="S44" s="21"/>
+      <c r="T44" s="21"/>
+      <c r="U44" s="21"/>
+      <c r="V44" s="21"/>
+      <c r="W44" s="21"/>
+      <c r="X44" s="21"/>
+      <c r="Y44" s="21"/>
       <c r="Z44" s="10" t="s">
         <v>130</v>
       </c>
@@ -3041,26 +3041,26 @@
       <c r="I45" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="J45" s="26" t="s">
+      <c r="J45" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="K45" s="26"/>
-      <c r="L45" s="26"/>
-      <c r="M45" s="22" t="s">
+      <c r="K45" s="22"/>
+      <c r="L45" s="22"/>
+      <c r="M45" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="N45" s="22"/>
-      <c r="O45" s="22"/>
-      <c r="P45" s="22"/>
-      <c r="Q45" s="22"/>
-      <c r="R45" s="22"/>
-      <c r="S45" s="22"/>
-      <c r="T45" s="22"/>
-      <c r="U45" s="22"/>
-      <c r="V45" s="22"/>
-      <c r="W45" s="22"/>
-      <c r="X45" s="22"/>
-      <c r="Y45" s="22"/>
+      <c r="N45" s="21"/>
+      <c r="O45" s="21"/>
+      <c r="P45" s="21"/>
+      <c r="Q45" s="21"/>
+      <c r="R45" s="21"/>
+      <c r="S45" s="21"/>
+      <c r="T45" s="21"/>
+      <c r="U45" s="21"/>
+      <c r="V45" s="21"/>
+      <c r="W45" s="21"/>
+      <c r="X45" s="21"/>
+      <c r="Y45" s="21"/>
       <c r="Z45" s="10" t="s">
         <v>129</v>
       </c>
@@ -3076,77 +3076,50 @@
       <c r="I46" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="J46" s="22" t="s">
+      <c r="J46" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="K46" s="22"/>
-      <c r="L46" s="22"/>
-      <c r="M46" s="22" t="s">
+      <c r="K46" s="21"/>
+      <c r="L46" s="21"/>
+      <c r="M46" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="N46" s="22"/>
-      <c r="O46" s="22"/>
-      <c r="P46" s="22"/>
-      <c r="Q46" s="22"/>
-      <c r="R46" s="22"/>
-      <c r="S46" s="22"/>
-      <c r="T46" s="22"/>
-      <c r="U46" s="22"/>
-      <c r="V46" s="22"/>
-      <c r="W46" s="22"/>
-      <c r="X46" s="22"/>
-      <c r="Y46" s="22"/>
+      <c r="N46" s="21"/>
+      <c r="O46" s="21"/>
+      <c r="P46" s="21"/>
+      <c r="Q46" s="21"/>
+      <c r="R46" s="21"/>
+      <c r="S46" s="21"/>
+      <c r="T46" s="21"/>
+      <c r="U46" s="21"/>
+      <c r="V46" s="21"/>
+      <c r="W46" s="21"/>
+      <c r="X46" s="21"/>
+      <c r="Y46" s="21"/>
       <c r="Z46" s="10" t="s">
         <v>128</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="79">
-    <mergeCell ref="J46:L46"/>
-    <mergeCell ref="J40:L40"/>
-    <mergeCell ref="J41:L41"/>
-    <mergeCell ref="J42:L42"/>
-    <mergeCell ref="J43:L43"/>
-    <mergeCell ref="J44:L44"/>
-    <mergeCell ref="J45:L45"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="M33:Y33"/>
-    <mergeCell ref="J33:L33"/>
-    <mergeCell ref="J34:L34"/>
-    <mergeCell ref="M34:Y34"/>
-    <mergeCell ref="M46:Y46"/>
-    <mergeCell ref="M43:Y43"/>
-    <mergeCell ref="M40:Y40"/>
-    <mergeCell ref="M39:Y39"/>
-    <mergeCell ref="M38:Y38"/>
-    <mergeCell ref="M42:Y42"/>
-    <mergeCell ref="M44:Y44"/>
-    <mergeCell ref="M41:Y41"/>
-    <mergeCell ref="M45:Y45"/>
-    <mergeCell ref="M23:Y23"/>
-    <mergeCell ref="M24:Y24"/>
-    <mergeCell ref="M26:Y26"/>
-    <mergeCell ref="M29:Y29"/>
-    <mergeCell ref="M32:Y32"/>
-    <mergeCell ref="M25:Y25"/>
-    <mergeCell ref="M28:Y28"/>
-    <mergeCell ref="M31:Y31"/>
-    <mergeCell ref="M27:Y27"/>
-    <mergeCell ref="M30:Y30"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="J37:L37"/>
-    <mergeCell ref="J38:L38"/>
-    <mergeCell ref="J39:L39"/>
-    <mergeCell ref="M37:Y37"/>
-    <mergeCell ref="J31:L31"/>
-    <mergeCell ref="M36:Y36"/>
-    <mergeCell ref="M35:Y35"/>
+    <mergeCell ref="Z10:Z12"/>
+    <mergeCell ref="M17:Y17"/>
+    <mergeCell ref="M20:Y20"/>
+    <mergeCell ref="M22:Y22"/>
+    <mergeCell ref="M16:Y16"/>
+    <mergeCell ref="M18:Y18"/>
+    <mergeCell ref="M19:Y19"/>
+    <mergeCell ref="M21:Y21"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="M13:Y13"/>
+    <mergeCell ref="M14:Y14"/>
+    <mergeCell ref="M10:Y12"/>
+    <mergeCell ref="M15:Y15"/>
+    <mergeCell ref="J12:K12"/>
     <mergeCell ref="I10:I12"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="J32:L32"/>
@@ -3163,24 +3136,51 @@
     <mergeCell ref="J17:K17"/>
     <mergeCell ref="K22:L22"/>
     <mergeCell ref="J16:L16"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="M13:Y13"/>
-    <mergeCell ref="M14:Y14"/>
-    <mergeCell ref="M10:Y12"/>
-    <mergeCell ref="M15:Y15"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="Z10:Z12"/>
-    <mergeCell ref="M17:Y17"/>
-    <mergeCell ref="M20:Y20"/>
-    <mergeCell ref="M22:Y22"/>
-    <mergeCell ref="M16:Y16"/>
-    <mergeCell ref="M18:Y18"/>
-    <mergeCell ref="M19:Y19"/>
-    <mergeCell ref="M21:Y21"/>
+    <mergeCell ref="J37:L37"/>
+    <mergeCell ref="J38:L38"/>
+    <mergeCell ref="J39:L39"/>
+    <mergeCell ref="M37:Y37"/>
+    <mergeCell ref="J31:L31"/>
+    <mergeCell ref="M36:Y36"/>
+    <mergeCell ref="M35:Y35"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="M23:Y23"/>
+    <mergeCell ref="M24:Y24"/>
+    <mergeCell ref="M26:Y26"/>
+    <mergeCell ref="M29:Y29"/>
+    <mergeCell ref="M32:Y32"/>
+    <mergeCell ref="M25:Y25"/>
+    <mergeCell ref="M28:Y28"/>
+    <mergeCell ref="M31:Y31"/>
+    <mergeCell ref="M27:Y27"/>
+    <mergeCell ref="M30:Y30"/>
+    <mergeCell ref="M46:Y46"/>
+    <mergeCell ref="M43:Y43"/>
+    <mergeCell ref="M40:Y40"/>
+    <mergeCell ref="M39:Y39"/>
+    <mergeCell ref="M38:Y38"/>
+    <mergeCell ref="M42:Y42"/>
+    <mergeCell ref="M44:Y44"/>
+    <mergeCell ref="M41:Y41"/>
+    <mergeCell ref="M45:Y45"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="M33:Y33"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="J34:L34"/>
+    <mergeCell ref="M34:Y34"/>
+    <mergeCell ref="J46:L46"/>
+    <mergeCell ref="J40:L40"/>
+    <mergeCell ref="J41:L41"/>
+    <mergeCell ref="J42:L42"/>
+    <mergeCell ref="J43:L43"/>
+    <mergeCell ref="J44:L44"/>
+    <mergeCell ref="J45:L45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3222,28 +3222,28 @@
       <c r="H2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="I2" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
       <c r="L2" s="9" t="s">
         <v>59</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="N2" s="24" t="s">
+      <c r="N2" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24" t="s">
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
       <c r="U2" s="9" t="s">
         <v>63</v>
       </c>
@@ -3333,11 +3333,11 @@
       <c r="H9" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="I9" s="22" t="s">
+      <c r="I9" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
       <c r="L9" s="9" t="s">
         <v>2</v>
       </c>
@@ -3385,30 +3385,30 @@
       <c r="B10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H10" s="23" t="s">
+      <c r="H10" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="I10" s="22" t="s">
+      <c r="I10" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="23" t="s">
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="23"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="23"/>
-      <c r="U10" s="23"/>
-      <c r="V10" s="23"/>
-      <c r="W10" s="23"/>
-      <c r="X10" s="23"/>
-      <c r="Y10" s="21" t="s">
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="24"/>
+      <c r="S10" s="24"/>
+      <c r="T10" s="24"/>
+      <c r="U10" s="24"/>
+      <c r="V10" s="24"/>
+      <c r="W10" s="24"/>
+      <c r="X10" s="24"/>
+      <c r="Y10" s="28" t="s">
         <v>125</v>
       </c>
     </row>
@@ -3416,334 +3416,334 @@
       <c r="B11" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="23"/>
-      <c r="I11" s="25" t="s">
+      <c r="H11" s="24"/>
+      <c r="I11" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="23"/>
-      <c r="U11" s="23"/>
-      <c r="V11" s="23"/>
-      <c r="W11" s="23"/>
-      <c r="X11" s="23"/>
-      <c r="Y11" s="21"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="24"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24"/>
+      <c r="U11" s="24"/>
+      <c r="V11" s="24"/>
+      <c r="W11" s="24"/>
+      <c r="X11" s="24"/>
+      <c r="Y11" s="28"/>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>4</v>
       </c>
-      <c r="H12" s="23"/>
-      <c r="I12" s="26" t="s">
+      <c r="H12" s="24"/>
+      <c r="I12" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="J12" s="22"/>
+      <c r="J12" s="21"/>
       <c r="K12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="23"/>
-      <c r="U12" s="23"/>
-      <c r="V12" s="23"/>
-      <c r="W12" s="23"/>
-      <c r="X12" s="23"/>
-      <c r="Y12" s="21"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="24"/>
+      <c r="R12" s="24"/>
+      <c r="S12" s="24"/>
+      <c r="T12" s="24"/>
+      <c r="U12" s="24"/>
+      <c r="V12" s="24"/>
+      <c r="W12" s="24"/>
+      <c r="X12" s="24"/>
+      <c r="Y12" s="28"/>
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>90</v>
       </c>
       <c r="C13" s="6"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="22" t="s">
+      <c r="H13" s="24"/>
+      <c r="I13" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="23"/>
-      <c r="R13" s="23"/>
-      <c r="S13" s="23"/>
-      <c r="T13" s="23"/>
-      <c r="U13" s="23"/>
-      <c r="V13" s="23"/>
-      <c r="W13" s="23"/>
-      <c r="X13" s="23"/>
-      <c r="Y13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="24"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="24"/>
+      <c r="Q13" s="24"/>
+      <c r="R13" s="24"/>
+      <c r="S13" s="24"/>
+      <c r="T13" s="24"/>
+      <c r="U13" s="24"/>
+      <c r="V13" s="24"/>
+      <c r="W13" s="24"/>
+      <c r="X13" s="24"/>
+      <c r="Y13" s="28"/>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>78</v>
       </c>
-      <c r="H14" s="23"/>
-      <c r="I14" s="25" t="s">
+      <c r="H14" s="24"/>
+      <c r="I14" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="23"/>
-      <c r="P14" s="23"/>
-      <c r="Q14" s="23"/>
-      <c r="R14" s="23"/>
-      <c r="S14" s="23"/>
-      <c r="T14" s="23"/>
-      <c r="U14" s="23"/>
-      <c r="V14" s="23"/>
-      <c r="W14" s="23"/>
-      <c r="X14" s="23"/>
-      <c r="Y14" s="21"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="24"/>
+      <c r="S14" s="24"/>
+      <c r="T14" s="24"/>
+      <c r="U14" s="24"/>
+      <c r="V14" s="24"/>
+      <c r="W14" s="24"/>
+      <c r="X14" s="24"/>
+      <c r="Y14" s="28"/>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>5</v>
       </c>
-      <c r="H15" s="23"/>
-      <c r="I15" s="24" t="s">
+      <c r="H15" s="24"/>
+      <c r="I15" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="23"/>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="23"/>
-      <c r="Q15" s="23"/>
-      <c r="R15" s="23"/>
-      <c r="S15" s="23"/>
-      <c r="T15" s="23"/>
-      <c r="U15" s="23"/>
-      <c r="V15" s="23"/>
-      <c r="W15" s="23"/>
-      <c r="X15" s="23"/>
-      <c r="Y15" s="21"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="24"/>
+      <c r="Q15" s="24"/>
+      <c r="R15" s="24"/>
+      <c r="S15" s="24"/>
+      <c r="T15" s="24"/>
+      <c r="U15" s="24"/>
+      <c r="V15" s="24"/>
+      <c r="W15" s="24"/>
+      <c r="X15" s="24"/>
+      <c r="Y15" s="28"/>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>79</v>
       </c>
-      <c r="H16" s="23"/>
-      <c r="I16" s="25" t="s">
+      <c r="H16" s="24"/>
+      <c r="I16" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="23"/>
-      <c r="S16" s="23"/>
-      <c r="T16" s="23"/>
-      <c r="U16" s="23"/>
-      <c r="V16" s="23"/>
-      <c r="W16" s="23"/>
-      <c r="X16" s="23"/>
-      <c r="Y16" s="21"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="24"/>
+      <c r="S16" s="24"/>
+      <c r="T16" s="24"/>
+      <c r="U16" s="24"/>
+      <c r="V16" s="24"/>
+      <c r="W16" s="24"/>
+      <c r="X16" s="24"/>
+      <c r="Y16" s="28"/>
     </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="23"/>
-      <c r="I17" s="24" t="s">
+      <c r="H17" s="24"/>
+      <c r="I17" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="J17" s="24"/>
+      <c r="J17" s="26"/>
       <c r="K17" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="L17" s="23"/>
-      <c r="M17" s="23"/>
-      <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="23"/>
-      <c r="Q17" s="23"/>
-      <c r="R17" s="23"/>
-      <c r="S17" s="23"/>
-      <c r="T17" s="23"/>
-      <c r="U17" s="23"/>
-      <c r="V17" s="23"/>
-      <c r="W17" s="23"/>
-      <c r="X17" s="23"/>
-      <c r="Y17" s="21"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="24"/>
+      <c r="R17" s="24"/>
+      <c r="S17" s="24"/>
+      <c r="T17" s="24"/>
+      <c r="U17" s="24"/>
+      <c r="V17" s="24"/>
+      <c r="W17" s="24"/>
+      <c r="X17" s="24"/>
+      <c r="Y17" s="28"/>
     </row>
     <row r="18" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>80</v>
       </c>
-      <c r="H18" s="23"/>
-      <c r="I18" s="25" t="s">
+      <c r="H18" s="24"/>
+      <c r="I18" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="23"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="23"/>
-      <c r="R18" s="23"/>
-      <c r="S18" s="23"/>
-      <c r="T18" s="23"/>
-      <c r="U18" s="23"/>
-      <c r="V18" s="23"/>
-      <c r="W18" s="23"/>
-      <c r="X18" s="23"/>
-      <c r="Y18" s="21"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="24"/>
+      <c r="S18" s="24"/>
+      <c r="T18" s="24"/>
+      <c r="U18" s="24"/>
+      <c r="V18" s="24"/>
+      <c r="W18" s="24"/>
+      <c r="X18" s="24"/>
+      <c r="Y18" s="28"/>
     </row>
     <row r="19" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
         <v>91</v>
       </c>
       <c r="C19" s="6"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="27" t="s">
+      <c r="H19" s="24"/>
+      <c r="I19" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="J19" s="27"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="23"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="23"/>
-      <c r="Q19" s="23"/>
-      <c r="R19" s="23"/>
-      <c r="S19" s="23"/>
-      <c r="T19" s="23"/>
-      <c r="U19" s="23"/>
-      <c r="V19" s="23"/>
-      <c r="W19" s="23"/>
-      <c r="X19" s="23"/>
-      <c r="Y19" s="21"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="25"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="24"/>
+      <c r="Q19" s="24"/>
+      <c r="R19" s="24"/>
+      <c r="S19" s="24"/>
+      <c r="T19" s="24"/>
+      <c r="U19" s="24"/>
+      <c r="V19" s="24"/>
+      <c r="W19" s="24"/>
+      <c r="X19" s="24"/>
+      <c r="Y19" s="28"/>
     </row>
     <row r="20" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>7</v>
       </c>
-      <c r="H20" s="23"/>
-      <c r="I20" s="24" t="s">
+      <c r="H20" s="24"/>
+      <c r="I20" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="23"/>
-      <c r="O20" s="23"/>
-      <c r="P20" s="23"/>
-      <c r="Q20" s="23"/>
-      <c r="R20" s="23"/>
-      <c r="S20" s="23"/>
-      <c r="T20" s="23"/>
-      <c r="U20" s="23"/>
-      <c r="V20" s="23"/>
-      <c r="W20" s="23"/>
-      <c r="X20" s="23"/>
-      <c r="Y20" s="21"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="24"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="24"/>
+      <c r="S20" s="24"/>
+      <c r="T20" s="24"/>
+      <c r="U20" s="24"/>
+      <c r="V20" s="24"/>
+      <c r="W20" s="24"/>
+      <c r="X20" s="24"/>
+      <c r="Y20" s="28"/>
     </row>
     <row r="21" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>81</v>
       </c>
-      <c r="H21" s="23"/>
-      <c r="I21" s="25" t="s">
+      <c r="H21" s="24"/>
+      <c r="I21" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="23"/>
-      <c r="N21" s="23"/>
-      <c r="O21" s="23"/>
-      <c r="P21" s="23"/>
-      <c r="Q21" s="23"/>
-      <c r="R21" s="23"/>
-      <c r="S21" s="23"/>
-      <c r="T21" s="23"/>
-      <c r="U21" s="23"/>
-      <c r="V21" s="23"/>
-      <c r="W21" s="23"/>
-      <c r="X21" s="23"/>
-      <c r="Y21" s="21"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
+      <c r="N21" s="24"/>
+      <c r="O21" s="24"/>
+      <c r="P21" s="24"/>
+      <c r="Q21" s="24"/>
+      <c r="R21" s="24"/>
+      <c r="S21" s="24"/>
+      <c r="T21" s="24"/>
+      <c r="U21" s="24"/>
+      <c r="V21" s="24"/>
+      <c r="W21" s="24"/>
+      <c r="X21" s="24"/>
+      <c r="Y21" s="28"/>
     </row>
     <row r="22" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>11</v>
       </c>
-      <c r="H22" s="23"/>
+      <c r="H22" s="24"/>
       <c r="I22" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="J22" s="24" t="s">
+      <c r="J22" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="K22" s="24"/>
-      <c r="L22" s="23"/>
-      <c r="M22" s="23"/>
-      <c r="N22" s="23"/>
-      <c r="O22" s="23"/>
-      <c r="P22" s="23"/>
-      <c r="Q22" s="23"/>
-      <c r="R22" s="23"/>
-      <c r="S22" s="23"/>
-      <c r="T22" s="23"/>
-      <c r="U22" s="23"/>
-      <c r="V22" s="23"/>
-      <c r="W22" s="23"/>
-      <c r="X22" s="23"/>
-      <c r="Y22" s="21"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="24"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="24"/>
+      <c r="Q22" s="24"/>
+      <c r="R22" s="24"/>
+      <c r="S22" s="24"/>
+      <c r="T22" s="24"/>
+      <c r="U22" s="24"/>
+      <c r="V22" s="24"/>
+      <c r="W22" s="24"/>
+      <c r="X22" s="24"/>
+      <c r="Y22" s="28"/>
     </row>
     <row r="23" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C23" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H23" s="23"/>
-      <c r="I23" s="26" t="s">
+      <c r="H23" s="24"/>
+      <c r="I23" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="23"/>
-      <c r="O23" s="23"/>
-      <c r="P23" s="23"/>
-      <c r="Q23" s="23"/>
-      <c r="R23" s="23"/>
-      <c r="S23" s="23"/>
-      <c r="T23" s="23"/>
-      <c r="U23" s="23"/>
-      <c r="V23" s="23"/>
-      <c r="W23" s="23"/>
-      <c r="X23" s="23"/>
-      <c r="Y23" s="21"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="24"/>
+      <c r="N23" s="24"/>
+      <c r="O23" s="24"/>
+      <c r="P23" s="24"/>
+      <c r="Q23" s="24"/>
+      <c r="R23" s="24"/>
+      <c r="S23" s="24"/>
+      <c r="T23" s="24"/>
+      <c r="U23" s="24"/>
+      <c r="V23" s="24"/>
+      <c r="W23" s="24"/>
+      <c r="X23" s="24"/>
+      <c r="Y23" s="28"/>
     </row>
     <row r="24" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
@@ -3751,280 +3751,280 @@
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="22" t="s">
+      <c r="H24" s="24"/>
+      <c r="I24" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="23"/>
-      <c r="M24" s="23"/>
-      <c r="N24" s="23"/>
-      <c r="O24" s="23"/>
-      <c r="P24" s="23"/>
-      <c r="Q24" s="23"/>
-      <c r="R24" s="23"/>
-      <c r="S24" s="23"/>
-      <c r="T24" s="23"/>
-      <c r="U24" s="23"/>
-      <c r="V24" s="23"/>
-      <c r="W24" s="23"/>
-      <c r="X24" s="23"/>
-      <c r="Y24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="24"/>
+      <c r="O24" s="24"/>
+      <c r="P24" s="24"/>
+      <c r="Q24" s="24"/>
+      <c r="R24" s="24"/>
+      <c r="S24" s="24"/>
+      <c r="T24" s="24"/>
+      <c r="U24" s="24"/>
+      <c r="V24" s="24"/>
+      <c r="W24" s="24"/>
+      <c r="X24" s="24"/>
+      <c r="Y24" s="28"/>
     </row>
     <row r="25" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>20</v>
       </c>
-      <c r="H25" s="23"/>
-      <c r="I25" s="24" t="s">
+      <c r="H25" s="24"/>
+      <c r="I25" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="J25" s="24"/>
-      <c r="K25" s="24"/>
-      <c r="L25" s="23"/>
-      <c r="M25" s="23"/>
-      <c r="N25" s="23"/>
-      <c r="O25" s="23"/>
-      <c r="P25" s="23"/>
-      <c r="Q25" s="23"/>
-      <c r="R25" s="23"/>
-      <c r="S25" s="23"/>
-      <c r="T25" s="23"/>
-      <c r="U25" s="23"/>
-      <c r="V25" s="23"/>
-      <c r="W25" s="23"/>
-      <c r="X25" s="23"/>
-      <c r="Y25" s="21"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="24"/>
+      <c r="N25" s="24"/>
+      <c r="O25" s="24"/>
+      <c r="P25" s="24"/>
+      <c r="Q25" s="24"/>
+      <c r="R25" s="24"/>
+      <c r="S25" s="24"/>
+      <c r="T25" s="24"/>
+      <c r="U25" s="24"/>
+      <c r="V25" s="24"/>
+      <c r="W25" s="24"/>
+      <c r="X25" s="24"/>
+      <c r="Y25" s="28"/>
     </row>
     <row r="26" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>82</v>
       </c>
-      <c r="H26" s="23"/>
-      <c r="I26" s="25" t="s">
+      <c r="H26" s="24"/>
+      <c r="I26" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="J26" s="25"/>
-      <c r="K26" s="25"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="23"/>
-      <c r="N26" s="23"/>
-      <c r="O26" s="23"/>
-      <c r="P26" s="23"/>
-      <c r="Q26" s="23"/>
-      <c r="R26" s="23"/>
-      <c r="S26" s="23"/>
-      <c r="T26" s="23"/>
-      <c r="U26" s="23"/>
-      <c r="V26" s="23"/>
-      <c r="W26" s="23"/>
-      <c r="X26" s="23"/>
-      <c r="Y26" s="21"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
+      <c r="N26" s="24"/>
+      <c r="O26" s="24"/>
+      <c r="P26" s="24"/>
+      <c r="Q26" s="24"/>
+      <c r="R26" s="24"/>
+      <c r="S26" s="24"/>
+      <c r="T26" s="24"/>
+      <c r="U26" s="24"/>
+      <c r="V26" s="24"/>
+      <c r="W26" s="24"/>
+      <c r="X26" s="24"/>
+      <c r="Y26" s="28"/>
     </row>
     <row r="27" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>12</v>
       </c>
-      <c r="H27" s="23"/>
-      <c r="I27" s="24" t="s">
+      <c r="H27" s="24"/>
+      <c r="I27" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="J27" s="24"/>
-      <c r="K27" s="24"/>
-      <c r="L27" s="23"/>
-      <c r="M27" s="23"/>
-      <c r="N27" s="23"/>
-      <c r="O27" s="23"/>
-      <c r="P27" s="23"/>
-      <c r="Q27" s="23"/>
-      <c r="R27" s="23"/>
-      <c r="S27" s="23"/>
-      <c r="T27" s="23"/>
-      <c r="U27" s="23"/>
-      <c r="V27" s="23"/>
-      <c r="W27" s="23"/>
-      <c r="X27" s="23"/>
-      <c r="Y27" s="21"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="24"/>
+      <c r="M27" s="24"/>
+      <c r="N27" s="24"/>
+      <c r="O27" s="24"/>
+      <c r="P27" s="24"/>
+      <c r="Q27" s="24"/>
+      <c r="R27" s="24"/>
+      <c r="S27" s="24"/>
+      <c r="T27" s="24"/>
+      <c r="U27" s="24"/>
+      <c r="V27" s="24"/>
+      <c r="W27" s="24"/>
+      <c r="X27" s="24"/>
+      <c r="Y27" s="28"/>
     </row>
     <row r="28" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>9</v>
       </c>
-      <c r="H28" s="23"/>
-      <c r="I28" s="24" t="s">
+      <c r="H28" s="24"/>
+      <c r="I28" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="J28" s="24"/>
-      <c r="K28" s="24"/>
-      <c r="L28" s="23"/>
-      <c r="M28" s="23"/>
-      <c r="N28" s="23"/>
-      <c r="O28" s="23"/>
-      <c r="P28" s="23"/>
-      <c r="Q28" s="23"/>
-      <c r="R28" s="23"/>
-      <c r="S28" s="23"/>
-      <c r="T28" s="23"/>
-      <c r="U28" s="23"/>
-      <c r="V28" s="23"/>
-      <c r="W28" s="23"/>
-      <c r="X28" s="23"/>
-      <c r="Y28" s="21"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="24"/>
+      <c r="N28" s="24"/>
+      <c r="O28" s="24"/>
+      <c r="P28" s="24"/>
+      <c r="Q28" s="24"/>
+      <c r="R28" s="24"/>
+      <c r="S28" s="24"/>
+      <c r="T28" s="24"/>
+      <c r="U28" s="24"/>
+      <c r="V28" s="24"/>
+      <c r="W28" s="24"/>
+      <c r="X28" s="24"/>
+      <c r="Y28" s="28"/>
     </row>
     <row r="29" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>83</v>
       </c>
-      <c r="H29" s="23"/>
-      <c r="I29" s="25" t="s">
+      <c r="H29" s="24"/>
+      <c r="I29" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="J29" s="25"/>
-      <c r="K29" s="25"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
-      <c r="P29" s="23"/>
-      <c r="Q29" s="23"/>
-      <c r="R29" s="23"/>
-      <c r="S29" s="23"/>
-      <c r="T29" s="23"/>
-      <c r="U29" s="23"/>
-      <c r="V29" s="23"/>
-      <c r="W29" s="23"/>
-      <c r="X29" s="23"/>
-      <c r="Y29" s="21"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="24"/>
+      <c r="N29" s="24"/>
+      <c r="O29" s="24"/>
+      <c r="P29" s="24"/>
+      <c r="Q29" s="24"/>
+      <c r="R29" s="24"/>
+      <c r="S29" s="24"/>
+      <c r="T29" s="24"/>
+      <c r="U29" s="24"/>
+      <c r="V29" s="24"/>
+      <c r="W29" s="24"/>
+      <c r="X29" s="24"/>
+      <c r="Y29" s="28"/>
     </row>
     <row r="30" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>13</v>
       </c>
-      <c r="H30" s="23"/>
+      <c r="H30" s="24"/>
       <c r="I30" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J30" s="28" t="s">
+      <c r="J30" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="K30" s="28"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="23"/>
-      <c r="N30" s="23"/>
-      <c r="O30" s="23"/>
-      <c r="P30" s="23"/>
-      <c r="Q30" s="23"/>
-      <c r="R30" s="23"/>
-      <c r="S30" s="23"/>
-      <c r="T30" s="23"/>
-      <c r="U30" s="23"/>
-      <c r="V30" s="23"/>
-      <c r="W30" s="23"/>
-      <c r="X30" s="23"/>
-      <c r="Y30" s="21"/>
+      <c r="K30" s="23"/>
+      <c r="L30" s="24"/>
+      <c r="M30" s="24"/>
+      <c r="N30" s="24"/>
+      <c r="O30" s="24"/>
+      <c r="P30" s="24"/>
+      <c r="Q30" s="24"/>
+      <c r="R30" s="24"/>
+      <c r="S30" s="24"/>
+      <c r="T30" s="24"/>
+      <c r="U30" s="24"/>
+      <c r="V30" s="24"/>
+      <c r="W30" s="24"/>
+      <c r="X30" s="24"/>
+      <c r="Y30" s="28"/>
     </row>
     <row r="31" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>19</v>
       </c>
-      <c r="H31" s="23"/>
-      <c r="I31" s="24" t="s">
+      <c r="H31" s="24"/>
+      <c r="I31" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="J31" s="24"/>
-      <c r="K31" s="24"/>
-      <c r="L31" s="23"/>
-      <c r="M31" s="23"/>
-      <c r="N31" s="23"/>
-      <c r="O31" s="23"/>
-      <c r="P31" s="23"/>
-      <c r="Q31" s="23"/>
-      <c r="R31" s="23"/>
-      <c r="S31" s="23"/>
-      <c r="T31" s="23"/>
-      <c r="U31" s="23"/>
-      <c r="V31" s="23"/>
-      <c r="W31" s="23"/>
-      <c r="X31" s="23"/>
-      <c r="Y31" s="21"/>
+      <c r="J31" s="26"/>
+      <c r="K31" s="26"/>
+      <c r="L31" s="24"/>
+      <c r="M31" s="24"/>
+      <c r="N31" s="24"/>
+      <c r="O31" s="24"/>
+      <c r="P31" s="24"/>
+      <c r="Q31" s="24"/>
+      <c r="R31" s="24"/>
+      <c r="S31" s="24"/>
+      <c r="T31" s="24"/>
+      <c r="U31" s="24"/>
+      <c r="V31" s="24"/>
+      <c r="W31" s="24"/>
+      <c r="X31" s="24"/>
+      <c r="Y31" s="28"/>
     </row>
     <row r="32" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>85</v>
       </c>
-      <c r="H32" s="23"/>
-      <c r="I32" s="25" t="s">
+      <c r="H32" s="24"/>
+      <c r="I32" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="J32" s="25"/>
-      <c r="K32" s="25"/>
-      <c r="L32" s="23"/>
-      <c r="M32" s="23"/>
-      <c r="N32" s="23"/>
-      <c r="O32" s="23"/>
-      <c r="P32" s="23"/>
-      <c r="Q32" s="23"/>
-      <c r="R32" s="23"/>
-      <c r="S32" s="23"/>
-      <c r="T32" s="23"/>
-      <c r="U32" s="23"/>
-      <c r="V32" s="23"/>
-      <c r="W32" s="23"/>
-      <c r="X32" s="23"/>
-      <c r="Y32" s="21"/>
+      <c r="J32" s="27"/>
+      <c r="K32" s="27"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="24"/>
+      <c r="N32" s="24"/>
+      <c r="O32" s="24"/>
+      <c r="P32" s="24"/>
+      <c r="Q32" s="24"/>
+      <c r="R32" s="24"/>
+      <c r="S32" s="24"/>
+      <c r="T32" s="24"/>
+      <c r="U32" s="24"/>
+      <c r="V32" s="24"/>
+      <c r="W32" s="24"/>
+      <c r="X32" s="24"/>
+      <c r="Y32" s="28"/>
     </row>
     <row r="33" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
         <v>84</v>
       </c>
       <c r="C33" s="6"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="28" t="s">
+      <c r="H33" s="24"/>
+      <c r="I33" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="J33" s="28"/>
-      <c r="K33" s="28"/>
-      <c r="L33" s="23"/>
-      <c r="M33" s="23"/>
-      <c r="N33" s="23"/>
-      <c r="O33" s="23"/>
-      <c r="P33" s="23"/>
-      <c r="Q33" s="23"/>
-      <c r="R33" s="23"/>
-      <c r="S33" s="23"/>
-      <c r="T33" s="23"/>
-      <c r="U33" s="23"/>
-      <c r="V33" s="23"/>
-      <c r="W33" s="23"/>
-      <c r="X33" s="23"/>
-      <c r="Y33" s="21"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="23"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="24"/>
+      <c r="N33" s="24"/>
+      <c r="O33" s="24"/>
+      <c r="P33" s="24"/>
+      <c r="Q33" s="24"/>
+      <c r="R33" s="24"/>
+      <c r="S33" s="24"/>
+      <c r="T33" s="24"/>
+      <c r="U33" s="24"/>
+      <c r="V33" s="24"/>
+      <c r="W33" s="24"/>
+      <c r="X33" s="24"/>
+      <c r="Y33" s="28"/>
     </row>
     <row r="34" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="s">
         <v>118</v>
       </c>
       <c r="C34" s="6"/>
-      <c r="H34" s="23"/>
-      <c r="I34" s="27" t="s">
+      <c r="H34" s="24"/>
+      <c r="I34" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="J34" s="27"/>
-      <c r="K34" s="27"/>
-      <c r="L34" s="23"/>
-      <c r="M34" s="23"/>
-      <c r="N34" s="23"/>
-      <c r="O34" s="23"/>
-      <c r="P34" s="23"/>
-      <c r="Q34" s="23"/>
-      <c r="R34" s="23"/>
-      <c r="S34" s="23"/>
-      <c r="T34" s="23"/>
-      <c r="U34" s="23"/>
-      <c r="V34" s="23"/>
-      <c r="W34" s="23"/>
-      <c r="X34" s="23"/>
-      <c r="Y34" s="21"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="25"/>
+      <c r="L34" s="24"/>
+      <c r="M34" s="24"/>
+      <c r="N34" s="24"/>
+      <c r="O34" s="24"/>
+      <c r="P34" s="24"/>
+      <c r="Q34" s="24"/>
+      <c r="R34" s="24"/>
+      <c r="S34" s="24"/>
+      <c r="T34" s="24"/>
+      <c r="U34" s="24"/>
+      <c r="V34" s="24"/>
+      <c r="W34" s="24"/>
+      <c r="X34" s="24"/>
+      <c r="Y34" s="28"/>
     </row>
     <row r="35" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
@@ -4033,26 +4033,26 @@
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="26" t="s">
+      <c r="H35" s="24"/>
+      <c r="I35" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="J35" s="26"/>
-      <c r="K35" s="26"/>
-      <c r="L35" s="23"/>
-      <c r="M35" s="23"/>
-      <c r="N35" s="23"/>
-      <c r="O35" s="23"/>
-      <c r="P35" s="23"/>
-      <c r="Q35" s="23"/>
-      <c r="R35" s="23"/>
-      <c r="S35" s="23"/>
-      <c r="T35" s="23"/>
-      <c r="U35" s="23"/>
-      <c r="V35" s="23"/>
-      <c r="W35" s="23"/>
-      <c r="X35" s="23"/>
-      <c r="Y35" s="21"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+      <c r="L35" s="24"/>
+      <c r="M35" s="24"/>
+      <c r="N35" s="24"/>
+      <c r="O35" s="24"/>
+      <c r="P35" s="24"/>
+      <c r="Q35" s="24"/>
+      <c r="R35" s="24"/>
+      <c r="S35" s="24"/>
+      <c r="T35" s="24"/>
+      <c r="U35" s="24"/>
+      <c r="V35" s="24"/>
+      <c r="W35" s="24"/>
+      <c r="X35" s="24"/>
+      <c r="Y35" s="28"/>
     </row>
     <row r="36" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B36" s="6"/>
@@ -4061,26 +4061,26 @@
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
-      <c r="H36" s="23"/>
-      <c r="I36" s="26" t="s">
+      <c r="H36" s="24"/>
+      <c r="I36" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="J36" s="26"/>
-      <c r="K36" s="26"/>
-      <c r="L36" s="23"/>
-      <c r="M36" s="23"/>
-      <c r="N36" s="23"/>
-      <c r="O36" s="23"/>
-      <c r="P36" s="23"/>
-      <c r="Q36" s="23"/>
-      <c r="R36" s="23"/>
-      <c r="S36" s="23"/>
-      <c r="T36" s="23"/>
-      <c r="U36" s="23"/>
-      <c r="V36" s="23"/>
-      <c r="W36" s="23"/>
-      <c r="X36" s="23"/>
-      <c r="Y36" s="21"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="22"/>
+      <c r="L36" s="24"/>
+      <c r="M36" s="24"/>
+      <c r="N36" s="24"/>
+      <c r="O36" s="24"/>
+      <c r="P36" s="24"/>
+      <c r="Q36" s="24"/>
+      <c r="R36" s="24"/>
+      <c r="S36" s="24"/>
+      <c r="T36" s="24"/>
+      <c r="U36" s="24"/>
+      <c r="V36" s="24"/>
+      <c r="W36" s="24"/>
+      <c r="X36" s="24"/>
+      <c r="Y36" s="28"/>
     </row>
     <row r="37" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
@@ -4089,26 +4089,26 @@
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
-      <c r="H37" s="23"/>
-      <c r="I37" s="22" t="s">
+      <c r="H37" s="24"/>
+      <c r="I37" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="J37" s="22"/>
-      <c r="K37" s="22"/>
-      <c r="L37" s="23"/>
-      <c r="M37" s="23"/>
-      <c r="N37" s="23"/>
-      <c r="O37" s="23"/>
-      <c r="P37" s="23"/>
-      <c r="Q37" s="23"/>
-      <c r="R37" s="23"/>
-      <c r="S37" s="23"/>
-      <c r="T37" s="23"/>
-      <c r="U37" s="23"/>
-      <c r="V37" s="23"/>
-      <c r="W37" s="23"/>
-      <c r="X37" s="23"/>
-      <c r="Y37" s="21"/>
+      <c r="J37" s="21"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="24"/>
+      <c r="M37" s="24"/>
+      <c r="N37" s="24"/>
+      <c r="O37" s="24"/>
+      <c r="P37" s="24"/>
+      <c r="Q37" s="24"/>
+      <c r="R37" s="24"/>
+      <c r="S37" s="24"/>
+      <c r="T37" s="24"/>
+      <c r="U37" s="24"/>
+      <c r="V37" s="24"/>
+      <c r="W37" s="24"/>
+      <c r="X37" s="24"/>
+      <c r="Y37" s="28"/>
     </row>
     <row r="38" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
@@ -4117,26 +4117,26 @@
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
-      <c r="H38" s="23"/>
-      <c r="I38" s="26" t="s">
+      <c r="H38" s="24"/>
+      <c r="I38" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="J38" s="26"/>
-      <c r="K38" s="26"/>
-      <c r="L38" s="23"/>
-      <c r="M38" s="23"/>
-      <c r="N38" s="23"/>
-      <c r="O38" s="23"/>
-      <c r="P38" s="23"/>
-      <c r="Q38" s="23"/>
-      <c r="R38" s="23"/>
-      <c r="S38" s="23"/>
-      <c r="T38" s="23"/>
-      <c r="U38" s="23"/>
-      <c r="V38" s="23"/>
-      <c r="W38" s="23"/>
-      <c r="X38" s="23"/>
-      <c r="Y38" s="21"/>
+      <c r="J38" s="22"/>
+      <c r="K38" s="22"/>
+      <c r="L38" s="24"/>
+      <c r="M38" s="24"/>
+      <c r="N38" s="24"/>
+      <c r="O38" s="24"/>
+      <c r="P38" s="24"/>
+      <c r="Q38" s="24"/>
+      <c r="R38" s="24"/>
+      <c r="S38" s="24"/>
+      <c r="T38" s="24"/>
+      <c r="U38" s="24"/>
+      <c r="V38" s="24"/>
+      <c r="W38" s="24"/>
+      <c r="X38" s="24"/>
+      <c r="Y38" s="28"/>
     </row>
     <row r="39" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B39" s="6"/>
@@ -4145,26 +4145,26 @@
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
-      <c r="H39" s="23"/>
-      <c r="I39" s="26" t="s">
+      <c r="H39" s="24"/>
+      <c r="I39" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="J39" s="26"/>
-      <c r="K39" s="26"/>
-      <c r="L39" s="23"/>
-      <c r="M39" s="23"/>
-      <c r="N39" s="23"/>
-      <c r="O39" s="23"/>
-      <c r="P39" s="23"/>
-      <c r="Q39" s="23"/>
-      <c r="R39" s="23"/>
-      <c r="S39" s="23"/>
-      <c r="T39" s="23"/>
-      <c r="U39" s="23"/>
-      <c r="V39" s="23"/>
-      <c r="W39" s="23"/>
-      <c r="X39" s="23"/>
-      <c r="Y39" s="21"/>
+      <c r="J39" s="22"/>
+      <c r="K39" s="22"/>
+      <c r="L39" s="24"/>
+      <c r="M39" s="24"/>
+      <c r="N39" s="24"/>
+      <c r="O39" s="24"/>
+      <c r="P39" s="24"/>
+      <c r="Q39" s="24"/>
+      <c r="R39" s="24"/>
+      <c r="S39" s="24"/>
+      <c r="T39" s="24"/>
+      <c r="U39" s="24"/>
+      <c r="V39" s="24"/>
+      <c r="W39" s="24"/>
+      <c r="X39" s="24"/>
+      <c r="Y39" s="28"/>
     </row>
     <row r="40" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B40" s="6"/>
@@ -4173,26 +4173,26 @@
         <v>9</v>
       </c>
       <c r="E40" s="6"/>
-      <c r="H40" s="23"/>
-      <c r="I40" s="26" t="s">
+      <c r="H40" s="24"/>
+      <c r="I40" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="J40" s="26"/>
-      <c r="K40" s="26"/>
-      <c r="L40" s="23"/>
-      <c r="M40" s="23"/>
-      <c r="N40" s="23"/>
-      <c r="O40" s="23"/>
-      <c r="P40" s="23"/>
-      <c r="Q40" s="23"/>
-      <c r="R40" s="23"/>
-      <c r="S40" s="23"/>
-      <c r="T40" s="23"/>
-      <c r="U40" s="23"/>
-      <c r="V40" s="23"/>
-      <c r="W40" s="23"/>
-      <c r="X40" s="23"/>
-      <c r="Y40" s="21"/>
+      <c r="J40" s="22"/>
+      <c r="K40" s="22"/>
+      <c r="L40" s="24"/>
+      <c r="M40" s="24"/>
+      <c r="N40" s="24"/>
+      <c r="O40" s="24"/>
+      <c r="P40" s="24"/>
+      <c r="Q40" s="24"/>
+      <c r="R40" s="24"/>
+      <c r="S40" s="24"/>
+      <c r="T40" s="24"/>
+      <c r="U40" s="24"/>
+      <c r="V40" s="24"/>
+      <c r="W40" s="24"/>
+      <c r="X40" s="24"/>
+      <c r="Y40" s="28"/>
     </row>
     <row r="41" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
@@ -4201,26 +4201,26 @@
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
-      <c r="H41" s="23"/>
-      <c r="I41" s="22" t="s">
+      <c r="H41" s="24"/>
+      <c r="I41" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="J41" s="22"/>
-      <c r="K41" s="22"/>
-      <c r="L41" s="23"/>
-      <c r="M41" s="23"/>
-      <c r="N41" s="23"/>
-      <c r="O41" s="23"/>
-      <c r="P41" s="23"/>
-      <c r="Q41" s="23"/>
-      <c r="R41" s="23"/>
-      <c r="S41" s="23"/>
-      <c r="T41" s="23"/>
-      <c r="U41" s="23"/>
-      <c r="V41" s="23"/>
-      <c r="W41" s="23"/>
-      <c r="X41" s="23"/>
-      <c r="Y41" s="21"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="21"/>
+      <c r="L41" s="24"/>
+      <c r="M41" s="24"/>
+      <c r="N41" s="24"/>
+      <c r="O41" s="24"/>
+      <c r="P41" s="24"/>
+      <c r="Q41" s="24"/>
+      <c r="R41" s="24"/>
+      <c r="S41" s="24"/>
+      <c r="T41" s="24"/>
+      <c r="U41" s="24"/>
+      <c r="V41" s="24"/>
+      <c r="W41" s="24"/>
+      <c r="X41" s="24"/>
+      <c r="Y41" s="28"/>
     </row>
     <row r="42" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
@@ -4229,26 +4229,26 @@
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
-      <c r="H42" s="23"/>
-      <c r="I42" s="26" t="s">
+      <c r="H42" s="24"/>
+      <c r="I42" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="J42" s="26"/>
-      <c r="K42" s="26"/>
-      <c r="L42" s="23"/>
-      <c r="M42" s="23"/>
-      <c r="N42" s="23"/>
-      <c r="O42" s="23"/>
-      <c r="P42" s="23"/>
-      <c r="Q42" s="23"/>
-      <c r="R42" s="23"/>
-      <c r="S42" s="23"/>
-      <c r="T42" s="23"/>
-      <c r="U42" s="23"/>
-      <c r="V42" s="23"/>
-      <c r="W42" s="23"/>
-      <c r="X42" s="23"/>
-      <c r="Y42" s="21"/>
+      <c r="J42" s="22"/>
+      <c r="K42" s="22"/>
+      <c r="L42" s="24"/>
+      <c r="M42" s="24"/>
+      <c r="N42" s="24"/>
+      <c r="O42" s="24"/>
+      <c r="P42" s="24"/>
+      <c r="Q42" s="24"/>
+      <c r="R42" s="24"/>
+      <c r="S42" s="24"/>
+      <c r="T42" s="24"/>
+      <c r="U42" s="24"/>
+      <c r="V42" s="24"/>
+      <c r="W42" s="24"/>
+      <c r="X42" s="24"/>
+      <c r="Y42" s="28"/>
     </row>
     <row r="43" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
@@ -4257,26 +4257,26 @@
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="26" t="s">
+      <c r="H43" s="24"/>
+      <c r="I43" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="J43" s="26"/>
-      <c r="K43" s="26"/>
-      <c r="L43" s="23"/>
-      <c r="M43" s="23"/>
-      <c r="N43" s="23"/>
-      <c r="O43" s="23"/>
-      <c r="P43" s="23"/>
-      <c r="Q43" s="23"/>
-      <c r="R43" s="23"/>
-      <c r="S43" s="23"/>
-      <c r="T43" s="23"/>
-      <c r="U43" s="23"/>
-      <c r="V43" s="23"/>
-      <c r="W43" s="23"/>
-      <c r="X43" s="23"/>
-      <c r="Y43" s="21"/>
+      <c r="J43" s="22"/>
+      <c r="K43" s="22"/>
+      <c r="L43" s="24"/>
+      <c r="M43" s="24"/>
+      <c r="N43" s="24"/>
+      <c r="O43" s="24"/>
+      <c r="P43" s="24"/>
+      <c r="Q43" s="24"/>
+      <c r="R43" s="24"/>
+      <c r="S43" s="24"/>
+      <c r="T43" s="24"/>
+      <c r="U43" s="24"/>
+      <c r="V43" s="24"/>
+      <c r="W43" s="24"/>
+      <c r="X43" s="24"/>
+      <c r="Y43" s="28"/>
     </row>
     <row r="44" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B44" s="6"/>
@@ -4285,26 +4285,26 @@
         <v>9</v>
       </c>
       <c r="E44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="26" t="s">
+      <c r="H44" s="24"/>
+      <c r="I44" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="J44" s="26"/>
-      <c r="K44" s="26"/>
-      <c r="L44" s="23"/>
-      <c r="M44" s="23"/>
-      <c r="N44" s="23"/>
-      <c r="O44" s="23"/>
-      <c r="P44" s="23"/>
-      <c r="Q44" s="23"/>
-      <c r="R44" s="23"/>
-      <c r="S44" s="23"/>
-      <c r="T44" s="23"/>
-      <c r="U44" s="23"/>
-      <c r="V44" s="23"/>
-      <c r="W44" s="23"/>
-      <c r="X44" s="23"/>
-      <c r="Y44" s="21"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="22"/>
+      <c r="L44" s="24"/>
+      <c r="M44" s="24"/>
+      <c r="N44" s="24"/>
+      <c r="O44" s="24"/>
+      <c r="P44" s="24"/>
+      <c r="Q44" s="24"/>
+      <c r="R44" s="24"/>
+      <c r="S44" s="24"/>
+      <c r="T44" s="24"/>
+      <c r="U44" s="24"/>
+      <c r="V44" s="24"/>
+      <c r="W44" s="24"/>
+      <c r="X44" s="24"/>
+      <c r="Y44" s="28"/>
     </row>
     <row r="45" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B45" s="6"/>
@@ -4313,26 +4313,26 @@
       <c r="E45" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H45" s="23"/>
-      <c r="I45" s="26" t="s">
+      <c r="H45" s="24"/>
+      <c r="I45" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="J45" s="26"/>
-      <c r="K45" s="26"/>
-      <c r="L45" s="23"/>
-      <c r="M45" s="23"/>
-      <c r="N45" s="23"/>
-      <c r="O45" s="23"/>
-      <c r="P45" s="23"/>
-      <c r="Q45" s="23"/>
-      <c r="R45" s="23"/>
-      <c r="S45" s="23"/>
-      <c r="T45" s="23"/>
-      <c r="U45" s="23"/>
-      <c r="V45" s="23"/>
-      <c r="W45" s="23"/>
-      <c r="X45" s="23"/>
-      <c r="Y45" s="21"/>
+      <c r="J45" s="22"/>
+      <c r="K45" s="22"/>
+      <c r="L45" s="24"/>
+      <c r="M45" s="24"/>
+      <c r="N45" s="24"/>
+      <c r="O45" s="24"/>
+      <c r="P45" s="24"/>
+      <c r="Q45" s="24"/>
+      <c r="R45" s="24"/>
+      <c r="S45" s="24"/>
+      <c r="T45" s="24"/>
+      <c r="U45" s="24"/>
+      <c r="V45" s="24"/>
+      <c r="W45" s="24"/>
+      <c r="X45" s="24"/>
+      <c r="Y45" s="28"/>
     </row>
     <row r="46" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B46" s="6" t="s">
@@ -4341,29 +4341,57 @@
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
-      <c r="H46" s="23"/>
-      <c r="I46" s="22" t="s">
+      <c r="H46" s="24"/>
+      <c r="I46" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="J46" s="22"/>
-      <c r="K46" s="22"/>
-      <c r="L46" s="23"/>
-      <c r="M46" s="23"/>
-      <c r="N46" s="23"/>
-      <c r="O46" s="23"/>
-      <c r="P46" s="23"/>
-      <c r="Q46" s="23"/>
-      <c r="R46" s="23"/>
-      <c r="S46" s="23"/>
-      <c r="T46" s="23"/>
-      <c r="U46" s="23"/>
-      <c r="V46" s="23"/>
-      <c r="W46" s="23"/>
-      <c r="X46" s="23"/>
-      <c r="Y46" s="21"/>
+      <c r="J46" s="21"/>
+      <c r="K46" s="21"/>
+      <c r="L46" s="24"/>
+      <c r="M46" s="24"/>
+      <c r="N46" s="24"/>
+      <c r="O46" s="24"/>
+      <c r="P46" s="24"/>
+      <c r="Q46" s="24"/>
+      <c r="R46" s="24"/>
+      <c r="S46" s="24"/>
+      <c r="T46" s="24"/>
+      <c r="U46" s="24"/>
+      <c r="V46" s="24"/>
+      <c r="W46" s="24"/>
+      <c r="X46" s="24"/>
+      <c r="Y46" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="H10:H46"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="J30:K30"/>
     <mergeCell ref="I34:K34"/>
     <mergeCell ref="Y10:Y46"/>
     <mergeCell ref="L10:X46"/>
@@ -4380,34 +4408,6 @@
     <mergeCell ref="I36:K36"/>
     <mergeCell ref="I37:K37"/>
     <mergeCell ref="I31:K31"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="H10:H46"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I17:J17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4451,28 +4451,28 @@
       <c r="H2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="I2" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
       <c r="L2" s="9" t="s">
         <v>59</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="N2" s="24" t="s">
+      <c r="N2" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24" t="s">
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
       <c r="U2" s="9" t="s">
         <v>63</v>
       </c>
@@ -4562,11 +4562,11 @@
       <c r="H9" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="I9" s="22" t="s">
+      <c r="I9" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
       <c r="L9" s="9" t="s">
         <v>93</v>
       </c>
@@ -4614,30 +4614,30 @@
       <c r="B10" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="H10" s="23" t="s">
+      <c r="H10" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="I10" s="22" t="s">
+      <c r="I10" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="23" t="s">
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="23"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="23"/>
-      <c r="U10" s="23"/>
-      <c r="V10" s="23"/>
-      <c r="W10" s="23"/>
-      <c r="X10" s="23"/>
-      <c r="Y10" s="21" t="s">
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="24"/>
+      <c r="S10" s="24"/>
+      <c r="T10" s="24"/>
+      <c r="U10" s="24"/>
+      <c r="V10" s="24"/>
+      <c r="W10" s="24"/>
+      <c r="X10" s="24"/>
+      <c r="Y10" s="28" t="s">
         <v>125</v>
       </c>
     </row>
@@ -4645,76 +4645,76 @@
       <c r="B11" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="H11" s="23"/>
-      <c r="I11" s="26" t="s">
+      <c r="H11" s="24"/>
+      <c r="I11" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="23"/>
-      <c r="U11" s="23"/>
-      <c r="V11" s="23"/>
-      <c r="W11" s="23"/>
-      <c r="X11" s="23"/>
-      <c r="Y11" s="21"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="24"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24"/>
+      <c r="U11" s="24"/>
+      <c r="V11" s="24"/>
+      <c r="W11" s="24"/>
+      <c r="X11" s="24"/>
+      <c r="Y11" s="28"/>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="H12" s="23"/>
-      <c r="I12" s="26" t="s">
+      <c r="H12" s="24"/>
+      <c r="I12" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="23"/>
-      <c r="U12" s="23"/>
-      <c r="V12" s="23"/>
-      <c r="W12" s="23"/>
-      <c r="X12" s="23"/>
-      <c r="Y12" s="21"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="24"/>
+      <c r="R12" s="24"/>
+      <c r="S12" s="24"/>
+      <c r="T12" s="24"/>
+      <c r="U12" s="24"/>
+      <c r="V12" s="24"/>
+      <c r="W12" s="24"/>
+      <c r="X12" s="24"/>
+      <c r="Y12" s="28"/>
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="H13" s="23"/>
-      <c r="I13" s="26" t="s">
+      <c r="H13" s="24"/>
+      <c r="I13" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="23"/>
-      <c r="R13" s="23"/>
-      <c r="S13" s="23"/>
-      <c r="T13" s="23"/>
-      <c r="U13" s="23"/>
-      <c r="V13" s="23"/>
-      <c r="W13" s="23"/>
-      <c r="X13" s="23"/>
-      <c r="Y13" s="21"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="24"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="24"/>
+      <c r="Q13" s="24"/>
+      <c r="R13" s="24"/>
+      <c r="S13" s="24"/>
+      <c r="T13" s="24"/>
+      <c r="U13" s="24"/>
+      <c r="V13" s="24"/>
+      <c r="W13" s="24"/>
+      <c r="X13" s="24"/>
+      <c r="Y13" s="28"/>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
@@ -4723,219 +4723,212 @@
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="26" t="s">
+      <c r="H14" s="24"/>
+      <c r="I14" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="23"/>
-      <c r="P14" s="23"/>
-      <c r="Q14" s="23"/>
-      <c r="R14" s="23"/>
-      <c r="S14" s="23"/>
-      <c r="T14" s="23"/>
-      <c r="U14" s="23"/>
-      <c r="V14" s="23"/>
-      <c r="W14" s="23"/>
-      <c r="X14" s="23"/>
-      <c r="Y14" s="21"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="24"/>
+      <c r="S14" s="24"/>
+      <c r="T14" s="24"/>
+      <c r="U14" s="24"/>
+      <c r="V14" s="24"/>
+      <c r="W14" s="24"/>
+      <c r="X14" s="24"/>
+      <c r="Y14" s="28"/>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B15" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="H15" s="23"/>
-      <c r="I15" s="25" t="s">
+      <c r="H15" s="24"/>
+      <c r="I15" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="23"/>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="23"/>
-      <c r="Q15" s="23"/>
-      <c r="R15" s="23"/>
-      <c r="S15" s="23"/>
-      <c r="T15" s="23"/>
-      <c r="U15" s="23"/>
-      <c r="V15" s="23"/>
-      <c r="W15" s="23"/>
-      <c r="X15" s="23"/>
-      <c r="Y15" s="21"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="24"/>
+      <c r="Q15" s="24"/>
+      <c r="R15" s="24"/>
+      <c r="S15" s="24"/>
+      <c r="T15" s="24"/>
+      <c r="U15" s="24"/>
+      <c r="V15" s="24"/>
+      <c r="W15" s="24"/>
+      <c r="X15" s="24"/>
+      <c r="Y15" s="28"/>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B16" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="H16" s="23"/>
-      <c r="I16" s="25" t="s">
+      <c r="H16" s="24"/>
+      <c r="I16" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="23"/>
-      <c r="S16" s="23"/>
-      <c r="T16" s="23"/>
-      <c r="U16" s="23"/>
-      <c r="V16" s="23"/>
-      <c r="W16" s="23"/>
-      <c r="X16" s="23"/>
-      <c r="Y16" s="21"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="24"/>
+      <c r="S16" s="24"/>
+      <c r="T16" s="24"/>
+      <c r="U16" s="24"/>
+      <c r="V16" s="24"/>
+      <c r="W16" s="24"/>
+      <c r="X16" s="24"/>
+      <c r="Y16" s="28"/>
     </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B17" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="H17" s="23"/>
-      <c r="I17" s="25" t="s">
+      <c r="H17" s="24"/>
+      <c r="I17" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="23"/>
-      <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="23"/>
-      <c r="Q17" s="23"/>
-      <c r="R17" s="23"/>
-      <c r="S17" s="23"/>
-      <c r="T17" s="23"/>
-      <c r="U17" s="23"/>
-      <c r="V17" s="23"/>
-      <c r="W17" s="23"/>
-      <c r="X17" s="23"/>
-      <c r="Y17" s="21"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="24"/>
+      <c r="R17" s="24"/>
+      <c r="S17" s="24"/>
+      <c r="T17" s="24"/>
+      <c r="U17" s="24"/>
+      <c r="V17" s="24"/>
+      <c r="W17" s="24"/>
+      <c r="X17" s="24"/>
+      <c r="Y17" s="28"/>
     </row>
     <row r="18" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>4</v>
       </c>
-      <c r="H18" s="23"/>
-      <c r="I18" s="26" t="s">
+      <c r="H18" s="24"/>
+      <c r="I18" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="J18" s="22"/>
+      <c r="J18" s="21"/>
       <c r="K18" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="23"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="23"/>
-      <c r="R18" s="23"/>
-      <c r="S18" s="23"/>
-      <c r="T18" s="23"/>
-      <c r="U18" s="23"/>
-      <c r="V18" s="23"/>
-      <c r="W18" s="23"/>
-      <c r="X18" s="23"/>
-      <c r="Y18" s="21"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="24"/>
+      <c r="S18" s="24"/>
+      <c r="T18" s="24"/>
+      <c r="U18" s="24"/>
+      <c r="V18" s="24"/>
+      <c r="W18" s="24"/>
+      <c r="X18" s="24"/>
+      <c r="Y18" s="28"/>
     </row>
     <row r="19" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>6</v>
       </c>
-      <c r="H19" s="23"/>
-      <c r="I19" s="24" t="s">
+      <c r="H19" s="24"/>
+      <c r="I19" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="J19" s="24"/>
+      <c r="J19" s="26"/>
       <c r="K19" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="23"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="23"/>
-      <c r="Q19" s="23"/>
-      <c r="R19" s="23"/>
-      <c r="S19" s="23"/>
-      <c r="T19" s="23"/>
-      <c r="U19" s="23"/>
-      <c r="V19" s="23"/>
-      <c r="W19" s="23"/>
-      <c r="X19" s="23"/>
-      <c r="Y19" s="21"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="24"/>
+      <c r="Q19" s="24"/>
+      <c r="R19" s="24"/>
+      <c r="S19" s="24"/>
+      <c r="T19" s="24"/>
+      <c r="U19" s="24"/>
+      <c r="V19" s="24"/>
+      <c r="W19" s="24"/>
+      <c r="X19" s="24"/>
+      <c r="Y19" s="28"/>
     </row>
     <row r="20" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="23"/>
+      <c r="H20" s="24"/>
       <c r="I20" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="J20" s="24" t="s">
+      <c r="J20" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="K20" s="24"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="23"/>
-      <c r="O20" s="23"/>
-      <c r="P20" s="23"/>
-      <c r="Q20" s="23"/>
-      <c r="R20" s="23"/>
-      <c r="S20" s="23"/>
-      <c r="T20" s="23"/>
-      <c r="U20" s="23"/>
-      <c r="V20" s="23"/>
-      <c r="W20" s="23"/>
-      <c r="X20" s="23"/>
-      <c r="Y20" s="21"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="24"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="24"/>
+      <c r="S20" s="24"/>
+      <c r="T20" s="24"/>
+      <c r="U20" s="24"/>
+      <c r="V20" s="24"/>
+      <c r="W20" s="24"/>
+      <c r="X20" s="24"/>
+      <c r="Y20" s="28"/>
     </row>
     <row r="21" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>13</v>
       </c>
-      <c r="H21" s="23"/>
+      <c r="H21" s="24"/>
       <c r="I21" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="J21" s="28" t="s">
+      <c r="J21" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="K21" s="28"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="23"/>
-      <c r="N21" s="23"/>
-      <c r="O21" s="23"/>
-      <c r="P21" s="23"/>
-      <c r="Q21" s="23"/>
-      <c r="R21" s="23"/>
-      <c r="S21" s="23"/>
-      <c r="T21" s="23"/>
-      <c r="U21" s="23"/>
-      <c r="V21" s="23"/>
-      <c r="W21" s="23"/>
-      <c r="X21" s="23"/>
-      <c r="Y21" s="21"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
+      <c r="N21" s="24"/>
+      <c r="O21" s="24"/>
+      <c r="P21" s="24"/>
+      <c r="Q21" s="24"/>
+      <c r="R21" s="24"/>
+      <c r="S21" s="24"/>
+      <c r="T21" s="24"/>
+      <c r="U21" s="24"/>
+      <c r="V21" s="24"/>
+      <c r="W21" s="24"/>
+      <c r="X21" s="24"/>
+      <c r="Y21" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="Y10:Y21"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I19:J19"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:T2"/>
@@ -4948,6 +4941,13 @@
     <mergeCell ref="I12:K12"/>
     <mergeCell ref="I13:K13"/>
     <mergeCell ref="J21:K21"/>
+    <mergeCell ref="Y10:Y21"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I19:J19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5075,7 +5075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -5176,8 +5176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Additional tests for GIF and Unicode.
</commit_message>
<xml_diff>
--- a/doc/unicode.xlsx
+++ b/doc/unicode.xlsx
@@ -1292,15 +1292,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1308,22 +1318,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1638,10 +1638,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="C1" s="24"/>
+      <c r="C1" s="26"/>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
@@ -1826,28 +1826,28 @@
       <c r="I2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
       <c r="M2" s="8" t="s">
         <v>59</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="O2" s="28" t="s">
+      <c r="O2" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28" t="s">
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="T2" s="28"/>
-      <c r="U2" s="28"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
       <c r="V2" s="8" t="s">
         <v>63</v>
       </c>
@@ -1937,11 +1937,11 @@
       <c r="I9" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J9" s="26" t="s">
+      <c r="J9" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
       <c r="M9" s="8" t="s">
         <v>119</v>
       </c>
@@ -1989,30 +1989,30 @@
       <c r="B10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I10" s="27" t="s">
+      <c r="I10" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="J10" s="26" t="s">
+      <c r="J10" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="27" t="s">
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="N10" s="27"/>
-      <c r="O10" s="27"/>
-      <c r="P10" s="27"/>
-      <c r="Q10" s="27"/>
-      <c r="R10" s="27"/>
-      <c r="S10" s="27"/>
-      <c r="T10" s="27"/>
-      <c r="U10" s="27"/>
-      <c r="V10" s="27"/>
-      <c r="W10" s="27"/>
-      <c r="X10" s="27"/>
-      <c r="Y10" s="27"/>
-      <c r="Z10" s="25" t="s">
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="30"/>
+      <c r="R10" s="30"/>
+      <c r="S10" s="30"/>
+      <c r="T10" s="30"/>
+      <c r="U10" s="30"/>
+      <c r="V10" s="30"/>
+      <c r="W10" s="30"/>
+      <c r="X10" s="30"/>
+      <c r="Y10" s="30"/>
+      <c r="Z10" s="34" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2020,81 +2020,81 @@
       <c r="B11" t="s">
         <v>3</v>
       </c>
-      <c r="I11" s="27"/>
-      <c r="J11" s="29" t="s">
+      <c r="I11" s="30"/>
+      <c r="J11" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="27"/>
-      <c r="N11" s="27"/>
-      <c r="O11" s="27"/>
-      <c r="P11" s="27"/>
-      <c r="Q11" s="27"/>
-      <c r="R11" s="27"/>
-      <c r="S11" s="27"/>
-      <c r="T11" s="27"/>
-      <c r="U11" s="27"/>
-      <c r="V11" s="27"/>
-      <c r="W11" s="27"/>
-      <c r="X11" s="27"/>
-      <c r="Y11" s="27"/>
-      <c r="Z11" s="25"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="30"/>
+      <c r="R11" s="30"/>
+      <c r="S11" s="30"/>
+      <c r="T11" s="30"/>
+      <c r="U11" s="30"/>
+      <c r="V11" s="30"/>
+      <c r="W11" s="30"/>
+      <c r="X11" s="30"/>
+      <c r="Y11" s="30"/>
+      <c r="Z11" s="34"/>
     </row>
     <row r="12" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>4</v>
       </c>
-      <c r="I12" s="27"/>
-      <c r="J12" s="26" t="s">
+      <c r="I12" s="30"/>
+      <c r="J12" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="K12" s="26"/>
+      <c r="K12" s="27"/>
       <c r="L12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="M12" s="27"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="27"/>
-      <c r="P12" s="27"/>
-      <c r="Q12" s="27"/>
-      <c r="R12" s="27"/>
-      <c r="S12" s="27"/>
-      <c r="T12" s="27"/>
-      <c r="U12" s="27"/>
-      <c r="V12" s="27"/>
-      <c r="W12" s="27"/>
-      <c r="X12" s="27"/>
-      <c r="Y12" s="27"/>
-      <c r="Z12" s="25"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="30"/>
+      <c r="R12" s="30"/>
+      <c r="S12" s="30"/>
+      <c r="T12" s="30"/>
+      <c r="U12" s="30"/>
+      <c r="V12" s="30"/>
+      <c r="W12" s="30"/>
+      <c r="X12" s="30"/>
+      <c r="Y12" s="30"/>
+      <c r="Z12" s="34"/>
     </row>
     <row r="13" spans="2:26" x14ac:dyDescent="0.25">
       <c r="C13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="27" t="s">
+      <c r="I13" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="J13" s="26" t="s">
+      <c r="J13" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="27" t="s">
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="N13" s="27"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="27"/>
-      <c r="R13" s="27"/>
-      <c r="S13" s="27"/>
-      <c r="T13" s="27"/>
-      <c r="U13" s="27"/>
-      <c r="V13" s="27"/>
-      <c r="W13" s="27"/>
-      <c r="X13" s="27"/>
-      <c r="Y13" s="27"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="30"/>
+      <c r="R13" s="30"/>
+      <c r="S13" s="30"/>
+      <c r="T13" s="30"/>
+      <c r="U13" s="30"/>
+      <c r="V13" s="30"/>
+      <c r="W13" s="30"/>
+      <c r="X13" s="30"/>
+      <c r="Y13" s="30"/>
       <c r="Z13" s="12" t="s">
         <v>127</v>
       </c>
@@ -2103,27 +2103,27 @@
       <c r="C14" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="27"/>
-      <c r="J14" s="29" t="s">
+      <c r="I14" s="30"/>
+      <c r="J14" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="27" t="s">
+      <c r="K14" s="33"/>
+      <c r="L14" s="33"/>
+      <c r="M14" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="N14" s="27"/>
-      <c r="O14" s="27"/>
-      <c r="P14" s="27"/>
-      <c r="Q14" s="27"/>
-      <c r="R14" s="27"/>
-      <c r="S14" s="27"/>
-      <c r="T14" s="27"/>
-      <c r="U14" s="27"/>
-      <c r="V14" s="27"/>
-      <c r="W14" s="27"/>
-      <c r="X14" s="27"/>
-      <c r="Y14" s="27"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="30"/>
+      <c r="R14" s="30"/>
+      <c r="S14" s="30"/>
+      <c r="T14" s="30"/>
+      <c r="U14" s="30"/>
+      <c r="V14" s="30"/>
+      <c r="W14" s="30"/>
+      <c r="X14" s="30"/>
+      <c r="Y14" s="30"/>
       <c r="Z14" s="12" t="s">
         <v>127</v>
       </c>
@@ -2135,26 +2135,26 @@
       <c r="I15" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J15" s="28" t="s">
+      <c r="J15" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="26" t="s">
+      <c r="K15" s="32"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="N15" s="26"/>
-      <c r="O15" s="26"/>
-      <c r="P15" s="26"/>
-      <c r="Q15" s="26"/>
-      <c r="R15" s="26"/>
-      <c r="S15" s="26"/>
-      <c r="T15" s="26"/>
-      <c r="U15" s="26"/>
-      <c r="V15" s="26"/>
-      <c r="W15" s="26"/>
-      <c r="X15" s="26"/>
-      <c r="Y15" s="26"/>
+      <c r="N15" s="27"/>
+      <c r="O15" s="27"/>
+      <c r="P15" s="27"/>
+      <c r="Q15" s="27"/>
+      <c r="R15" s="27"/>
+      <c r="S15" s="27"/>
+      <c r="T15" s="27"/>
+      <c r="U15" s="27"/>
+      <c r="V15" s="27"/>
+      <c r="W15" s="27"/>
+      <c r="X15" s="27"/>
+      <c r="Y15" s="27"/>
       <c r="Z15" s="14" t="s">
         <v>126</v>
       </c>
@@ -2166,26 +2166,26 @@
       <c r="I16" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J16" s="29" t="s">
+      <c r="J16" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="27" t="s">
+      <c r="K16" s="33"/>
+      <c r="L16" s="33"/>
+      <c r="M16" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="N16" s="27"/>
-      <c r="O16" s="27"/>
-      <c r="P16" s="27"/>
-      <c r="Q16" s="27"/>
-      <c r="R16" s="27"/>
-      <c r="S16" s="27"/>
-      <c r="T16" s="27"/>
-      <c r="U16" s="27"/>
-      <c r="V16" s="27"/>
-      <c r="W16" s="27"/>
-      <c r="X16" s="27"/>
-      <c r="Y16" s="27"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="30"/>
+      <c r="R16" s="30"/>
+      <c r="S16" s="30"/>
+      <c r="T16" s="30"/>
+      <c r="U16" s="30"/>
+      <c r="V16" s="30"/>
+      <c r="W16" s="30"/>
+      <c r="X16" s="30"/>
+      <c r="Y16" s="30"/>
       <c r="Z16" s="12" t="s">
         <v>127</v>
       </c>
@@ -2197,28 +2197,28 @@
       <c r="I17" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J17" s="28" t="s">
+      <c r="J17" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="K17" s="28"/>
+      <c r="K17" s="32"/>
       <c r="L17" t="s">
         <v>55</v>
       </c>
-      <c r="M17" s="26" t="s">
+      <c r="M17" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
-      <c r="Q17" s="26"/>
-      <c r="R17" s="26"/>
-      <c r="S17" s="26"/>
-      <c r="T17" s="26"/>
-      <c r="U17" s="26"/>
-      <c r="V17" s="26"/>
-      <c r="W17" s="26"/>
-      <c r="X17" s="26"/>
-      <c r="Y17" s="26"/>
+      <c r="N17" s="27"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="27"/>
+      <c r="Q17" s="27"/>
+      <c r="R17" s="27"/>
+      <c r="S17" s="27"/>
+      <c r="T17" s="27"/>
+      <c r="U17" s="27"/>
+      <c r="V17" s="27"/>
+      <c r="W17" s="27"/>
+      <c r="X17" s="27"/>
+      <c r="Y17" s="27"/>
       <c r="Z17" s="14" t="s">
         <v>126</v>
       </c>
@@ -2230,26 +2230,26 @@
       <c r="I18" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J18" s="29" t="s">
+      <c r="J18" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="27" t="s">
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
+      <c r="M18" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="N18" s="27"/>
-      <c r="O18" s="27"/>
-      <c r="P18" s="27"/>
-      <c r="Q18" s="27"/>
-      <c r="R18" s="27"/>
-      <c r="S18" s="27"/>
-      <c r="T18" s="27"/>
-      <c r="U18" s="27"/>
-      <c r="V18" s="27"/>
-      <c r="W18" s="27"/>
-      <c r="X18" s="27"/>
-      <c r="Y18" s="27"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="30"/>
+      <c r="P18" s="30"/>
+      <c r="Q18" s="30"/>
+      <c r="R18" s="30"/>
+      <c r="S18" s="30"/>
+      <c r="T18" s="30"/>
+      <c r="U18" s="30"/>
+      <c r="V18" s="30"/>
+      <c r="W18" s="30"/>
+      <c r="X18" s="30"/>
+      <c r="Y18" s="30"/>
       <c r="Z18" s="12" t="s">
         <v>127</v>
       </c>
@@ -2266,21 +2266,21 @@
       </c>
       <c r="K19" s="31"/>
       <c r="L19" s="31"/>
-      <c r="M19" s="27" t="s">
+      <c r="M19" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="N19" s="27"/>
-      <c r="O19" s="27"/>
-      <c r="P19" s="27"/>
-      <c r="Q19" s="27"/>
-      <c r="R19" s="27"/>
-      <c r="S19" s="27"/>
-      <c r="T19" s="27"/>
-      <c r="U19" s="27"/>
-      <c r="V19" s="27"/>
-      <c r="W19" s="27"/>
-      <c r="X19" s="27"/>
-      <c r="Y19" s="27"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="30"/>
+      <c r="P19" s="30"/>
+      <c r="Q19" s="30"/>
+      <c r="R19" s="30"/>
+      <c r="S19" s="30"/>
+      <c r="T19" s="30"/>
+      <c r="U19" s="30"/>
+      <c r="V19" s="30"/>
+      <c r="W19" s="30"/>
+      <c r="X19" s="30"/>
+      <c r="Y19" s="30"/>
       <c r="Z19" s="12" t="s">
         <v>127</v>
       </c>
@@ -2292,26 +2292,26 @@
       <c r="I20" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J20" s="28" t="s">
+      <c r="J20" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="K20" s="28"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="26" t="s">
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="N20" s="26"/>
-      <c r="O20" s="26"/>
-      <c r="P20" s="26"/>
-      <c r="Q20" s="26"/>
-      <c r="R20" s="26"/>
-      <c r="S20" s="26"/>
-      <c r="T20" s="26"/>
-      <c r="U20" s="26"/>
-      <c r="V20" s="26"/>
-      <c r="W20" s="26"/>
-      <c r="X20" s="26"/>
-      <c r="Y20" s="26"/>
+      <c r="N20" s="27"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="27"/>
+      <c r="Q20" s="27"/>
+      <c r="R20" s="27"/>
+      <c r="S20" s="27"/>
+      <c r="T20" s="27"/>
+      <c r="U20" s="27"/>
+      <c r="V20" s="27"/>
+      <c r="W20" s="27"/>
+      <c r="X20" s="27"/>
+      <c r="Y20" s="27"/>
       <c r="Z20" s="14" t="s">
         <v>126</v>
       </c>
@@ -2323,26 +2323,26 @@
       <c r="I21" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J21" s="29" t="s">
+      <c r="J21" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="K21" s="29"/>
-      <c r="L21" s="29"/>
-      <c r="M21" s="27" t="s">
+      <c r="K21" s="33"/>
+      <c r="L21" s="33"/>
+      <c r="M21" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="N21" s="27"/>
-      <c r="O21" s="27"/>
-      <c r="P21" s="27"/>
-      <c r="Q21" s="27"/>
-      <c r="R21" s="27"/>
-      <c r="S21" s="27"/>
-      <c r="T21" s="27"/>
-      <c r="U21" s="27"/>
-      <c r="V21" s="27"/>
-      <c r="W21" s="27"/>
-      <c r="X21" s="27"/>
-      <c r="Y21" s="27"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="30"/>
+      <c r="P21" s="30"/>
+      <c r="Q21" s="30"/>
+      <c r="R21" s="30"/>
+      <c r="S21" s="30"/>
+      <c r="T21" s="30"/>
+      <c r="U21" s="30"/>
+      <c r="V21" s="30"/>
+      <c r="W21" s="30"/>
+      <c r="X21" s="30"/>
+      <c r="Y21" s="30"/>
       <c r="Z21" s="12" t="s">
         <v>127</v>
       </c>
@@ -2357,25 +2357,25 @@
       <c r="J22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K22" s="28" t="s">
+      <c r="K22" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="L22" s="28"/>
-      <c r="M22" s="26" t="s">
+      <c r="L22" s="32"/>
+      <c r="M22" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="N22" s="26"/>
-      <c r="O22" s="26"/>
-      <c r="P22" s="26"/>
-      <c r="Q22" s="26"/>
-      <c r="R22" s="26"/>
-      <c r="S22" s="26"/>
-      <c r="T22" s="26"/>
-      <c r="U22" s="26"/>
-      <c r="V22" s="26"/>
-      <c r="W22" s="26"/>
-      <c r="X22" s="26"/>
-      <c r="Y22" s="26"/>
+      <c r="N22" s="27"/>
+      <c r="O22" s="27"/>
+      <c r="P22" s="27"/>
+      <c r="Q22" s="27"/>
+      <c r="R22" s="27"/>
+      <c r="S22" s="27"/>
+      <c r="T22" s="27"/>
+      <c r="U22" s="27"/>
+      <c r="V22" s="27"/>
+      <c r="W22" s="27"/>
+      <c r="X22" s="27"/>
+      <c r="Y22" s="27"/>
       <c r="Z22" s="14" t="s">
         <v>126</v>
       </c>
@@ -2387,26 +2387,26 @@
       <c r="I23" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J23" s="30" t="s">
+      <c r="J23" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="K23" s="30"/>
-      <c r="L23" s="30"/>
-      <c r="M23" s="27" t="s">
+      <c r="K23" s="28"/>
+      <c r="L23" s="28"/>
+      <c r="M23" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="N23" s="27"/>
-      <c r="O23" s="27"/>
-      <c r="P23" s="27"/>
-      <c r="Q23" s="27"/>
-      <c r="R23" s="27"/>
-      <c r="S23" s="27"/>
-      <c r="T23" s="27"/>
-      <c r="U23" s="27"/>
-      <c r="V23" s="27"/>
-      <c r="W23" s="27"/>
-      <c r="X23" s="27"/>
-      <c r="Y23" s="27"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="30"/>
+      <c r="P23" s="30"/>
+      <c r="Q23" s="30"/>
+      <c r="R23" s="30"/>
+      <c r="S23" s="30"/>
+      <c r="T23" s="30"/>
+      <c r="U23" s="30"/>
+      <c r="V23" s="30"/>
+      <c r="W23" s="30"/>
+      <c r="X23" s="30"/>
+      <c r="Y23" s="30"/>
       <c r="Z23" s="12" t="s">
         <v>127</v>
       </c>
@@ -2419,26 +2419,26 @@
       <c r="I24" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="J24" s="26" t="s">
+      <c r="J24" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26" t="s">
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="N24" s="26"/>
-      <c r="O24" s="26"/>
-      <c r="P24" s="26"/>
-      <c r="Q24" s="26"/>
-      <c r="R24" s="26"/>
-      <c r="S24" s="26"/>
-      <c r="T24" s="26"/>
-      <c r="U24" s="26"/>
-      <c r="V24" s="26"/>
-      <c r="W24" s="26"/>
-      <c r="X24" s="26"/>
-      <c r="Y24" s="26"/>
+      <c r="N24" s="27"/>
+      <c r="O24" s="27"/>
+      <c r="P24" s="27"/>
+      <c r="Q24" s="27"/>
+      <c r="R24" s="27"/>
+      <c r="S24" s="27"/>
+      <c r="T24" s="27"/>
+      <c r="U24" s="27"/>
+      <c r="V24" s="27"/>
+      <c r="W24" s="27"/>
+      <c r="X24" s="27"/>
+      <c r="Y24" s="27"/>
       <c r="Z24" s="10" t="s">
         <v>130</v>
       </c>
@@ -2450,26 +2450,26 @@
       <c r="I25" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J25" s="28" t="s">
+      <c r="J25" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="K25" s="28"/>
-      <c r="L25" s="28"/>
-      <c r="M25" s="27" t="s">
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="N25" s="27"/>
-      <c r="O25" s="27"/>
-      <c r="P25" s="27"/>
-      <c r="Q25" s="27"/>
-      <c r="R25" s="27"/>
-      <c r="S25" s="27"/>
-      <c r="T25" s="27"/>
-      <c r="U25" s="27"/>
-      <c r="V25" s="27"/>
-      <c r="W25" s="27"/>
-      <c r="X25" s="27"/>
-      <c r="Y25" s="27"/>
+      <c r="N25" s="30"/>
+      <c r="O25" s="30"/>
+      <c r="P25" s="30"/>
+      <c r="Q25" s="30"/>
+      <c r="R25" s="30"/>
+      <c r="S25" s="30"/>
+      <c r="T25" s="30"/>
+      <c r="U25" s="30"/>
+      <c r="V25" s="30"/>
+      <c r="W25" s="30"/>
+      <c r="X25" s="30"/>
+      <c r="Y25" s="30"/>
       <c r="Z25" s="12" t="s">
         <v>127</v>
       </c>
@@ -2481,26 +2481,26 @@
       <c r="I26" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="J26" s="29" t="s">
+      <c r="J26" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="K26" s="29"/>
-      <c r="L26" s="29"/>
-      <c r="M26" s="26" t="s">
+      <c r="K26" s="33"/>
+      <c r="L26" s="33"/>
+      <c r="M26" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="N26" s="26"/>
-      <c r="O26" s="26"/>
-      <c r="P26" s="26"/>
-      <c r="Q26" s="26"/>
-      <c r="R26" s="26"/>
-      <c r="S26" s="26"/>
-      <c r="T26" s="26"/>
-      <c r="U26" s="26"/>
-      <c r="V26" s="26"/>
-      <c r="W26" s="26"/>
-      <c r="X26" s="26"/>
-      <c r="Y26" s="26"/>
+      <c r="N26" s="27"/>
+      <c r="O26" s="27"/>
+      <c r="P26" s="27"/>
+      <c r="Q26" s="27"/>
+      <c r="R26" s="27"/>
+      <c r="S26" s="27"/>
+      <c r="T26" s="27"/>
+      <c r="U26" s="27"/>
+      <c r="V26" s="27"/>
+      <c r="W26" s="27"/>
+      <c r="X26" s="27"/>
+      <c r="Y26" s="27"/>
       <c r="Z26" s="10" t="s">
         <v>130</v>
       </c>
@@ -2512,26 +2512,26 @@
       <c r="I27" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J27" s="28" t="s">
+      <c r="J27" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="K27" s="28"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="26" t="s">
+      <c r="K27" s="32"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="N27" s="26"/>
-      <c r="O27" s="26"/>
-      <c r="P27" s="26"/>
-      <c r="Q27" s="26"/>
-      <c r="R27" s="26"/>
-      <c r="S27" s="26"/>
-      <c r="T27" s="26"/>
-      <c r="U27" s="26"/>
-      <c r="V27" s="26"/>
-      <c r="W27" s="26"/>
-      <c r="X27" s="26"/>
-      <c r="Y27" s="26"/>
+      <c r="N27" s="27"/>
+      <c r="O27" s="27"/>
+      <c r="P27" s="27"/>
+      <c r="Q27" s="27"/>
+      <c r="R27" s="27"/>
+      <c r="S27" s="27"/>
+      <c r="T27" s="27"/>
+      <c r="U27" s="27"/>
+      <c r="V27" s="27"/>
+      <c r="W27" s="27"/>
+      <c r="X27" s="27"/>
+      <c r="Y27" s="27"/>
       <c r="Z27" s="14" t="s">
         <v>126</v>
       </c>
@@ -2543,26 +2543,26 @@
       <c r="I28" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J28" s="28" t="s">
+      <c r="J28" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="27" t="s">
+      <c r="K28" s="32"/>
+      <c r="L28" s="32"/>
+      <c r="M28" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="N28" s="27"/>
-      <c r="O28" s="27"/>
-      <c r="P28" s="27"/>
-      <c r="Q28" s="27"/>
-      <c r="R28" s="27"/>
-      <c r="S28" s="27"/>
-      <c r="T28" s="27"/>
-      <c r="U28" s="27"/>
-      <c r="V28" s="27"/>
-      <c r="W28" s="27"/>
-      <c r="X28" s="27"/>
-      <c r="Y28" s="27"/>
+      <c r="N28" s="30"/>
+      <c r="O28" s="30"/>
+      <c r="P28" s="30"/>
+      <c r="Q28" s="30"/>
+      <c r="R28" s="30"/>
+      <c r="S28" s="30"/>
+      <c r="T28" s="30"/>
+      <c r="U28" s="30"/>
+      <c r="V28" s="30"/>
+      <c r="W28" s="30"/>
+      <c r="X28" s="30"/>
+      <c r="Y28" s="30"/>
       <c r="Z28" s="12" t="s">
         <v>127</v>
       </c>
@@ -2574,26 +2574,26 @@
       <c r="I29" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="J29" s="29" t="s">
+      <c r="J29" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="K29" s="29"/>
-      <c r="L29" s="29"/>
-      <c r="M29" s="26" t="s">
+      <c r="K29" s="33"/>
+      <c r="L29" s="33"/>
+      <c r="M29" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="N29" s="26"/>
-      <c r="O29" s="26"/>
-      <c r="P29" s="26"/>
-      <c r="Q29" s="26"/>
-      <c r="R29" s="26"/>
-      <c r="S29" s="26"/>
-      <c r="T29" s="26"/>
-      <c r="U29" s="26"/>
-      <c r="V29" s="26"/>
-      <c r="W29" s="26"/>
-      <c r="X29" s="26"/>
-      <c r="Y29" s="26"/>
+      <c r="N29" s="27"/>
+      <c r="O29" s="27"/>
+      <c r="P29" s="27"/>
+      <c r="Q29" s="27"/>
+      <c r="R29" s="27"/>
+      <c r="S29" s="27"/>
+      <c r="T29" s="27"/>
+      <c r="U29" s="27"/>
+      <c r="V29" s="27"/>
+      <c r="W29" s="27"/>
+      <c r="X29" s="27"/>
+      <c r="Y29" s="27"/>
       <c r="Z29" s="10" t="s">
         <v>130</v>
       </c>
@@ -2608,25 +2608,25 @@
       <c r="J30" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K30" s="32" t="s">
+      <c r="K30" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="L30" s="32"/>
-      <c r="M30" s="26" t="s">
+      <c r="L30" s="29"/>
+      <c r="M30" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="N30" s="26"/>
-      <c r="O30" s="26"/>
-      <c r="P30" s="26"/>
-      <c r="Q30" s="26"/>
-      <c r="R30" s="26"/>
-      <c r="S30" s="26"/>
-      <c r="T30" s="26"/>
-      <c r="U30" s="26"/>
-      <c r="V30" s="26"/>
-      <c r="W30" s="26"/>
-      <c r="X30" s="26"/>
-      <c r="Y30" s="26"/>
+      <c r="N30" s="27"/>
+      <c r="O30" s="27"/>
+      <c r="P30" s="27"/>
+      <c r="Q30" s="27"/>
+      <c r="R30" s="27"/>
+      <c r="S30" s="27"/>
+      <c r="T30" s="27"/>
+      <c r="U30" s="27"/>
+      <c r="V30" s="27"/>
+      <c r="W30" s="27"/>
+      <c r="X30" s="27"/>
+      <c r="Y30" s="27"/>
       <c r="Z30" s="14" t="s">
         <v>126</v>
       </c>
@@ -2638,26 +2638,26 @@
       <c r="I31" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J31" s="28" t="s">
+      <c r="J31" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="K31" s="28"/>
-      <c r="L31" s="28"/>
-      <c r="M31" s="27" t="s">
+      <c r="K31" s="32"/>
+      <c r="L31" s="32"/>
+      <c r="M31" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="N31" s="27"/>
-      <c r="O31" s="27"/>
-      <c r="P31" s="27"/>
-      <c r="Q31" s="27"/>
-      <c r="R31" s="27"/>
-      <c r="S31" s="27"/>
-      <c r="T31" s="27"/>
-      <c r="U31" s="27"/>
-      <c r="V31" s="27"/>
-      <c r="W31" s="27"/>
-      <c r="X31" s="27"/>
-      <c r="Y31" s="27"/>
+      <c r="N31" s="30"/>
+      <c r="O31" s="30"/>
+      <c r="P31" s="30"/>
+      <c r="Q31" s="30"/>
+      <c r="R31" s="30"/>
+      <c r="S31" s="30"/>
+      <c r="T31" s="30"/>
+      <c r="U31" s="30"/>
+      <c r="V31" s="30"/>
+      <c r="W31" s="30"/>
+      <c r="X31" s="30"/>
+      <c r="Y31" s="30"/>
       <c r="Z31" s="12" t="s">
         <v>127</v>
       </c>
@@ -2669,26 +2669,26 @@
       <c r="I32" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="J32" s="29" t="s">
+      <c r="J32" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="26" t="s">
+      <c r="K32" s="33"/>
+      <c r="L32" s="33"/>
+      <c r="M32" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="N32" s="26"/>
-      <c r="O32" s="26"/>
-      <c r="P32" s="26"/>
-      <c r="Q32" s="26"/>
-      <c r="R32" s="26"/>
-      <c r="S32" s="26"/>
-      <c r="T32" s="26"/>
-      <c r="U32" s="26"/>
-      <c r="V32" s="26"/>
-      <c r="W32" s="26"/>
-      <c r="X32" s="26"/>
-      <c r="Y32" s="26"/>
+      <c r="N32" s="27"/>
+      <c r="O32" s="27"/>
+      <c r="P32" s="27"/>
+      <c r="Q32" s="27"/>
+      <c r="R32" s="27"/>
+      <c r="S32" s="27"/>
+      <c r="T32" s="27"/>
+      <c r="U32" s="27"/>
+      <c r="V32" s="27"/>
+      <c r="W32" s="27"/>
+      <c r="X32" s="27"/>
+      <c r="Y32" s="27"/>
       <c r="Z32" s="10" t="s">
         <v>130</v>
       </c>
@@ -2700,26 +2700,26 @@
       <c r="I33" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="J33" s="32" t="s">
+      <c r="J33" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="K33" s="32"/>
-      <c r="L33" s="32"/>
-      <c r="M33" s="27" t="s">
+      <c r="K33" s="29"/>
+      <c r="L33" s="29"/>
+      <c r="M33" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="N33" s="27"/>
-      <c r="O33" s="27"/>
-      <c r="P33" s="27"/>
-      <c r="Q33" s="27"/>
-      <c r="R33" s="27"/>
-      <c r="S33" s="27"/>
-      <c r="T33" s="27"/>
-      <c r="U33" s="27"/>
-      <c r="V33" s="27"/>
-      <c r="W33" s="27"/>
-      <c r="X33" s="27"/>
-      <c r="Y33" s="27"/>
+      <c r="N33" s="30"/>
+      <c r="O33" s="30"/>
+      <c r="P33" s="30"/>
+      <c r="Q33" s="30"/>
+      <c r="R33" s="30"/>
+      <c r="S33" s="30"/>
+      <c r="T33" s="30"/>
+      <c r="U33" s="30"/>
+      <c r="V33" s="30"/>
+      <c r="W33" s="30"/>
+      <c r="X33" s="30"/>
+      <c r="Y33" s="30"/>
       <c r="Z33" s="12" t="s">
         <v>127</v>
       </c>
@@ -2737,21 +2737,21 @@
       </c>
       <c r="K34" s="31"/>
       <c r="L34" s="31"/>
-      <c r="M34" s="26" t="s">
+      <c r="M34" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="N34" s="26"/>
-      <c r="O34" s="26"/>
-      <c r="P34" s="26"/>
-      <c r="Q34" s="26"/>
-      <c r="R34" s="26"/>
-      <c r="S34" s="26"/>
-      <c r="T34" s="26"/>
-      <c r="U34" s="26"/>
-      <c r="V34" s="26"/>
-      <c r="W34" s="26"/>
-      <c r="X34" s="26"/>
-      <c r="Y34" s="26"/>
+      <c r="N34" s="27"/>
+      <c r="O34" s="27"/>
+      <c r="P34" s="27"/>
+      <c r="Q34" s="27"/>
+      <c r="R34" s="27"/>
+      <c r="S34" s="27"/>
+      <c r="T34" s="27"/>
+      <c r="U34" s="27"/>
+      <c r="V34" s="27"/>
+      <c r="W34" s="27"/>
+      <c r="X34" s="27"/>
+      <c r="Y34" s="27"/>
       <c r="Z34" s="10" t="s">
         <v>130</v>
       </c>
@@ -2767,26 +2767,26 @@
       <c r="I35" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J35" s="30" t="s">
+      <c r="J35" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="K35" s="30"/>
-      <c r="L35" s="30"/>
-      <c r="M35" s="26" t="s">
+      <c r="K35" s="28"/>
+      <c r="L35" s="28"/>
+      <c r="M35" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="N35" s="26"/>
-      <c r="O35" s="26"/>
-      <c r="P35" s="26"/>
-      <c r="Q35" s="26"/>
-      <c r="R35" s="26"/>
-      <c r="S35" s="26"/>
-      <c r="T35" s="26"/>
-      <c r="U35" s="26"/>
-      <c r="V35" s="26"/>
-      <c r="W35" s="26"/>
-      <c r="X35" s="26"/>
-      <c r="Y35" s="26"/>
+      <c r="N35" s="27"/>
+      <c r="O35" s="27"/>
+      <c r="P35" s="27"/>
+      <c r="Q35" s="27"/>
+      <c r="R35" s="27"/>
+      <c r="S35" s="27"/>
+      <c r="T35" s="27"/>
+      <c r="U35" s="27"/>
+      <c r="V35" s="27"/>
+      <c r="W35" s="27"/>
+      <c r="X35" s="27"/>
+      <c r="Y35" s="27"/>
       <c r="Z35" s="14" t="s">
         <v>126</v>
       </c>
@@ -2802,26 +2802,26 @@
       <c r="I36" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J36" s="30" t="s">
+      <c r="J36" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="K36" s="30"/>
-      <c r="L36" s="30"/>
-      <c r="M36" s="27" t="s">
+      <c r="K36" s="28"/>
+      <c r="L36" s="28"/>
+      <c r="M36" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="N36" s="27"/>
-      <c r="O36" s="27"/>
-      <c r="P36" s="27"/>
-      <c r="Q36" s="27"/>
-      <c r="R36" s="27"/>
-      <c r="S36" s="27"/>
-      <c r="T36" s="27"/>
-      <c r="U36" s="27"/>
-      <c r="V36" s="27"/>
-      <c r="W36" s="27"/>
-      <c r="X36" s="27"/>
-      <c r="Y36" s="27"/>
+      <c r="N36" s="30"/>
+      <c r="O36" s="30"/>
+      <c r="P36" s="30"/>
+      <c r="Q36" s="30"/>
+      <c r="R36" s="30"/>
+      <c r="S36" s="30"/>
+      <c r="T36" s="30"/>
+      <c r="U36" s="30"/>
+      <c r="V36" s="30"/>
+      <c r="W36" s="30"/>
+      <c r="X36" s="30"/>
+      <c r="Y36" s="30"/>
       <c r="Z36" s="12" t="s">
         <v>127</v>
       </c>
@@ -2837,26 +2837,26 @@
       <c r="I37" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="J37" s="26" t="s">
+      <c r="J37" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="K37" s="26"/>
-      <c r="L37" s="26"/>
-      <c r="M37" s="26" t="s">
+      <c r="K37" s="27"/>
+      <c r="L37" s="27"/>
+      <c r="M37" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="N37" s="26"/>
-      <c r="O37" s="26"/>
-      <c r="P37" s="26"/>
-      <c r="Q37" s="26"/>
-      <c r="R37" s="26"/>
-      <c r="S37" s="26"/>
-      <c r="T37" s="26"/>
-      <c r="U37" s="26"/>
-      <c r="V37" s="26"/>
-      <c r="W37" s="26"/>
-      <c r="X37" s="26"/>
-      <c r="Y37" s="26"/>
+      <c r="N37" s="27"/>
+      <c r="O37" s="27"/>
+      <c r="P37" s="27"/>
+      <c r="Q37" s="27"/>
+      <c r="R37" s="27"/>
+      <c r="S37" s="27"/>
+      <c r="T37" s="27"/>
+      <c r="U37" s="27"/>
+      <c r="V37" s="27"/>
+      <c r="W37" s="27"/>
+      <c r="X37" s="27"/>
+      <c r="Y37" s="27"/>
       <c r="Z37" s="10" t="s">
         <v>130</v>
       </c>
@@ -2872,26 +2872,26 @@
       <c r="I38" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J38" s="30" t="s">
+      <c r="J38" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="K38" s="30"/>
-      <c r="L38" s="30"/>
-      <c r="M38" s="26" t="s">
+      <c r="K38" s="28"/>
+      <c r="L38" s="28"/>
+      <c r="M38" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="N38" s="26"/>
-      <c r="O38" s="26"/>
-      <c r="P38" s="26"/>
-      <c r="Q38" s="26"/>
-      <c r="R38" s="26"/>
-      <c r="S38" s="26"/>
-      <c r="T38" s="26"/>
-      <c r="U38" s="26"/>
-      <c r="V38" s="26"/>
-      <c r="W38" s="26"/>
-      <c r="X38" s="26"/>
-      <c r="Y38" s="26"/>
+      <c r="N38" s="27"/>
+      <c r="O38" s="27"/>
+      <c r="P38" s="27"/>
+      <c r="Q38" s="27"/>
+      <c r="R38" s="27"/>
+      <c r="S38" s="27"/>
+      <c r="T38" s="27"/>
+      <c r="U38" s="27"/>
+      <c r="V38" s="27"/>
+      <c r="W38" s="27"/>
+      <c r="X38" s="27"/>
+      <c r="Y38" s="27"/>
       <c r="Z38" s="14" t="s">
         <v>126</v>
       </c>
@@ -2907,26 +2907,26 @@
       <c r="I39" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J39" s="30" t="s">
+      <c r="J39" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="K39" s="30"/>
-      <c r="L39" s="30"/>
-      <c r="M39" s="27" t="s">
+      <c r="K39" s="28"/>
+      <c r="L39" s="28"/>
+      <c r="M39" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="N39" s="27"/>
-      <c r="O39" s="27"/>
-      <c r="P39" s="27"/>
-      <c r="Q39" s="27"/>
-      <c r="R39" s="27"/>
-      <c r="S39" s="27"/>
-      <c r="T39" s="27"/>
-      <c r="U39" s="27"/>
-      <c r="V39" s="27"/>
-      <c r="W39" s="27"/>
-      <c r="X39" s="27"/>
-      <c r="Y39" s="27"/>
+      <c r="N39" s="30"/>
+      <c r="O39" s="30"/>
+      <c r="P39" s="30"/>
+      <c r="Q39" s="30"/>
+      <c r="R39" s="30"/>
+      <c r="S39" s="30"/>
+      <c r="T39" s="30"/>
+      <c r="U39" s="30"/>
+      <c r="V39" s="30"/>
+      <c r="W39" s="30"/>
+      <c r="X39" s="30"/>
+      <c r="Y39" s="30"/>
       <c r="Z39" s="12" t="s">
         <v>127</v>
       </c>
@@ -2942,26 +2942,26 @@
       <c r="I40" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="J40" s="30" t="s">
+      <c r="J40" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="K40" s="30"/>
-      <c r="L40" s="30"/>
-      <c r="M40" s="26" t="s">
+      <c r="K40" s="28"/>
+      <c r="L40" s="28"/>
+      <c r="M40" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="N40" s="26"/>
-      <c r="O40" s="26"/>
-      <c r="P40" s="26"/>
-      <c r="Q40" s="26"/>
-      <c r="R40" s="26"/>
-      <c r="S40" s="26"/>
-      <c r="T40" s="26"/>
-      <c r="U40" s="26"/>
-      <c r="V40" s="26"/>
-      <c r="W40" s="26"/>
-      <c r="X40" s="26"/>
-      <c r="Y40" s="26"/>
+      <c r="N40" s="27"/>
+      <c r="O40" s="27"/>
+      <c r="P40" s="27"/>
+      <c r="Q40" s="27"/>
+      <c r="R40" s="27"/>
+      <c r="S40" s="27"/>
+      <c r="T40" s="27"/>
+      <c r="U40" s="27"/>
+      <c r="V40" s="27"/>
+      <c r="W40" s="27"/>
+      <c r="X40" s="27"/>
+      <c r="Y40" s="27"/>
       <c r="Z40" s="10" t="s">
         <v>130</v>
       </c>
@@ -2977,26 +2977,26 @@
       <c r="I41" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="J41" s="26" t="s">
+      <c r="J41" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="K41" s="26"/>
-      <c r="L41" s="26"/>
-      <c r="M41" s="26" t="s">
+      <c r="K41" s="27"/>
+      <c r="L41" s="27"/>
+      <c r="M41" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="N41" s="26"/>
-      <c r="O41" s="26"/>
-      <c r="P41" s="26"/>
-      <c r="Q41" s="26"/>
-      <c r="R41" s="26"/>
-      <c r="S41" s="26"/>
-      <c r="T41" s="26"/>
-      <c r="U41" s="26"/>
-      <c r="V41" s="26"/>
-      <c r="W41" s="26"/>
-      <c r="X41" s="26"/>
-      <c r="Y41" s="26"/>
+      <c r="N41" s="27"/>
+      <c r="O41" s="27"/>
+      <c r="P41" s="27"/>
+      <c r="Q41" s="27"/>
+      <c r="R41" s="27"/>
+      <c r="S41" s="27"/>
+      <c r="T41" s="27"/>
+      <c r="U41" s="27"/>
+      <c r="V41" s="27"/>
+      <c r="W41" s="27"/>
+      <c r="X41" s="27"/>
+      <c r="Y41" s="27"/>
       <c r="Z41" s="10" t="s">
         <v>129</v>
       </c>
@@ -3012,26 +3012,26 @@
       <c r="I42" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J42" s="30" t="s">
+      <c r="J42" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="K42" s="30"/>
-      <c r="L42" s="30"/>
-      <c r="M42" s="26" t="s">
+      <c r="K42" s="28"/>
+      <c r="L42" s="28"/>
+      <c r="M42" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="N42" s="26"/>
-      <c r="O42" s="26"/>
-      <c r="P42" s="26"/>
-      <c r="Q42" s="26"/>
-      <c r="R42" s="26"/>
-      <c r="S42" s="26"/>
-      <c r="T42" s="26"/>
-      <c r="U42" s="26"/>
-      <c r="V42" s="26"/>
-      <c r="W42" s="26"/>
-      <c r="X42" s="26"/>
-      <c r="Y42" s="26"/>
+      <c r="N42" s="27"/>
+      <c r="O42" s="27"/>
+      <c r="P42" s="27"/>
+      <c r="Q42" s="27"/>
+      <c r="R42" s="27"/>
+      <c r="S42" s="27"/>
+      <c r="T42" s="27"/>
+      <c r="U42" s="27"/>
+      <c r="V42" s="27"/>
+      <c r="W42" s="27"/>
+      <c r="X42" s="27"/>
+      <c r="Y42" s="27"/>
       <c r="Z42" s="14" t="s">
         <v>126</v>
       </c>
@@ -3047,26 +3047,26 @@
       <c r="I43" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J43" s="30" t="s">
+      <c r="J43" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="K43" s="30"/>
-      <c r="L43" s="30"/>
-      <c r="M43" s="27" t="s">
+      <c r="K43" s="28"/>
+      <c r="L43" s="28"/>
+      <c r="M43" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="N43" s="27"/>
-      <c r="O43" s="27"/>
-      <c r="P43" s="27"/>
-      <c r="Q43" s="27"/>
-      <c r="R43" s="27"/>
-      <c r="S43" s="27"/>
-      <c r="T43" s="27"/>
-      <c r="U43" s="27"/>
-      <c r="V43" s="27"/>
-      <c r="W43" s="27"/>
-      <c r="X43" s="27"/>
-      <c r="Y43" s="27"/>
+      <c r="N43" s="30"/>
+      <c r="O43" s="30"/>
+      <c r="P43" s="30"/>
+      <c r="Q43" s="30"/>
+      <c r="R43" s="30"/>
+      <c r="S43" s="30"/>
+      <c r="T43" s="30"/>
+      <c r="U43" s="30"/>
+      <c r="V43" s="30"/>
+      <c r="W43" s="30"/>
+      <c r="X43" s="30"/>
+      <c r="Y43" s="30"/>
       <c r="Z43" s="12" t="s">
         <v>127</v>
       </c>
@@ -3082,26 +3082,26 @@
       <c r="I44" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="J44" s="30" t="s">
+      <c r="J44" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="K44" s="30"/>
-      <c r="L44" s="30"/>
-      <c r="M44" s="26" t="s">
+      <c r="K44" s="28"/>
+      <c r="L44" s="28"/>
+      <c r="M44" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="N44" s="26"/>
-      <c r="O44" s="26"/>
-      <c r="P44" s="26"/>
-      <c r="Q44" s="26"/>
-      <c r="R44" s="26"/>
-      <c r="S44" s="26"/>
-      <c r="T44" s="26"/>
-      <c r="U44" s="26"/>
-      <c r="V44" s="26"/>
-      <c r="W44" s="26"/>
-      <c r="X44" s="26"/>
-      <c r="Y44" s="26"/>
+      <c r="N44" s="27"/>
+      <c r="O44" s="27"/>
+      <c r="P44" s="27"/>
+      <c r="Q44" s="27"/>
+      <c r="R44" s="27"/>
+      <c r="S44" s="27"/>
+      <c r="T44" s="27"/>
+      <c r="U44" s="27"/>
+      <c r="V44" s="27"/>
+      <c r="W44" s="27"/>
+      <c r="X44" s="27"/>
+      <c r="Y44" s="27"/>
       <c r="Z44" s="10" t="s">
         <v>130</v>
       </c>
@@ -3117,26 +3117,26 @@
       <c r="I45" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="J45" s="30" t="s">
+      <c r="J45" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="K45" s="30"/>
-      <c r="L45" s="30"/>
-      <c r="M45" s="26" t="s">
+      <c r="K45" s="28"/>
+      <c r="L45" s="28"/>
+      <c r="M45" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="N45" s="26"/>
-      <c r="O45" s="26"/>
-      <c r="P45" s="26"/>
-      <c r="Q45" s="26"/>
-      <c r="R45" s="26"/>
-      <c r="S45" s="26"/>
-      <c r="T45" s="26"/>
-      <c r="U45" s="26"/>
-      <c r="V45" s="26"/>
-      <c r="W45" s="26"/>
-      <c r="X45" s="26"/>
-      <c r="Y45" s="26"/>
+      <c r="N45" s="27"/>
+      <c r="O45" s="27"/>
+      <c r="P45" s="27"/>
+      <c r="Q45" s="27"/>
+      <c r="R45" s="27"/>
+      <c r="S45" s="27"/>
+      <c r="T45" s="27"/>
+      <c r="U45" s="27"/>
+      <c r="V45" s="27"/>
+      <c r="W45" s="27"/>
+      <c r="X45" s="27"/>
+      <c r="Y45" s="27"/>
       <c r="Z45" s="10" t="s">
         <v>129</v>
       </c>
@@ -3152,77 +3152,50 @@
       <c r="I46" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="J46" s="26" t="s">
+      <c r="J46" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="K46" s="26"/>
-      <c r="L46" s="26"/>
-      <c r="M46" s="26" t="s">
+      <c r="K46" s="27"/>
+      <c r="L46" s="27"/>
+      <c r="M46" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="N46" s="26"/>
-      <c r="O46" s="26"/>
-      <c r="P46" s="26"/>
-      <c r="Q46" s="26"/>
-      <c r="R46" s="26"/>
-      <c r="S46" s="26"/>
-      <c r="T46" s="26"/>
-      <c r="U46" s="26"/>
-      <c r="V46" s="26"/>
-      <c r="W46" s="26"/>
-      <c r="X46" s="26"/>
-      <c r="Y46" s="26"/>
+      <c r="N46" s="27"/>
+      <c r="O46" s="27"/>
+      <c r="P46" s="27"/>
+      <c r="Q46" s="27"/>
+      <c r="R46" s="27"/>
+      <c r="S46" s="27"/>
+      <c r="T46" s="27"/>
+      <c r="U46" s="27"/>
+      <c r="V46" s="27"/>
+      <c r="W46" s="27"/>
+      <c r="X46" s="27"/>
+      <c r="Y46" s="27"/>
       <c r="Z46" s="10" t="s">
         <v>128</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="79">
-    <mergeCell ref="J46:L46"/>
-    <mergeCell ref="J40:L40"/>
-    <mergeCell ref="J41:L41"/>
-    <mergeCell ref="J42:L42"/>
-    <mergeCell ref="J43:L43"/>
-    <mergeCell ref="J44:L44"/>
-    <mergeCell ref="J45:L45"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="M33:Y33"/>
-    <mergeCell ref="J33:L33"/>
-    <mergeCell ref="J34:L34"/>
-    <mergeCell ref="M34:Y34"/>
-    <mergeCell ref="M46:Y46"/>
-    <mergeCell ref="M43:Y43"/>
-    <mergeCell ref="M40:Y40"/>
-    <mergeCell ref="M39:Y39"/>
-    <mergeCell ref="M38:Y38"/>
-    <mergeCell ref="M42:Y42"/>
-    <mergeCell ref="M44:Y44"/>
-    <mergeCell ref="M41:Y41"/>
-    <mergeCell ref="M45:Y45"/>
-    <mergeCell ref="M23:Y23"/>
-    <mergeCell ref="M24:Y24"/>
-    <mergeCell ref="M26:Y26"/>
-    <mergeCell ref="M29:Y29"/>
-    <mergeCell ref="M32:Y32"/>
-    <mergeCell ref="M25:Y25"/>
-    <mergeCell ref="M28:Y28"/>
-    <mergeCell ref="M31:Y31"/>
-    <mergeCell ref="M27:Y27"/>
-    <mergeCell ref="M30:Y30"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="J37:L37"/>
-    <mergeCell ref="J38:L38"/>
-    <mergeCell ref="J39:L39"/>
-    <mergeCell ref="M37:Y37"/>
-    <mergeCell ref="J31:L31"/>
-    <mergeCell ref="M36:Y36"/>
-    <mergeCell ref="M35:Y35"/>
+    <mergeCell ref="Z10:Z12"/>
+    <mergeCell ref="M17:Y17"/>
+    <mergeCell ref="M20:Y20"/>
+    <mergeCell ref="M22:Y22"/>
+    <mergeCell ref="M16:Y16"/>
+    <mergeCell ref="M18:Y18"/>
+    <mergeCell ref="M19:Y19"/>
+    <mergeCell ref="M21:Y21"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="M13:Y13"/>
+    <mergeCell ref="M14:Y14"/>
+    <mergeCell ref="M10:Y12"/>
+    <mergeCell ref="M15:Y15"/>
+    <mergeCell ref="J12:K12"/>
     <mergeCell ref="I10:I12"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="J32:L32"/>
@@ -3239,24 +3212,51 @@
     <mergeCell ref="J17:K17"/>
     <mergeCell ref="K22:L22"/>
     <mergeCell ref="J16:L16"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="M13:Y13"/>
-    <mergeCell ref="M14:Y14"/>
-    <mergeCell ref="M10:Y12"/>
-    <mergeCell ref="M15:Y15"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="Z10:Z12"/>
-    <mergeCell ref="M17:Y17"/>
-    <mergeCell ref="M20:Y20"/>
-    <mergeCell ref="M22:Y22"/>
-    <mergeCell ref="M16:Y16"/>
-    <mergeCell ref="M18:Y18"/>
-    <mergeCell ref="M19:Y19"/>
-    <mergeCell ref="M21:Y21"/>
+    <mergeCell ref="J37:L37"/>
+    <mergeCell ref="J38:L38"/>
+    <mergeCell ref="J39:L39"/>
+    <mergeCell ref="M37:Y37"/>
+    <mergeCell ref="J31:L31"/>
+    <mergeCell ref="M36:Y36"/>
+    <mergeCell ref="M35:Y35"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="M23:Y23"/>
+    <mergeCell ref="M24:Y24"/>
+    <mergeCell ref="M26:Y26"/>
+    <mergeCell ref="M29:Y29"/>
+    <mergeCell ref="M32:Y32"/>
+    <mergeCell ref="M25:Y25"/>
+    <mergeCell ref="M28:Y28"/>
+    <mergeCell ref="M31:Y31"/>
+    <mergeCell ref="M27:Y27"/>
+    <mergeCell ref="M30:Y30"/>
+    <mergeCell ref="M46:Y46"/>
+    <mergeCell ref="M43:Y43"/>
+    <mergeCell ref="M40:Y40"/>
+    <mergeCell ref="M39:Y39"/>
+    <mergeCell ref="M38:Y38"/>
+    <mergeCell ref="M42:Y42"/>
+    <mergeCell ref="M44:Y44"/>
+    <mergeCell ref="M41:Y41"/>
+    <mergeCell ref="M45:Y45"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="M33:Y33"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="J34:L34"/>
+    <mergeCell ref="M34:Y34"/>
+    <mergeCell ref="J46:L46"/>
+    <mergeCell ref="J40:L40"/>
+    <mergeCell ref="J41:L41"/>
+    <mergeCell ref="J42:L42"/>
+    <mergeCell ref="J43:L43"/>
+    <mergeCell ref="J44:L44"/>
+    <mergeCell ref="J45:L45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3298,28 +3298,28 @@
       <c r="H2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
       <c r="L2" s="9" t="s">
         <v>59</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="N2" s="28" t="s">
+      <c r="N2" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28" t="s">
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
       <c r="U2" s="9" t="s">
         <v>63</v>
       </c>
@@ -3409,11 +3409,11 @@
       <c r="H9" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="I9" s="26" t="s">
+      <c r="I9" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
       <c r="L9" s="9" t="s">
         <v>2</v>
       </c>
@@ -3461,30 +3461,30 @@
       <c r="B10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H10" s="27" t="s">
+      <c r="H10" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="I10" s="26" t="s">
+      <c r="I10" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="27" t="s">
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="M10" s="27"/>
-      <c r="N10" s="27"/>
-      <c r="O10" s="27"/>
-      <c r="P10" s="27"/>
-      <c r="Q10" s="27"/>
-      <c r="R10" s="27"/>
-      <c r="S10" s="27"/>
-      <c r="T10" s="27"/>
-      <c r="U10" s="27"/>
-      <c r="V10" s="27"/>
-      <c r="W10" s="27"/>
-      <c r="X10" s="27"/>
-      <c r="Y10" s="25" t="s">
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="30"/>
+      <c r="R10" s="30"/>
+      <c r="S10" s="30"/>
+      <c r="T10" s="30"/>
+      <c r="U10" s="30"/>
+      <c r="V10" s="30"/>
+      <c r="W10" s="30"/>
+      <c r="X10" s="30"/>
+      <c r="Y10" s="34" t="s">
         <v>125</v>
       </c>
     </row>
@@ -3492,334 +3492,334 @@
       <c r="B11" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="27"/>
-      <c r="I11" s="29" t="s">
+      <c r="H11" s="30"/>
+      <c r="I11" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27"/>
-      <c r="N11" s="27"/>
-      <c r="O11" s="27"/>
-      <c r="P11" s="27"/>
-      <c r="Q11" s="27"/>
-      <c r="R11" s="27"/>
-      <c r="S11" s="27"/>
-      <c r="T11" s="27"/>
-      <c r="U11" s="27"/>
-      <c r="V11" s="27"/>
-      <c r="W11" s="27"/>
-      <c r="X11" s="27"/>
-      <c r="Y11" s="25"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="30"/>
+      <c r="R11" s="30"/>
+      <c r="S11" s="30"/>
+      <c r="T11" s="30"/>
+      <c r="U11" s="30"/>
+      <c r="V11" s="30"/>
+      <c r="W11" s="30"/>
+      <c r="X11" s="30"/>
+      <c r="Y11" s="34"/>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>4</v>
       </c>
-      <c r="H12" s="27"/>
-      <c r="I12" s="30" t="s">
+      <c r="H12" s="30"/>
+      <c r="I12" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="J12" s="26"/>
+      <c r="J12" s="27"/>
       <c r="K12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="L12" s="27"/>
-      <c r="M12" s="27"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="27"/>
-      <c r="P12" s="27"/>
-      <c r="Q12" s="27"/>
-      <c r="R12" s="27"/>
-      <c r="S12" s="27"/>
-      <c r="T12" s="27"/>
-      <c r="U12" s="27"/>
-      <c r="V12" s="27"/>
-      <c r="W12" s="27"/>
-      <c r="X12" s="27"/>
-      <c r="Y12" s="25"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="30"/>
+      <c r="R12" s="30"/>
+      <c r="S12" s="30"/>
+      <c r="T12" s="30"/>
+      <c r="U12" s="30"/>
+      <c r="V12" s="30"/>
+      <c r="W12" s="30"/>
+      <c r="X12" s="30"/>
+      <c r="Y12" s="34"/>
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>90</v>
       </c>
       <c r="C13" s="6"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="26" t="s">
+      <c r="H13" s="30"/>
+      <c r="I13" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="27"/>
-      <c r="R13" s="27"/>
-      <c r="S13" s="27"/>
-      <c r="T13" s="27"/>
-      <c r="U13" s="27"/>
-      <c r="V13" s="27"/>
-      <c r="W13" s="27"/>
-      <c r="X13" s="27"/>
-      <c r="Y13" s="25"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="30"/>
+      <c r="R13" s="30"/>
+      <c r="S13" s="30"/>
+      <c r="T13" s="30"/>
+      <c r="U13" s="30"/>
+      <c r="V13" s="30"/>
+      <c r="W13" s="30"/>
+      <c r="X13" s="30"/>
+      <c r="Y13" s="34"/>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>78</v>
       </c>
-      <c r="H14" s="27"/>
-      <c r="I14" s="29" t="s">
+      <c r="H14" s="30"/>
+      <c r="I14" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="27"/>
-      <c r="N14" s="27"/>
-      <c r="O14" s="27"/>
-      <c r="P14" s="27"/>
-      <c r="Q14" s="27"/>
-      <c r="R14" s="27"/>
-      <c r="S14" s="27"/>
-      <c r="T14" s="27"/>
-      <c r="U14" s="27"/>
-      <c r="V14" s="27"/>
-      <c r="W14" s="27"/>
-      <c r="X14" s="27"/>
-      <c r="Y14" s="25"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="30"/>
+      <c r="R14" s="30"/>
+      <c r="S14" s="30"/>
+      <c r="T14" s="30"/>
+      <c r="U14" s="30"/>
+      <c r="V14" s="30"/>
+      <c r="W14" s="30"/>
+      <c r="X14" s="30"/>
+      <c r="Y14" s="34"/>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>5</v>
       </c>
-      <c r="H15" s="27"/>
-      <c r="I15" s="28" t="s">
+      <c r="H15" s="30"/>
+      <c r="I15" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="27"/>
-      <c r="N15" s="27"/>
-      <c r="O15" s="27"/>
-      <c r="P15" s="27"/>
-      <c r="Q15" s="27"/>
-      <c r="R15" s="27"/>
-      <c r="S15" s="27"/>
-      <c r="T15" s="27"/>
-      <c r="U15" s="27"/>
-      <c r="V15" s="27"/>
-      <c r="W15" s="27"/>
-      <c r="X15" s="27"/>
-      <c r="Y15" s="25"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="30"/>
+      <c r="R15" s="30"/>
+      <c r="S15" s="30"/>
+      <c r="T15" s="30"/>
+      <c r="U15" s="30"/>
+      <c r="V15" s="30"/>
+      <c r="W15" s="30"/>
+      <c r="X15" s="30"/>
+      <c r="Y15" s="34"/>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>79</v>
       </c>
-      <c r="H16" s="27"/>
-      <c r="I16" s="29" t="s">
+      <c r="H16" s="30"/>
+      <c r="I16" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="27"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="27"/>
-      <c r="P16" s="27"/>
-      <c r="Q16" s="27"/>
-      <c r="R16" s="27"/>
-      <c r="S16" s="27"/>
-      <c r="T16" s="27"/>
-      <c r="U16" s="27"/>
-      <c r="V16" s="27"/>
-      <c r="W16" s="27"/>
-      <c r="X16" s="27"/>
-      <c r="Y16" s="25"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="30"/>
+      <c r="R16" s="30"/>
+      <c r="S16" s="30"/>
+      <c r="T16" s="30"/>
+      <c r="U16" s="30"/>
+      <c r="V16" s="30"/>
+      <c r="W16" s="30"/>
+      <c r="X16" s="30"/>
+      <c r="Y16" s="34"/>
     </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="27"/>
-      <c r="I17" s="28" t="s">
+      <c r="H17" s="30"/>
+      <c r="I17" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="J17" s="28"/>
+      <c r="J17" s="32"/>
       <c r="K17" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="L17" s="27"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="27"/>
-      <c r="O17" s="27"/>
-      <c r="P17" s="27"/>
-      <c r="Q17" s="27"/>
-      <c r="R17" s="27"/>
-      <c r="S17" s="27"/>
-      <c r="T17" s="27"/>
-      <c r="U17" s="27"/>
-      <c r="V17" s="27"/>
-      <c r="W17" s="27"/>
-      <c r="X17" s="27"/>
-      <c r="Y17" s="25"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="30"/>
+      <c r="P17" s="30"/>
+      <c r="Q17" s="30"/>
+      <c r="R17" s="30"/>
+      <c r="S17" s="30"/>
+      <c r="T17" s="30"/>
+      <c r="U17" s="30"/>
+      <c r="V17" s="30"/>
+      <c r="W17" s="30"/>
+      <c r="X17" s="30"/>
+      <c r="Y17" s="34"/>
     </row>
     <row r="18" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>80</v>
       </c>
-      <c r="H18" s="27"/>
-      <c r="I18" s="29" t="s">
+      <c r="H18" s="30"/>
+      <c r="I18" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="J18" s="29"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="27"/>
-      <c r="N18" s="27"/>
-      <c r="O18" s="27"/>
-      <c r="P18" s="27"/>
-      <c r="Q18" s="27"/>
-      <c r="R18" s="27"/>
-      <c r="S18" s="27"/>
-      <c r="T18" s="27"/>
-      <c r="U18" s="27"/>
-      <c r="V18" s="27"/>
-      <c r="W18" s="27"/>
-      <c r="X18" s="27"/>
-      <c r="Y18" s="25"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="30"/>
+      <c r="P18" s="30"/>
+      <c r="Q18" s="30"/>
+      <c r="R18" s="30"/>
+      <c r="S18" s="30"/>
+      <c r="T18" s="30"/>
+      <c r="U18" s="30"/>
+      <c r="V18" s="30"/>
+      <c r="W18" s="30"/>
+      <c r="X18" s="30"/>
+      <c r="Y18" s="34"/>
     </row>
     <row r="19" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
         <v>91</v>
       </c>
       <c r="C19" s="6"/>
-      <c r="H19" s="27"/>
+      <c r="H19" s="30"/>
       <c r="I19" s="31" t="s">
         <v>75</v>
       </c>
       <c r="J19" s="31"/>
       <c r="K19" s="31"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="27"/>
-      <c r="N19" s="27"/>
-      <c r="O19" s="27"/>
-      <c r="P19" s="27"/>
-      <c r="Q19" s="27"/>
-      <c r="R19" s="27"/>
-      <c r="S19" s="27"/>
-      <c r="T19" s="27"/>
-      <c r="U19" s="27"/>
-      <c r="V19" s="27"/>
-      <c r="W19" s="27"/>
-      <c r="X19" s="27"/>
-      <c r="Y19" s="25"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="30"/>
+      <c r="P19" s="30"/>
+      <c r="Q19" s="30"/>
+      <c r="R19" s="30"/>
+      <c r="S19" s="30"/>
+      <c r="T19" s="30"/>
+      <c r="U19" s="30"/>
+      <c r="V19" s="30"/>
+      <c r="W19" s="30"/>
+      <c r="X19" s="30"/>
+      <c r="Y19" s="34"/>
     </row>
     <row r="20" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>7</v>
       </c>
-      <c r="H20" s="27"/>
-      <c r="I20" s="28" t="s">
+      <c r="H20" s="30"/>
+      <c r="I20" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="27"/>
-      <c r="N20" s="27"/>
-      <c r="O20" s="27"/>
-      <c r="P20" s="27"/>
-      <c r="Q20" s="27"/>
-      <c r="R20" s="27"/>
-      <c r="S20" s="27"/>
-      <c r="T20" s="27"/>
-      <c r="U20" s="27"/>
-      <c r="V20" s="27"/>
-      <c r="W20" s="27"/>
-      <c r="X20" s="27"/>
-      <c r="Y20" s="25"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="30"/>
+      <c r="P20" s="30"/>
+      <c r="Q20" s="30"/>
+      <c r="R20" s="30"/>
+      <c r="S20" s="30"/>
+      <c r="T20" s="30"/>
+      <c r="U20" s="30"/>
+      <c r="V20" s="30"/>
+      <c r="W20" s="30"/>
+      <c r="X20" s="30"/>
+      <c r="Y20" s="34"/>
     </row>
     <row r="21" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>81</v>
       </c>
-      <c r="H21" s="27"/>
-      <c r="I21" s="29" t="s">
+      <c r="H21" s="30"/>
+      <c r="I21" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="27"/>
-      <c r="N21" s="27"/>
-      <c r="O21" s="27"/>
-      <c r="P21" s="27"/>
-      <c r="Q21" s="27"/>
-      <c r="R21" s="27"/>
-      <c r="S21" s="27"/>
-      <c r="T21" s="27"/>
-      <c r="U21" s="27"/>
-      <c r="V21" s="27"/>
-      <c r="W21" s="27"/>
-      <c r="X21" s="27"/>
-      <c r="Y21" s="25"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="30"/>
+      <c r="P21" s="30"/>
+      <c r="Q21" s="30"/>
+      <c r="R21" s="30"/>
+      <c r="S21" s="30"/>
+      <c r="T21" s="30"/>
+      <c r="U21" s="30"/>
+      <c r="V21" s="30"/>
+      <c r="W21" s="30"/>
+      <c r="X21" s="30"/>
+      <c r="Y21" s="34"/>
     </row>
     <row r="22" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>11</v>
       </c>
-      <c r="H22" s="27"/>
+      <c r="H22" s="30"/>
       <c r="I22" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="J22" s="28" t="s">
+      <c r="J22" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="K22" s="28"/>
-      <c r="L22" s="27"/>
-      <c r="M22" s="27"/>
-      <c r="N22" s="27"/>
-      <c r="O22" s="27"/>
-      <c r="P22" s="27"/>
-      <c r="Q22" s="27"/>
-      <c r="R22" s="27"/>
-      <c r="S22" s="27"/>
-      <c r="T22" s="27"/>
-      <c r="U22" s="27"/>
-      <c r="V22" s="27"/>
-      <c r="W22" s="27"/>
-      <c r="X22" s="27"/>
-      <c r="Y22" s="25"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="30"/>
+      <c r="P22" s="30"/>
+      <c r="Q22" s="30"/>
+      <c r="R22" s="30"/>
+      <c r="S22" s="30"/>
+      <c r="T22" s="30"/>
+      <c r="U22" s="30"/>
+      <c r="V22" s="30"/>
+      <c r="W22" s="30"/>
+      <c r="X22" s="30"/>
+      <c r="Y22" s="34"/>
     </row>
     <row r="23" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C23" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H23" s="27"/>
-      <c r="I23" s="30" t="s">
+      <c r="H23" s="30"/>
+      <c r="I23" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="J23" s="30"/>
-      <c r="K23" s="30"/>
-      <c r="L23" s="27"/>
-      <c r="M23" s="27"/>
-      <c r="N23" s="27"/>
-      <c r="O23" s="27"/>
-      <c r="P23" s="27"/>
-      <c r="Q23" s="27"/>
-      <c r="R23" s="27"/>
-      <c r="S23" s="27"/>
-      <c r="T23" s="27"/>
-      <c r="U23" s="27"/>
-      <c r="V23" s="27"/>
-      <c r="W23" s="27"/>
-      <c r="X23" s="27"/>
-      <c r="Y23" s="25"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="28"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="30"/>
+      <c r="P23" s="30"/>
+      <c r="Q23" s="30"/>
+      <c r="R23" s="30"/>
+      <c r="S23" s="30"/>
+      <c r="T23" s="30"/>
+      <c r="U23" s="30"/>
+      <c r="V23" s="30"/>
+      <c r="W23" s="30"/>
+      <c r="X23" s="30"/>
+      <c r="Y23" s="34"/>
     </row>
     <row r="24" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
@@ -3827,280 +3827,280 @@
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="26" t="s">
+      <c r="H24" s="30"/>
+      <c r="I24" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27"/>
-      <c r="N24" s="27"/>
-      <c r="O24" s="27"/>
-      <c r="P24" s="27"/>
-      <c r="Q24" s="27"/>
-      <c r="R24" s="27"/>
-      <c r="S24" s="27"/>
-      <c r="T24" s="27"/>
-      <c r="U24" s="27"/>
-      <c r="V24" s="27"/>
-      <c r="W24" s="27"/>
-      <c r="X24" s="27"/>
-      <c r="Y24" s="25"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="30"/>
+      <c r="O24" s="30"/>
+      <c r="P24" s="30"/>
+      <c r="Q24" s="30"/>
+      <c r="R24" s="30"/>
+      <c r="S24" s="30"/>
+      <c r="T24" s="30"/>
+      <c r="U24" s="30"/>
+      <c r="V24" s="30"/>
+      <c r="W24" s="30"/>
+      <c r="X24" s="30"/>
+      <c r="Y24" s="34"/>
     </row>
     <row r="25" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>20</v>
       </c>
-      <c r="H25" s="27"/>
-      <c r="I25" s="28" t="s">
+      <c r="H25" s="30"/>
+      <c r="I25" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="J25" s="28"/>
-      <c r="K25" s="28"/>
-      <c r="L25" s="27"/>
-      <c r="M25" s="27"/>
-      <c r="N25" s="27"/>
-      <c r="O25" s="27"/>
-      <c r="P25" s="27"/>
-      <c r="Q25" s="27"/>
-      <c r="R25" s="27"/>
-      <c r="S25" s="27"/>
-      <c r="T25" s="27"/>
-      <c r="U25" s="27"/>
-      <c r="V25" s="27"/>
-      <c r="W25" s="27"/>
-      <c r="X25" s="27"/>
-      <c r="Y25" s="25"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="30"/>
+      <c r="M25" s="30"/>
+      <c r="N25" s="30"/>
+      <c r="O25" s="30"/>
+      <c r="P25" s="30"/>
+      <c r="Q25" s="30"/>
+      <c r="R25" s="30"/>
+      <c r="S25" s="30"/>
+      <c r="T25" s="30"/>
+      <c r="U25" s="30"/>
+      <c r="V25" s="30"/>
+      <c r="W25" s="30"/>
+      <c r="X25" s="30"/>
+      <c r="Y25" s="34"/>
     </row>
     <row r="26" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>82</v>
       </c>
-      <c r="H26" s="27"/>
-      <c r="I26" s="29" t="s">
+      <c r="H26" s="30"/>
+      <c r="I26" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="J26" s="29"/>
-      <c r="K26" s="29"/>
-      <c r="L26" s="27"/>
-      <c r="M26" s="27"/>
-      <c r="N26" s="27"/>
-      <c r="O26" s="27"/>
-      <c r="P26" s="27"/>
-      <c r="Q26" s="27"/>
-      <c r="R26" s="27"/>
-      <c r="S26" s="27"/>
-      <c r="T26" s="27"/>
-      <c r="U26" s="27"/>
-      <c r="V26" s="27"/>
-      <c r="W26" s="27"/>
-      <c r="X26" s="27"/>
-      <c r="Y26" s="25"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="33"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="30"/>
+      <c r="N26" s="30"/>
+      <c r="O26" s="30"/>
+      <c r="P26" s="30"/>
+      <c r="Q26" s="30"/>
+      <c r="R26" s="30"/>
+      <c r="S26" s="30"/>
+      <c r="T26" s="30"/>
+      <c r="U26" s="30"/>
+      <c r="V26" s="30"/>
+      <c r="W26" s="30"/>
+      <c r="X26" s="30"/>
+      <c r="Y26" s="34"/>
     </row>
     <row r="27" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>12</v>
       </c>
-      <c r="H27" s="27"/>
-      <c r="I27" s="28" t="s">
+      <c r="H27" s="30"/>
+      <c r="I27" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="J27" s="28"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="27"/>
-      <c r="M27" s="27"/>
-      <c r="N27" s="27"/>
-      <c r="O27" s="27"/>
-      <c r="P27" s="27"/>
-      <c r="Q27" s="27"/>
-      <c r="R27" s="27"/>
-      <c r="S27" s="27"/>
-      <c r="T27" s="27"/>
-      <c r="U27" s="27"/>
-      <c r="V27" s="27"/>
-      <c r="W27" s="27"/>
-      <c r="X27" s="27"/>
-      <c r="Y27" s="25"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="32"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="30"/>
+      <c r="O27" s="30"/>
+      <c r="P27" s="30"/>
+      <c r="Q27" s="30"/>
+      <c r="R27" s="30"/>
+      <c r="S27" s="30"/>
+      <c r="T27" s="30"/>
+      <c r="U27" s="30"/>
+      <c r="V27" s="30"/>
+      <c r="W27" s="30"/>
+      <c r="X27" s="30"/>
+      <c r="Y27" s="34"/>
     </row>
     <row r="28" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>9</v>
       </c>
-      <c r="H28" s="27"/>
-      <c r="I28" s="28" t="s">
+      <c r="H28" s="30"/>
+      <c r="I28" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="27"/>
-      <c r="M28" s="27"/>
-      <c r="N28" s="27"/>
-      <c r="O28" s="27"/>
-      <c r="P28" s="27"/>
-      <c r="Q28" s="27"/>
-      <c r="R28" s="27"/>
-      <c r="S28" s="27"/>
-      <c r="T28" s="27"/>
-      <c r="U28" s="27"/>
-      <c r="V28" s="27"/>
-      <c r="W28" s="27"/>
-      <c r="X28" s="27"/>
-      <c r="Y28" s="25"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="32"/>
+      <c r="L28" s="30"/>
+      <c r="M28" s="30"/>
+      <c r="N28" s="30"/>
+      <c r="O28" s="30"/>
+      <c r="P28" s="30"/>
+      <c r="Q28" s="30"/>
+      <c r="R28" s="30"/>
+      <c r="S28" s="30"/>
+      <c r="T28" s="30"/>
+      <c r="U28" s="30"/>
+      <c r="V28" s="30"/>
+      <c r="W28" s="30"/>
+      <c r="X28" s="30"/>
+      <c r="Y28" s="34"/>
     </row>
     <row r="29" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>83</v>
       </c>
-      <c r="H29" s="27"/>
-      <c r="I29" s="29" t="s">
+      <c r="H29" s="30"/>
+      <c r="I29" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="J29" s="29"/>
-      <c r="K29" s="29"/>
-      <c r="L29" s="27"/>
-      <c r="M29" s="27"/>
-      <c r="N29" s="27"/>
-      <c r="O29" s="27"/>
-      <c r="P29" s="27"/>
-      <c r="Q29" s="27"/>
-      <c r="R29" s="27"/>
-      <c r="S29" s="27"/>
-      <c r="T29" s="27"/>
-      <c r="U29" s="27"/>
-      <c r="V29" s="27"/>
-      <c r="W29" s="27"/>
-      <c r="X29" s="27"/>
-      <c r="Y29" s="25"/>
+      <c r="J29" s="33"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="30"/>
+      <c r="M29" s="30"/>
+      <c r="N29" s="30"/>
+      <c r="O29" s="30"/>
+      <c r="P29" s="30"/>
+      <c r="Q29" s="30"/>
+      <c r="R29" s="30"/>
+      <c r="S29" s="30"/>
+      <c r="T29" s="30"/>
+      <c r="U29" s="30"/>
+      <c r="V29" s="30"/>
+      <c r="W29" s="30"/>
+      <c r="X29" s="30"/>
+      <c r="Y29" s="34"/>
     </row>
     <row r="30" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>13</v>
       </c>
-      <c r="H30" s="27"/>
+      <c r="H30" s="30"/>
       <c r="I30" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J30" s="32" t="s">
+      <c r="J30" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="K30" s="32"/>
-      <c r="L30" s="27"/>
-      <c r="M30" s="27"/>
-      <c r="N30" s="27"/>
-      <c r="O30" s="27"/>
-      <c r="P30" s="27"/>
-      <c r="Q30" s="27"/>
-      <c r="R30" s="27"/>
-      <c r="S30" s="27"/>
-      <c r="T30" s="27"/>
-      <c r="U30" s="27"/>
-      <c r="V30" s="27"/>
-      <c r="W30" s="27"/>
-      <c r="X30" s="27"/>
-      <c r="Y30" s="25"/>
+      <c r="K30" s="29"/>
+      <c r="L30" s="30"/>
+      <c r="M30" s="30"/>
+      <c r="N30" s="30"/>
+      <c r="O30" s="30"/>
+      <c r="P30" s="30"/>
+      <c r="Q30" s="30"/>
+      <c r="R30" s="30"/>
+      <c r="S30" s="30"/>
+      <c r="T30" s="30"/>
+      <c r="U30" s="30"/>
+      <c r="V30" s="30"/>
+      <c r="W30" s="30"/>
+      <c r="X30" s="30"/>
+      <c r="Y30" s="34"/>
     </row>
     <row r="31" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>19</v>
       </c>
-      <c r="H31" s="27"/>
-      <c r="I31" s="28" t="s">
+      <c r="H31" s="30"/>
+      <c r="I31" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="J31" s="28"/>
-      <c r="K31" s="28"/>
-      <c r="L31" s="27"/>
-      <c r="M31" s="27"/>
-      <c r="N31" s="27"/>
-      <c r="O31" s="27"/>
-      <c r="P31" s="27"/>
-      <c r="Q31" s="27"/>
-      <c r="R31" s="27"/>
-      <c r="S31" s="27"/>
-      <c r="T31" s="27"/>
-      <c r="U31" s="27"/>
-      <c r="V31" s="27"/>
-      <c r="W31" s="27"/>
-      <c r="X31" s="27"/>
-      <c r="Y31" s="25"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="32"/>
+      <c r="L31" s="30"/>
+      <c r="M31" s="30"/>
+      <c r="N31" s="30"/>
+      <c r="O31" s="30"/>
+      <c r="P31" s="30"/>
+      <c r="Q31" s="30"/>
+      <c r="R31" s="30"/>
+      <c r="S31" s="30"/>
+      <c r="T31" s="30"/>
+      <c r="U31" s="30"/>
+      <c r="V31" s="30"/>
+      <c r="W31" s="30"/>
+      <c r="X31" s="30"/>
+      <c r="Y31" s="34"/>
     </row>
     <row r="32" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>85</v>
       </c>
-      <c r="H32" s="27"/>
-      <c r="I32" s="29" t="s">
+      <c r="H32" s="30"/>
+      <c r="I32" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="J32" s="29"/>
-      <c r="K32" s="29"/>
-      <c r="L32" s="27"/>
-      <c r="M32" s="27"/>
-      <c r="N32" s="27"/>
-      <c r="O32" s="27"/>
-      <c r="P32" s="27"/>
-      <c r="Q32" s="27"/>
-      <c r="R32" s="27"/>
-      <c r="S32" s="27"/>
-      <c r="T32" s="27"/>
-      <c r="U32" s="27"/>
-      <c r="V32" s="27"/>
-      <c r="W32" s="27"/>
-      <c r="X32" s="27"/>
-      <c r="Y32" s="25"/>
+      <c r="J32" s="33"/>
+      <c r="K32" s="33"/>
+      <c r="L32" s="30"/>
+      <c r="M32" s="30"/>
+      <c r="N32" s="30"/>
+      <c r="O32" s="30"/>
+      <c r="P32" s="30"/>
+      <c r="Q32" s="30"/>
+      <c r="R32" s="30"/>
+      <c r="S32" s="30"/>
+      <c r="T32" s="30"/>
+      <c r="U32" s="30"/>
+      <c r="V32" s="30"/>
+      <c r="W32" s="30"/>
+      <c r="X32" s="30"/>
+      <c r="Y32" s="34"/>
     </row>
     <row r="33" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
         <v>84</v>
       </c>
       <c r="C33" s="6"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="32" t="s">
+      <c r="H33" s="30"/>
+      <c r="I33" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="J33" s="32"/>
-      <c r="K33" s="32"/>
-      <c r="L33" s="27"/>
-      <c r="M33" s="27"/>
-      <c r="N33" s="27"/>
-      <c r="O33" s="27"/>
-      <c r="P33" s="27"/>
-      <c r="Q33" s="27"/>
-      <c r="R33" s="27"/>
-      <c r="S33" s="27"/>
-      <c r="T33" s="27"/>
-      <c r="U33" s="27"/>
-      <c r="V33" s="27"/>
-      <c r="W33" s="27"/>
-      <c r="X33" s="27"/>
-      <c r="Y33" s="25"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="29"/>
+      <c r="L33" s="30"/>
+      <c r="M33" s="30"/>
+      <c r="N33" s="30"/>
+      <c r="O33" s="30"/>
+      <c r="P33" s="30"/>
+      <c r="Q33" s="30"/>
+      <c r="R33" s="30"/>
+      <c r="S33" s="30"/>
+      <c r="T33" s="30"/>
+      <c r="U33" s="30"/>
+      <c r="V33" s="30"/>
+      <c r="W33" s="30"/>
+      <c r="X33" s="30"/>
+      <c r="Y33" s="34"/>
     </row>
     <row r="34" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="s">
         <v>118</v>
       </c>
       <c r="C34" s="6"/>
-      <c r="H34" s="27"/>
+      <c r="H34" s="30"/>
       <c r="I34" s="31" t="s">
         <v>75</v>
       </c>
       <c r="J34" s="31"/>
       <c r="K34" s="31"/>
-      <c r="L34" s="27"/>
-      <c r="M34" s="27"/>
-      <c r="N34" s="27"/>
-      <c r="O34" s="27"/>
-      <c r="P34" s="27"/>
-      <c r="Q34" s="27"/>
-      <c r="R34" s="27"/>
-      <c r="S34" s="27"/>
-      <c r="T34" s="27"/>
-      <c r="U34" s="27"/>
-      <c r="V34" s="27"/>
-      <c r="W34" s="27"/>
-      <c r="X34" s="27"/>
-      <c r="Y34" s="25"/>
+      <c r="L34" s="30"/>
+      <c r="M34" s="30"/>
+      <c r="N34" s="30"/>
+      <c r="O34" s="30"/>
+      <c r="P34" s="30"/>
+      <c r="Q34" s="30"/>
+      <c r="R34" s="30"/>
+      <c r="S34" s="30"/>
+      <c r="T34" s="30"/>
+      <c r="U34" s="30"/>
+      <c r="V34" s="30"/>
+      <c r="W34" s="30"/>
+      <c r="X34" s="30"/>
+      <c r="Y34" s="34"/>
     </row>
     <row r="35" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
@@ -4109,26 +4109,26 @@
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="30" t="s">
+      <c r="H35" s="30"/>
+      <c r="I35" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="J35" s="30"/>
-      <c r="K35" s="30"/>
-      <c r="L35" s="27"/>
-      <c r="M35" s="27"/>
-      <c r="N35" s="27"/>
-      <c r="O35" s="27"/>
-      <c r="P35" s="27"/>
-      <c r="Q35" s="27"/>
-      <c r="R35" s="27"/>
-      <c r="S35" s="27"/>
-      <c r="T35" s="27"/>
-      <c r="U35" s="27"/>
-      <c r="V35" s="27"/>
-      <c r="W35" s="27"/>
-      <c r="X35" s="27"/>
-      <c r="Y35" s="25"/>
+      <c r="J35" s="28"/>
+      <c r="K35" s="28"/>
+      <c r="L35" s="30"/>
+      <c r="M35" s="30"/>
+      <c r="N35" s="30"/>
+      <c r="O35" s="30"/>
+      <c r="P35" s="30"/>
+      <c r="Q35" s="30"/>
+      <c r="R35" s="30"/>
+      <c r="S35" s="30"/>
+      <c r="T35" s="30"/>
+      <c r="U35" s="30"/>
+      <c r="V35" s="30"/>
+      <c r="W35" s="30"/>
+      <c r="X35" s="30"/>
+      <c r="Y35" s="34"/>
     </row>
     <row r="36" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B36" s="6"/>
@@ -4137,26 +4137,26 @@
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
-      <c r="H36" s="27"/>
-      <c r="I36" s="30" t="s">
+      <c r="H36" s="30"/>
+      <c r="I36" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="J36" s="30"/>
-      <c r="K36" s="30"/>
-      <c r="L36" s="27"/>
-      <c r="M36" s="27"/>
-      <c r="N36" s="27"/>
-      <c r="O36" s="27"/>
-      <c r="P36" s="27"/>
-      <c r="Q36" s="27"/>
-      <c r="R36" s="27"/>
-      <c r="S36" s="27"/>
-      <c r="T36" s="27"/>
-      <c r="U36" s="27"/>
-      <c r="V36" s="27"/>
-      <c r="W36" s="27"/>
-      <c r="X36" s="27"/>
-      <c r="Y36" s="25"/>
+      <c r="J36" s="28"/>
+      <c r="K36" s="28"/>
+      <c r="L36" s="30"/>
+      <c r="M36" s="30"/>
+      <c r="N36" s="30"/>
+      <c r="O36" s="30"/>
+      <c r="P36" s="30"/>
+      <c r="Q36" s="30"/>
+      <c r="R36" s="30"/>
+      <c r="S36" s="30"/>
+      <c r="T36" s="30"/>
+      <c r="U36" s="30"/>
+      <c r="V36" s="30"/>
+      <c r="W36" s="30"/>
+      <c r="X36" s="30"/>
+      <c r="Y36" s="34"/>
     </row>
     <row r="37" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
@@ -4165,26 +4165,26 @@
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
-      <c r="H37" s="27"/>
-      <c r="I37" s="26" t="s">
+      <c r="H37" s="30"/>
+      <c r="I37" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="J37" s="26"/>
-      <c r="K37" s="26"/>
-      <c r="L37" s="27"/>
-      <c r="M37" s="27"/>
-      <c r="N37" s="27"/>
-      <c r="O37" s="27"/>
-      <c r="P37" s="27"/>
-      <c r="Q37" s="27"/>
-      <c r="R37" s="27"/>
-      <c r="S37" s="27"/>
-      <c r="T37" s="27"/>
-      <c r="U37" s="27"/>
-      <c r="V37" s="27"/>
-      <c r="W37" s="27"/>
-      <c r="X37" s="27"/>
-      <c r="Y37" s="25"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="27"/>
+      <c r="L37" s="30"/>
+      <c r="M37" s="30"/>
+      <c r="N37" s="30"/>
+      <c r="O37" s="30"/>
+      <c r="P37" s="30"/>
+      <c r="Q37" s="30"/>
+      <c r="R37" s="30"/>
+      <c r="S37" s="30"/>
+      <c r="T37" s="30"/>
+      <c r="U37" s="30"/>
+      <c r="V37" s="30"/>
+      <c r="W37" s="30"/>
+      <c r="X37" s="30"/>
+      <c r="Y37" s="34"/>
     </row>
     <row r="38" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
@@ -4193,26 +4193,26 @@
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="30" t="s">
+      <c r="H38" s="30"/>
+      <c r="I38" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="J38" s="30"/>
-      <c r="K38" s="30"/>
-      <c r="L38" s="27"/>
-      <c r="M38" s="27"/>
-      <c r="N38" s="27"/>
-      <c r="O38" s="27"/>
-      <c r="P38" s="27"/>
-      <c r="Q38" s="27"/>
-      <c r="R38" s="27"/>
-      <c r="S38" s="27"/>
-      <c r="T38" s="27"/>
-      <c r="U38" s="27"/>
-      <c r="V38" s="27"/>
-      <c r="W38" s="27"/>
-      <c r="X38" s="27"/>
-      <c r="Y38" s="25"/>
+      <c r="J38" s="28"/>
+      <c r="K38" s="28"/>
+      <c r="L38" s="30"/>
+      <c r="M38" s="30"/>
+      <c r="N38" s="30"/>
+      <c r="O38" s="30"/>
+      <c r="P38" s="30"/>
+      <c r="Q38" s="30"/>
+      <c r="R38" s="30"/>
+      <c r="S38" s="30"/>
+      <c r="T38" s="30"/>
+      <c r="U38" s="30"/>
+      <c r="V38" s="30"/>
+      <c r="W38" s="30"/>
+      <c r="X38" s="30"/>
+      <c r="Y38" s="34"/>
     </row>
     <row r="39" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B39" s="6"/>
@@ -4221,26 +4221,26 @@
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
-      <c r="H39" s="27"/>
-      <c r="I39" s="30" t="s">
+      <c r="H39" s="30"/>
+      <c r="I39" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="J39" s="30"/>
-      <c r="K39" s="30"/>
-      <c r="L39" s="27"/>
-      <c r="M39" s="27"/>
-      <c r="N39" s="27"/>
-      <c r="O39" s="27"/>
-      <c r="P39" s="27"/>
-      <c r="Q39" s="27"/>
-      <c r="R39" s="27"/>
-      <c r="S39" s="27"/>
-      <c r="T39" s="27"/>
-      <c r="U39" s="27"/>
-      <c r="V39" s="27"/>
-      <c r="W39" s="27"/>
-      <c r="X39" s="27"/>
-      <c r="Y39" s="25"/>
+      <c r="J39" s="28"/>
+      <c r="K39" s="28"/>
+      <c r="L39" s="30"/>
+      <c r="M39" s="30"/>
+      <c r="N39" s="30"/>
+      <c r="O39" s="30"/>
+      <c r="P39" s="30"/>
+      <c r="Q39" s="30"/>
+      <c r="R39" s="30"/>
+      <c r="S39" s="30"/>
+      <c r="T39" s="30"/>
+      <c r="U39" s="30"/>
+      <c r="V39" s="30"/>
+      <c r="W39" s="30"/>
+      <c r="X39" s="30"/>
+      <c r="Y39" s="34"/>
     </row>
     <row r="40" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B40" s="6"/>
@@ -4249,26 +4249,26 @@
         <v>9</v>
       </c>
       <c r="E40" s="6"/>
-      <c r="H40" s="27"/>
-      <c r="I40" s="30" t="s">
+      <c r="H40" s="30"/>
+      <c r="I40" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="J40" s="30"/>
-      <c r="K40" s="30"/>
-      <c r="L40" s="27"/>
-      <c r="M40" s="27"/>
-      <c r="N40" s="27"/>
-      <c r="O40" s="27"/>
-      <c r="P40" s="27"/>
-      <c r="Q40" s="27"/>
-      <c r="R40" s="27"/>
-      <c r="S40" s="27"/>
-      <c r="T40" s="27"/>
-      <c r="U40" s="27"/>
-      <c r="V40" s="27"/>
-      <c r="W40" s="27"/>
-      <c r="X40" s="27"/>
-      <c r="Y40" s="25"/>
+      <c r="J40" s="28"/>
+      <c r="K40" s="28"/>
+      <c r="L40" s="30"/>
+      <c r="M40" s="30"/>
+      <c r="N40" s="30"/>
+      <c r="O40" s="30"/>
+      <c r="P40" s="30"/>
+      <c r="Q40" s="30"/>
+      <c r="R40" s="30"/>
+      <c r="S40" s="30"/>
+      <c r="T40" s="30"/>
+      <c r="U40" s="30"/>
+      <c r="V40" s="30"/>
+      <c r="W40" s="30"/>
+      <c r="X40" s="30"/>
+      <c r="Y40" s="34"/>
     </row>
     <row r="41" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
@@ -4277,26 +4277,26 @@
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
-      <c r="H41" s="27"/>
-      <c r="I41" s="26" t="s">
+      <c r="H41" s="30"/>
+      <c r="I41" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="J41" s="26"/>
-      <c r="K41" s="26"/>
-      <c r="L41" s="27"/>
-      <c r="M41" s="27"/>
-      <c r="N41" s="27"/>
-      <c r="O41" s="27"/>
-      <c r="P41" s="27"/>
-      <c r="Q41" s="27"/>
-      <c r="R41" s="27"/>
-      <c r="S41" s="27"/>
-      <c r="T41" s="27"/>
-      <c r="U41" s="27"/>
-      <c r="V41" s="27"/>
-      <c r="W41" s="27"/>
-      <c r="X41" s="27"/>
-      <c r="Y41" s="25"/>
+      <c r="J41" s="27"/>
+      <c r="K41" s="27"/>
+      <c r="L41" s="30"/>
+      <c r="M41" s="30"/>
+      <c r="N41" s="30"/>
+      <c r="O41" s="30"/>
+      <c r="P41" s="30"/>
+      <c r="Q41" s="30"/>
+      <c r="R41" s="30"/>
+      <c r="S41" s="30"/>
+      <c r="T41" s="30"/>
+      <c r="U41" s="30"/>
+      <c r="V41" s="30"/>
+      <c r="W41" s="30"/>
+      <c r="X41" s="30"/>
+      <c r="Y41" s="34"/>
     </row>
     <row r="42" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
@@ -4305,26 +4305,26 @@
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
-      <c r="H42" s="27"/>
-      <c r="I42" s="30" t="s">
+      <c r="H42" s="30"/>
+      <c r="I42" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="J42" s="30"/>
-      <c r="K42" s="30"/>
-      <c r="L42" s="27"/>
-      <c r="M42" s="27"/>
-      <c r="N42" s="27"/>
-      <c r="O42" s="27"/>
-      <c r="P42" s="27"/>
-      <c r="Q42" s="27"/>
-      <c r="R42" s="27"/>
-      <c r="S42" s="27"/>
-      <c r="T42" s="27"/>
-      <c r="U42" s="27"/>
-      <c r="V42" s="27"/>
-      <c r="W42" s="27"/>
-      <c r="X42" s="27"/>
-      <c r="Y42" s="25"/>
+      <c r="J42" s="28"/>
+      <c r="K42" s="28"/>
+      <c r="L42" s="30"/>
+      <c r="M42" s="30"/>
+      <c r="N42" s="30"/>
+      <c r="O42" s="30"/>
+      <c r="P42" s="30"/>
+      <c r="Q42" s="30"/>
+      <c r="R42" s="30"/>
+      <c r="S42" s="30"/>
+      <c r="T42" s="30"/>
+      <c r="U42" s="30"/>
+      <c r="V42" s="30"/>
+      <c r="W42" s="30"/>
+      <c r="X42" s="30"/>
+      <c r="Y42" s="34"/>
     </row>
     <row r="43" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
@@ -4333,26 +4333,26 @@
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="30" t="s">
+      <c r="H43" s="30"/>
+      <c r="I43" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="J43" s="30"/>
-      <c r="K43" s="30"/>
-      <c r="L43" s="27"/>
-      <c r="M43" s="27"/>
-      <c r="N43" s="27"/>
-      <c r="O43" s="27"/>
-      <c r="P43" s="27"/>
-      <c r="Q43" s="27"/>
-      <c r="R43" s="27"/>
-      <c r="S43" s="27"/>
-      <c r="T43" s="27"/>
-      <c r="U43" s="27"/>
-      <c r="V43" s="27"/>
-      <c r="W43" s="27"/>
-      <c r="X43" s="27"/>
-      <c r="Y43" s="25"/>
+      <c r="J43" s="28"/>
+      <c r="K43" s="28"/>
+      <c r="L43" s="30"/>
+      <c r="M43" s="30"/>
+      <c r="N43" s="30"/>
+      <c r="O43" s="30"/>
+      <c r="P43" s="30"/>
+      <c r="Q43" s="30"/>
+      <c r="R43" s="30"/>
+      <c r="S43" s="30"/>
+      <c r="T43" s="30"/>
+      <c r="U43" s="30"/>
+      <c r="V43" s="30"/>
+      <c r="W43" s="30"/>
+      <c r="X43" s="30"/>
+      <c r="Y43" s="34"/>
     </row>
     <row r="44" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B44" s="6"/>
@@ -4361,26 +4361,26 @@
         <v>9</v>
       </c>
       <c r="E44" s="6"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="30" t="s">
+      <c r="H44" s="30"/>
+      <c r="I44" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="J44" s="30"/>
-      <c r="K44" s="30"/>
-      <c r="L44" s="27"/>
-      <c r="M44" s="27"/>
-      <c r="N44" s="27"/>
-      <c r="O44" s="27"/>
-      <c r="P44" s="27"/>
-      <c r="Q44" s="27"/>
-      <c r="R44" s="27"/>
-      <c r="S44" s="27"/>
-      <c r="T44" s="27"/>
-      <c r="U44" s="27"/>
-      <c r="V44" s="27"/>
-      <c r="W44" s="27"/>
-      <c r="X44" s="27"/>
-      <c r="Y44" s="25"/>
+      <c r="J44" s="28"/>
+      <c r="K44" s="28"/>
+      <c r="L44" s="30"/>
+      <c r="M44" s="30"/>
+      <c r="N44" s="30"/>
+      <c r="O44" s="30"/>
+      <c r="P44" s="30"/>
+      <c r="Q44" s="30"/>
+      <c r="R44" s="30"/>
+      <c r="S44" s="30"/>
+      <c r="T44" s="30"/>
+      <c r="U44" s="30"/>
+      <c r="V44" s="30"/>
+      <c r="W44" s="30"/>
+      <c r="X44" s="30"/>
+      <c r="Y44" s="34"/>
     </row>
     <row r="45" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B45" s="6"/>
@@ -4389,26 +4389,26 @@
       <c r="E45" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H45" s="27"/>
-      <c r="I45" s="30" t="s">
+      <c r="H45" s="30"/>
+      <c r="I45" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="J45" s="30"/>
-      <c r="K45" s="30"/>
-      <c r="L45" s="27"/>
-      <c r="M45" s="27"/>
-      <c r="N45" s="27"/>
-      <c r="O45" s="27"/>
-      <c r="P45" s="27"/>
-      <c r="Q45" s="27"/>
-      <c r="R45" s="27"/>
-      <c r="S45" s="27"/>
-      <c r="T45" s="27"/>
-      <c r="U45" s="27"/>
-      <c r="V45" s="27"/>
-      <c r="W45" s="27"/>
-      <c r="X45" s="27"/>
-      <c r="Y45" s="25"/>
+      <c r="J45" s="28"/>
+      <c r="K45" s="28"/>
+      <c r="L45" s="30"/>
+      <c r="M45" s="30"/>
+      <c r="N45" s="30"/>
+      <c r="O45" s="30"/>
+      <c r="P45" s="30"/>
+      <c r="Q45" s="30"/>
+      <c r="R45" s="30"/>
+      <c r="S45" s="30"/>
+      <c r="T45" s="30"/>
+      <c r="U45" s="30"/>
+      <c r="V45" s="30"/>
+      <c r="W45" s="30"/>
+      <c r="X45" s="30"/>
+      <c r="Y45" s="34"/>
     </row>
     <row r="46" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B46" s="6" t="s">
@@ -4417,29 +4417,57 @@
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
-      <c r="H46" s="27"/>
-      <c r="I46" s="26" t="s">
+      <c r="H46" s="30"/>
+      <c r="I46" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="J46" s="26"/>
-      <c r="K46" s="26"/>
-      <c r="L46" s="27"/>
-      <c r="M46" s="27"/>
-      <c r="N46" s="27"/>
-      <c r="O46" s="27"/>
-      <c r="P46" s="27"/>
-      <c r="Q46" s="27"/>
-      <c r="R46" s="27"/>
-      <c r="S46" s="27"/>
-      <c r="T46" s="27"/>
-      <c r="U46" s="27"/>
-      <c r="V46" s="27"/>
-      <c r="W46" s="27"/>
-      <c r="X46" s="27"/>
-      <c r="Y46" s="25"/>
+      <c r="J46" s="27"/>
+      <c r="K46" s="27"/>
+      <c r="L46" s="30"/>
+      <c r="M46" s="30"/>
+      <c r="N46" s="30"/>
+      <c r="O46" s="30"/>
+      <c r="P46" s="30"/>
+      <c r="Q46" s="30"/>
+      <c r="R46" s="30"/>
+      <c r="S46" s="30"/>
+      <c r="T46" s="30"/>
+      <c r="U46" s="30"/>
+      <c r="V46" s="30"/>
+      <c r="W46" s="30"/>
+      <c r="X46" s="30"/>
+      <c r="Y46" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="H10:H46"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="J30:K30"/>
     <mergeCell ref="I34:K34"/>
     <mergeCell ref="Y10:Y46"/>
     <mergeCell ref="L10:X46"/>
@@ -4456,34 +4484,6 @@
     <mergeCell ref="I36:K36"/>
     <mergeCell ref="I37:K37"/>
     <mergeCell ref="I31:K31"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="H10:H46"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I17:J17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4527,28 +4527,28 @@
       <c r="H2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
       <c r="L2" s="9" t="s">
         <v>59</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="N2" s="28" t="s">
+      <c r="N2" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28" t="s">
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
       <c r="U2" s="9" t="s">
         <v>63</v>
       </c>
@@ -4638,11 +4638,11 @@
       <c r="H9" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="I9" s="26" t="s">
+      <c r="I9" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
       <c r="L9" s="9" t="s">
         <v>93</v>
       </c>
@@ -4690,30 +4690,30 @@
       <c r="B10" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="H10" s="27" t="s">
+      <c r="H10" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="I10" s="26" t="s">
+      <c r="I10" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="27" t="s">
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="M10" s="27"/>
-      <c r="N10" s="27"/>
-      <c r="O10" s="27"/>
-      <c r="P10" s="27"/>
-      <c r="Q10" s="27"/>
-      <c r="R10" s="27"/>
-      <c r="S10" s="27"/>
-      <c r="T10" s="27"/>
-      <c r="U10" s="27"/>
-      <c r="V10" s="27"/>
-      <c r="W10" s="27"/>
-      <c r="X10" s="27"/>
-      <c r="Y10" s="25" t="s">
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="30"/>
+      <c r="R10" s="30"/>
+      <c r="S10" s="30"/>
+      <c r="T10" s="30"/>
+      <c r="U10" s="30"/>
+      <c r="V10" s="30"/>
+      <c r="W10" s="30"/>
+      <c r="X10" s="30"/>
+      <c r="Y10" s="34" t="s">
         <v>125</v>
       </c>
     </row>
@@ -4721,76 +4721,76 @@
       <c r="B11" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="H11" s="27"/>
-      <c r="I11" s="30" t="s">
+      <c r="H11" s="30"/>
+      <c r="I11" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27"/>
-      <c r="N11" s="27"/>
-      <c r="O11" s="27"/>
-      <c r="P11" s="27"/>
-      <c r="Q11" s="27"/>
-      <c r="R11" s="27"/>
-      <c r="S11" s="27"/>
-      <c r="T11" s="27"/>
-      <c r="U11" s="27"/>
-      <c r="V11" s="27"/>
-      <c r="W11" s="27"/>
-      <c r="X11" s="27"/>
-      <c r="Y11" s="25"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="30"/>
+      <c r="R11" s="30"/>
+      <c r="S11" s="30"/>
+      <c r="T11" s="30"/>
+      <c r="U11" s="30"/>
+      <c r="V11" s="30"/>
+      <c r="W11" s="30"/>
+      <c r="X11" s="30"/>
+      <c r="Y11" s="34"/>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="H12" s="27"/>
-      <c r="I12" s="30" t="s">
+      <c r="H12" s="30"/>
+      <c r="I12" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="27"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="27"/>
-      <c r="P12" s="27"/>
-      <c r="Q12" s="27"/>
-      <c r="R12" s="27"/>
-      <c r="S12" s="27"/>
-      <c r="T12" s="27"/>
-      <c r="U12" s="27"/>
-      <c r="V12" s="27"/>
-      <c r="W12" s="27"/>
-      <c r="X12" s="27"/>
-      <c r="Y12" s="25"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="30"/>
+      <c r="R12" s="30"/>
+      <c r="S12" s="30"/>
+      <c r="T12" s="30"/>
+      <c r="U12" s="30"/>
+      <c r="V12" s="30"/>
+      <c r="W12" s="30"/>
+      <c r="X12" s="30"/>
+      <c r="Y12" s="34"/>
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="H13" s="27"/>
-      <c r="I13" s="30" t="s">
+      <c r="H13" s="30"/>
+      <c r="I13" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="27"/>
-      <c r="R13" s="27"/>
-      <c r="S13" s="27"/>
-      <c r="T13" s="27"/>
-      <c r="U13" s="27"/>
-      <c r="V13" s="27"/>
-      <c r="W13" s="27"/>
-      <c r="X13" s="27"/>
-      <c r="Y13" s="25"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="30"/>
+      <c r="R13" s="30"/>
+      <c r="S13" s="30"/>
+      <c r="T13" s="30"/>
+      <c r="U13" s="30"/>
+      <c r="V13" s="30"/>
+      <c r="W13" s="30"/>
+      <c r="X13" s="30"/>
+      <c r="Y13" s="34"/>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
@@ -4799,219 +4799,212 @@
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="30" t="s">
+      <c r="H14" s="30"/>
+      <c r="I14" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="27"/>
-      <c r="N14" s="27"/>
-      <c r="O14" s="27"/>
-      <c r="P14" s="27"/>
-      <c r="Q14" s="27"/>
-      <c r="R14" s="27"/>
-      <c r="S14" s="27"/>
-      <c r="T14" s="27"/>
-      <c r="U14" s="27"/>
-      <c r="V14" s="27"/>
-      <c r="W14" s="27"/>
-      <c r="X14" s="27"/>
-      <c r="Y14" s="25"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="30"/>
+      <c r="R14" s="30"/>
+      <c r="S14" s="30"/>
+      <c r="T14" s="30"/>
+      <c r="U14" s="30"/>
+      <c r="V14" s="30"/>
+      <c r="W14" s="30"/>
+      <c r="X14" s="30"/>
+      <c r="Y14" s="34"/>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B15" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="H15" s="27"/>
-      <c r="I15" s="29" t="s">
+      <c r="H15" s="30"/>
+      <c r="I15" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="27"/>
-      <c r="N15" s="27"/>
-      <c r="O15" s="27"/>
-      <c r="P15" s="27"/>
-      <c r="Q15" s="27"/>
-      <c r="R15" s="27"/>
-      <c r="S15" s="27"/>
-      <c r="T15" s="27"/>
-      <c r="U15" s="27"/>
-      <c r="V15" s="27"/>
-      <c r="W15" s="27"/>
-      <c r="X15" s="27"/>
-      <c r="Y15" s="25"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="30"/>
+      <c r="R15" s="30"/>
+      <c r="S15" s="30"/>
+      <c r="T15" s="30"/>
+      <c r="U15" s="30"/>
+      <c r="V15" s="30"/>
+      <c r="W15" s="30"/>
+      <c r="X15" s="30"/>
+      <c r="Y15" s="34"/>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B16" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="H16" s="27"/>
-      <c r="I16" s="29" t="s">
+      <c r="H16" s="30"/>
+      <c r="I16" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="27"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="27"/>
-      <c r="P16" s="27"/>
-      <c r="Q16" s="27"/>
-      <c r="R16" s="27"/>
-      <c r="S16" s="27"/>
-      <c r="T16" s="27"/>
-      <c r="U16" s="27"/>
-      <c r="V16" s="27"/>
-      <c r="W16" s="27"/>
-      <c r="X16" s="27"/>
-      <c r="Y16" s="25"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="30"/>
+      <c r="R16" s="30"/>
+      <c r="S16" s="30"/>
+      <c r="T16" s="30"/>
+      <c r="U16" s="30"/>
+      <c r="V16" s="30"/>
+      <c r="W16" s="30"/>
+      <c r="X16" s="30"/>
+      <c r="Y16" s="34"/>
     </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B17" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="H17" s="27"/>
-      <c r="I17" s="29" t="s">
+      <c r="H17" s="30"/>
+      <c r="I17" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="J17" s="29"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="27"/>
-      <c r="O17" s="27"/>
-      <c r="P17" s="27"/>
-      <c r="Q17" s="27"/>
-      <c r="R17" s="27"/>
-      <c r="S17" s="27"/>
-      <c r="T17" s="27"/>
-      <c r="U17" s="27"/>
-      <c r="V17" s="27"/>
-      <c r="W17" s="27"/>
-      <c r="X17" s="27"/>
-      <c r="Y17" s="25"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="30"/>
+      <c r="P17" s="30"/>
+      <c r="Q17" s="30"/>
+      <c r="R17" s="30"/>
+      <c r="S17" s="30"/>
+      <c r="T17" s="30"/>
+      <c r="U17" s="30"/>
+      <c r="V17" s="30"/>
+      <c r="W17" s="30"/>
+      <c r="X17" s="30"/>
+      <c r="Y17" s="34"/>
     </row>
     <row r="18" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>4</v>
       </c>
-      <c r="H18" s="27"/>
-      <c r="I18" s="30" t="s">
+      <c r="H18" s="30"/>
+      <c r="I18" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="J18" s="26"/>
+      <c r="J18" s="27"/>
       <c r="K18" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="L18" s="27"/>
-      <c r="M18" s="27"/>
-      <c r="N18" s="27"/>
-      <c r="O18" s="27"/>
-      <c r="P18" s="27"/>
-      <c r="Q18" s="27"/>
-      <c r="R18" s="27"/>
-      <c r="S18" s="27"/>
-      <c r="T18" s="27"/>
-      <c r="U18" s="27"/>
-      <c r="V18" s="27"/>
-      <c r="W18" s="27"/>
-      <c r="X18" s="27"/>
-      <c r="Y18" s="25"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="30"/>
+      <c r="P18" s="30"/>
+      <c r="Q18" s="30"/>
+      <c r="R18" s="30"/>
+      <c r="S18" s="30"/>
+      <c r="T18" s="30"/>
+      <c r="U18" s="30"/>
+      <c r="V18" s="30"/>
+      <c r="W18" s="30"/>
+      <c r="X18" s="30"/>
+      <c r="Y18" s="34"/>
     </row>
     <row r="19" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>6</v>
       </c>
-      <c r="H19" s="27"/>
-      <c r="I19" s="28" t="s">
+      <c r="H19" s="30"/>
+      <c r="I19" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="J19" s="28"/>
+      <c r="J19" s="32"/>
       <c r="K19" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="L19" s="27"/>
-      <c r="M19" s="27"/>
-      <c r="N19" s="27"/>
-      <c r="O19" s="27"/>
-      <c r="P19" s="27"/>
-      <c r="Q19" s="27"/>
-      <c r="R19" s="27"/>
-      <c r="S19" s="27"/>
-      <c r="T19" s="27"/>
-      <c r="U19" s="27"/>
-      <c r="V19" s="27"/>
-      <c r="W19" s="27"/>
-      <c r="X19" s="27"/>
-      <c r="Y19" s="25"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="30"/>
+      <c r="P19" s="30"/>
+      <c r="Q19" s="30"/>
+      <c r="R19" s="30"/>
+      <c r="S19" s="30"/>
+      <c r="T19" s="30"/>
+      <c r="U19" s="30"/>
+      <c r="V19" s="30"/>
+      <c r="W19" s="30"/>
+      <c r="X19" s="30"/>
+      <c r="Y19" s="34"/>
     </row>
     <row r="20" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="27"/>
+      <c r="H20" s="30"/>
       <c r="I20" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="J20" s="28" t="s">
+      <c r="J20" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="K20" s="28"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="27"/>
-      <c r="N20" s="27"/>
-      <c r="O20" s="27"/>
-      <c r="P20" s="27"/>
-      <c r="Q20" s="27"/>
-      <c r="R20" s="27"/>
-      <c r="S20" s="27"/>
-      <c r="T20" s="27"/>
-      <c r="U20" s="27"/>
-      <c r="V20" s="27"/>
-      <c r="W20" s="27"/>
-      <c r="X20" s="27"/>
-      <c r="Y20" s="25"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="30"/>
+      <c r="P20" s="30"/>
+      <c r="Q20" s="30"/>
+      <c r="R20" s="30"/>
+      <c r="S20" s="30"/>
+      <c r="T20" s="30"/>
+      <c r="U20" s="30"/>
+      <c r="V20" s="30"/>
+      <c r="W20" s="30"/>
+      <c r="X20" s="30"/>
+      <c r="Y20" s="34"/>
     </row>
     <row r="21" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>13</v>
       </c>
-      <c r="H21" s="27"/>
+      <c r="H21" s="30"/>
       <c r="I21" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="J21" s="32" t="s">
+      <c r="J21" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="K21" s="32"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="27"/>
-      <c r="N21" s="27"/>
-      <c r="O21" s="27"/>
-      <c r="P21" s="27"/>
-      <c r="Q21" s="27"/>
-      <c r="R21" s="27"/>
-      <c r="S21" s="27"/>
-      <c r="T21" s="27"/>
-      <c r="U21" s="27"/>
-      <c r="V21" s="27"/>
-      <c r="W21" s="27"/>
-      <c r="X21" s="27"/>
-      <c r="Y21" s="25"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="30"/>
+      <c r="P21" s="30"/>
+      <c r="Q21" s="30"/>
+      <c r="R21" s="30"/>
+      <c r="S21" s="30"/>
+      <c r="T21" s="30"/>
+      <c r="U21" s="30"/>
+      <c r="V21" s="30"/>
+      <c r="W21" s="30"/>
+      <c r="X21" s="30"/>
+      <c r="Y21" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="Y10:Y21"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I19:J19"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:T2"/>
@@ -5024,6 +5017,13 @@
     <mergeCell ref="I12:K12"/>
     <mergeCell ref="I13:K13"/>
     <mergeCell ref="J21:K21"/>
+    <mergeCell ref="Y10:Y21"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I19:J19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5151,8 +5151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B8:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15:O16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5173,31 +5173,31 @@
   </cols>
   <sheetData>
     <row r="8" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="F8" s="33" t="s">
+      <c r="F8" s="35" t="s">
         <v>191</v>
       </c>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="33" t="s">
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="35" t="s">
         <v>192</v>
       </c>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="33"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="35"/>
-      <c r="Q8" s="34" t="s">
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="35"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="24" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="K9" s="28" t="s">
+      <c r="K9" s="32" t="s">
         <v>193</v>
       </c>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
       <c r="N9" s="22"/>
       <c r="O9" t="s">
         <v>194</v>
@@ -5271,12 +5271,12 @@
         <v>56</v>
       </c>
       <c r="J15" s="23"/>
-      <c r="K15" s="26" t="s">
+      <c r="K15" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="O15" s="27" t="s">
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+      <c r="O15" s="30" t="s">
         <v>125</v>
       </c>
       <c r="Q15" s="11" t="s">
@@ -5310,7 +5310,7 @@
         <v>201</v>
       </c>
       <c r="N16" s="21"/>
-      <c r="O16" s="27"/>
+      <c r="O16" s="30"/>
       <c r="Q16" s="21" t="s">
         <v>125</v>
       </c>
@@ -5336,7 +5336,7 @@
   <dimension ref="C3:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed bug in data model of UTF-16 (luckily it is not in the code).
</commit_message>
<xml_diff>
--- a/doc/unicode.xlsx
+++ b/doc/unicode.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="203">
   <si>
     <t>S</t>
   </si>
@@ -1122,9 +1122,6 @@
     <t>E0-FF</t>
   </si>
   <si>
-    <t>00-D8</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">error(1), </t>
     </r>
@@ -1157,6 +1154,12 @@
       </rPr>
       <t>terminate</t>
     </r>
+  </si>
+  <si>
+    <t>00-D7</t>
+  </si>
+  <si>
+    <t>D8-DB</t>
   </si>
 </sst>
 </file>
@@ -1233,7 +1236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1300,17 +1303,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1318,8 +1322,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1638,10 +1648,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="C1" s="26"/>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
@@ -1826,28 +1836,28 @@
       <c r="I2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
       <c r="M2" s="8" t="s">
         <v>59</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="O2" s="32" t="s">
+      <c r="O2" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32" t="s">
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
       <c r="V2" s="8" t="s">
         <v>63</v>
       </c>
@@ -1937,11 +1947,11 @@
       <c r="I9" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J9" s="27" t="s">
+      <c r="J9" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
       <c r="M9" s="8" t="s">
         <v>119</v>
       </c>
@@ -1989,30 +1999,30 @@
       <c r="B10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I10" s="30" t="s">
+      <c r="I10" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="J10" s="27" t="s">
+      <c r="J10" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="30" t="s">
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="N10" s="30"/>
-      <c r="O10" s="30"/>
-      <c r="P10" s="30"/>
-      <c r="Q10" s="30"/>
-      <c r="R10" s="30"/>
-      <c r="S10" s="30"/>
-      <c r="T10" s="30"/>
-      <c r="U10" s="30"/>
-      <c r="V10" s="30"/>
-      <c r="W10" s="30"/>
-      <c r="X10" s="30"/>
-      <c r="Y10" s="30"/>
-      <c r="Z10" s="34" t="s">
+      <c r="N10" s="32"/>
+      <c r="O10" s="32"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="32"/>
+      <c r="R10" s="32"/>
+      <c r="S10" s="32"/>
+      <c r="T10" s="32"/>
+      <c r="U10" s="32"/>
+      <c r="V10" s="32"/>
+      <c r="W10" s="32"/>
+      <c r="X10" s="32"/>
+      <c r="Y10" s="32"/>
+      <c r="Z10" s="30" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2020,81 +2030,81 @@
       <c r="B11" t="s">
         <v>3</v>
       </c>
-      <c r="I11" s="30"/>
-      <c r="J11" s="33" t="s">
+      <c r="I11" s="32"/>
+      <c r="J11" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="30"/>
-      <c r="O11" s="30"/>
-      <c r="P11" s="30"/>
-      <c r="Q11" s="30"/>
-      <c r="R11" s="30"/>
-      <c r="S11" s="30"/>
-      <c r="T11" s="30"/>
-      <c r="U11" s="30"/>
-      <c r="V11" s="30"/>
-      <c r="W11" s="30"/>
-      <c r="X11" s="30"/>
-      <c r="Y11" s="30"/>
-      <c r="Z11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="32"/>
+      <c r="Q11" s="32"/>
+      <c r="R11" s="32"/>
+      <c r="S11" s="32"/>
+      <c r="T11" s="32"/>
+      <c r="U11" s="32"/>
+      <c r="V11" s="32"/>
+      <c r="W11" s="32"/>
+      <c r="X11" s="32"/>
+      <c r="Y11" s="32"/>
+      <c r="Z11" s="30"/>
     </row>
     <row r="12" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>4</v>
       </c>
-      <c r="I12" s="30"/>
-      <c r="J12" s="27" t="s">
+      <c r="I12" s="32"/>
+      <c r="J12" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="K12" s="27"/>
+      <c r="K12" s="31"/>
       <c r="L12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="30"/>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="30"/>
-      <c r="R12" s="30"/>
-      <c r="S12" s="30"/>
-      <c r="T12" s="30"/>
-      <c r="U12" s="30"/>
-      <c r="V12" s="30"/>
-      <c r="W12" s="30"/>
-      <c r="X12" s="30"/>
-      <c r="Y12" s="30"/>
-      <c r="Z12" s="34"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="32"/>
+      <c r="O12" s="32"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="32"/>
+      <c r="R12" s="32"/>
+      <c r="S12" s="32"/>
+      <c r="T12" s="32"/>
+      <c r="U12" s="32"/>
+      <c r="V12" s="32"/>
+      <c r="W12" s="32"/>
+      <c r="X12" s="32"/>
+      <c r="Y12" s="32"/>
+      <c r="Z12" s="30"/>
     </row>
     <row r="13" spans="2:26" x14ac:dyDescent="0.25">
       <c r="C13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="30" t="s">
+      <c r="I13" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="J13" s="27" t="s">
+      <c r="J13" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="30" t="s">
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="N13" s="30"/>
-      <c r="O13" s="30"/>
-      <c r="P13" s="30"/>
-      <c r="Q13" s="30"/>
-      <c r="R13" s="30"/>
-      <c r="S13" s="30"/>
-      <c r="T13" s="30"/>
-      <c r="U13" s="30"/>
-      <c r="V13" s="30"/>
-      <c r="W13" s="30"/>
-      <c r="X13" s="30"/>
-      <c r="Y13" s="30"/>
+      <c r="N13" s="32"/>
+      <c r="O13" s="32"/>
+      <c r="P13" s="32"/>
+      <c r="Q13" s="32"/>
+      <c r="R13" s="32"/>
+      <c r="S13" s="32"/>
+      <c r="T13" s="32"/>
+      <c r="U13" s="32"/>
+      <c r="V13" s="32"/>
+      <c r="W13" s="32"/>
+      <c r="X13" s="32"/>
+      <c r="Y13" s="32"/>
       <c r="Z13" s="12" t="s">
         <v>127</v>
       </c>
@@ -2103,27 +2113,27 @@
       <c r="C14" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="30"/>
-      <c r="J14" s="33" t="s">
+      <c r="I14" s="32"/>
+      <c r="J14" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="K14" s="33"/>
-      <c r="L14" s="33"/>
-      <c r="M14" s="30" t="s">
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="N14" s="30"/>
-      <c r="O14" s="30"/>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="30"/>
-      <c r="R14" s="30"/>
-      <c r="S14" s="30"/>
-      <c r="T14" s="30"/>
-      <c r="U14" s="30"/>
-      <c r="V14" s="30"/>
-      <c r="W14" s="30"/>
-      <c r="X14" s="30"/>
-      <c r="Y14" s="30"/>
+      <c r="N14" s="32"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="32"/>
+      <c r="R14" s="32"/>
+      <c r="S14" s="32"/>
+      <c r="T14" s="32"/>
+      <c r="U14" s="32"/>
+      <c r="V14" s="32"/>
+      <c r="W14" s="32"/>
+      <c r="X14" s="32"/>
+      <c r="Y14" s="32"/>
       <c r="Z14" s="12" t="s">
         <v>127</v>
       </c>
@@ -2135,26 +2145,26 @@
       <c r="I15" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J15" s="32" t="s">
+      <c r="J15" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="27" t="s">
+      <c r="K15" s="33"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="N15" s="27"/>
-      <c r="O15" s="27"/>
-      <c r="P15" s="27"/>
-      <c r="Q15" s="27"/>
-      <c r="R15" s="27"/>
-      <c r="S15" s="27"/>
-      <c r="T15" s="27"/>
-      <c r="U15" s="27"/>
-      <c r="V15" s="27"/>
-      <c r="W15" s="27"/>
-      <c r="X15" s="27"/>
-      <c r="Y15" s="27"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="31"/>
+      <c r="Q15" s="31"/>
+      <c r="R15" s="31"/>
+      <c r="S15" s="31"/>
+      <c r="T15" s="31"/>
+      <c r="U15" s="31"/>
+      <c r="V15" s="31"/>
+      <c r="W15" s="31"/>
+      <c r="X15" s="31"/>
+      <c r="Y15" s="31"/>
       <c r="Z15" s="14" t="s">
         <v>126</v>
       </c>
@@ -2166,26 +2176,26 @@
       <c r="I16" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J16" s="33" t="s">
+      <c r="J16" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="K16" s="33"/>
-      <c r="L16" s="33"/>
-      <c r="M16" s="30" t="s">
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="N16" s="30"/>
-      <c r="O16" s="30"/>
-      <c r="P16" s="30"/>
-      <c r="Q16" s="30"/>
-      <c r="R16" s="30"/>
-      <c r="S16" s="30"/>
-      <c r="T16" s="30"/>
-      <c r="U16" s="30"/>
-      <c r="V16" s="30"/>
-      <c r="W16" s="30"/>
-      <c r="X16" s="30"/>
-      <c r="Y16" s="30"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="32"/>
+      <c r="Q16" s="32"/>
+      <c r="R16" s="32"/>
+      <c r="S16" s="32"/>
+      <c r="T16" s="32"/>
+      <c r="U16" s="32"/>
+      <c r="V16" s="32"/>
+      <c r="W16" s="32"/>
+      <c r="X16" s="32"/>
+      <c r="Y16" s="32"/>
       <c r="Z16" s="12" t="s">
         <v>127</v>
       </c>
@@ -2197,28 +2207,28 @@
       <c r="I17" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J17" s="32" t="s">
+      <c r="J17" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="K17" s="32"/>
+      <c r="K17" s="33"/>
       <c r="L17" t="s">
         <v>55</v>
       </c>
-      <c r="M17" s="27" t="s">
+      <c r="M17" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="N17" s="27"/>
-      <c r="O17" s="27"/>
-      <c r="P17" s="27"/>
-      <c r="Q17" s="27"/>
-      <c r="R17" s="27"/>
-      <c r="S17" s="27"/>
-      <c r="T17" s="27"/>
-      <c r="U17" s="27"/>
-      <c r="V17" s="27"/>
-      <c r="W17" s="27"/>
-      <c r="X17" s="27"/>
-      <c r="Y17" s="27"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="31"/>
+      <c r="P17" s="31"/>
+      <c r="Q17" s="31"/>
+      <c r="R17" s="31"/>
+      <c r="S17" s="31"/>
+      <c r="T17" s="31"/>
+      <c r="U17" s="31"/>
+      <c r="V17" s="31"/>
+      <c r="W17" s="31"/>
+      <c r="X17" s="31"/>
+      <c r="Y17" s="31"/>
       <c r="Z17" s="14" t="s">
         <v>126</v>
       </c>
@@ -2230,26 +2240,26 @@
       <c r="I18" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J18" s="33" t="s">
+      <c r="J18" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="K18" s="33"/>
-      <c r="L18" s="33"/>
-      <c r="M18" s="30" t="s">
+      <c r="K18" s="34"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="N18" s="30"/>
-      <c r="O18" s="30"/>
-      <c r="P18" s="30"/>
-      <c r="Q18" s="30"/>
-      <c r="R18" s="30"/>
-      <c r="S18" s="30"/>
-      <c r="T18" s="30"/>
-      <c r="U18" s="30"/>
-      <c r="V18" s="30"/>
-      <c r="W18" s="30"/>
-      <c r="X18" s="30"/>
-      <c r="Y18" s="30"/>
+      <c r="N18" s="32"/>
+      <c r="O18" s="32"/>
+      <c r="P18" s="32"/>
+      <c r="Q18" s="32"/>
+      <c r="R18" s="32"/>
+      <c r="S18" s="32"/>
+      <c r="T18" s="32"/>
+      <c r="U18" s="32"/>
+      <c r="V18" s="32"/>
+      <c r="W18" s="32"/>
+      <c r="X18" s="32"/>
+      <c r="Y18" s="32"/>
       <c r="Z18" s="12" t="s">
         <v>127</v>
       </c>
@@ -2261,26 +2271,26 @@
       <c r="I19" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J19" s="31" t="s">
+      <c r="J19" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="K19" s="31"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="30" t="s">
+      <c r="K19" s="36"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="N19" s="30"/>
-      <c r="O19" s="30"/>
-      <c r="P19" s="30"/>
-      <c r="Q19" s="30"/>
-      <c r="R19" s="30"/>
-      <c r="S19" s="30"/>
-      <c r="T19" s="30"/>
-      <c r="U19" s="30"/>
-      <c r="V19" s="30"/>
-      <c r="W19" s="30"/>
-      <c r="X19" s="30"/>
-      <c r="Y19" s="30"/>
+      <c r="N19" s="32"/>
+      <c r="O19" s="32"/>
+      <c r="P19" s="32"/>
+      <c r="Q19" s="32"/>
+      <c r="R19" s="32"/>
+      <c r="S19" s="32"/>
+      <c r="T19" s="32"/>
+      <c r="U19" s="32"/>
+      <c r="V19" s="32"/>
+      <c r="W19" s="32"/>
+      <c r="X19" s="32"/>
+      <c r="Y19" s="32"/>
       <c r="Z19" s="12" t="s">
         <v>127</v>
       </c>
@@ -2292,26 +2302,26 @@
       <c r="I20" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J20" s="32" t="s">
+      <c r="J20" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="27" t="s">
+      <c r="K20" s="33"/>
+      <c r="L20" s="33"/>
+      <c r="M20" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="N20" s="27"/>
-      <c r="O20" s="27"/>
-      <c r="P20" s="27"/>
-      <c r="Q20" s="27"/>
-      <c r="R20" s="27"/>
-      <c r="S20" s="27"/>
-      <c r="T20" s="27"/>
-      <c r="U20" s="27"/>
-      <c r="V20" s="27"/>
-      <c r="W20" s="27"/>
-      <c r="X20" s="27"/>
-      <c r="Y20" s="27"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="31"/>
+      <c r="P20" s="31"/>
+      <c r="Q20" s="31"/>
+      <c r="R20" s="31"/>
+      <c r="S20" s="31"/>
+      <c r="T20" s="31"/>
+      <c r="U20" s="31"/>
+      <c r="V20" s="31"/>
+      <c r="W20" s="31"/>
+      <c r="X20" s="31"/>
+      <c r="Y20" s="31"/>
       <c r="Z20" s="14" t="s">
         <v>126</v>
       </c>
@@ -2323,26 +2333,26 @@
       <c r="I21" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J21" s="33" t="s">
+      <c r="J21" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="30" t="s">
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="N21" s="30"/>
-      <c r="O21" s="30"/>
-      <c r="P21" s="30"/>
-      <c r="Q21" s="30"/>
-      <c r="R21" s="30"/>
-      <c r="S21" s="30"/>
-      <c r="T21" s="30"/>
-      <c r="U21" s="30"/>
-      <c r="V21" s="30"/>
-      <c r="W21" s="30"/>
-      <c r="X21" s="30"/>
-      <c r="Y21" s="30"/>
+      <c r="N21" s="32"/>
+      <c r="O21" s="32"/>
+      <c r="P21" s="32"/>
+      <c r="Q21" s="32"/>
+      <c r="R21" s="32"/>
+      <c r="S21" s="32"/>
+      <c r="T21" s="32"/>
+      <c r="U21" s="32"/>
+      <c r="V21" s="32"/>
+      <c r="W21" s="32"/>
+      <c r="X21" s="32"/>
+      <c r="Y21" s="32"/>
       <c r="Z21" s="12" t="s">
         <v>127</v>
       </c>
@@ -2357,25 +2367,25 @@
       <c r="J22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K22" s="32" t="s">
+      <c r="K22" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="L22" s="32"/>
-      <c r="M22" s="27" t="s">
+      <c r="L22" s="33"/>
+      <c r="M22" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="N22" s="27"/>
-      <c r="O22" s="27"/>
-      <c r="P22" s="27"/>
-      <c r="Q22" s="27"/>
-      <c r="R22" s="27"/>
-      <c r="S22" s="27"/>
-      <c r="T22" s="27"/>
-      <c r="U22" s="27"/>
-      <c r="V22" s="27"/>
-      <c r="W22" s="27"/>
-      <c r="X22" s="27"/>
-      <c r="Y22" s="27"/>
+      <c r="N22" s="31"/>
+      <c r="O22" s="31"/>
+      <c r="P22" s="31"/>
+      <c r="Q22" s="31"/>
+      <c r="R22" s="31"/>
+      <c r="S22" s="31"/>
+      <c r="T22" s="31"/>
+      <c r="U22" s="31"/>
+      <c r="V22" s="31"/>
+      <c r="W22" s="31"/>
+      <c r="X22" s="31"/>
+      <c r="Y22" s="31"/>
       <c r="Z22" s="14" t="s">
         <v>126</v>
       </c>
@@ -2387,26 +2397,26 @@
       <c r="I23" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J23" s="28" t="s">
+      <c r="J23" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="K23" s="28"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="30" t="s">
+      <c r="K23" s="35"/>
+      <c r="L23" s="35"/>
+      <c r="M23" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="N23" s="30"/>
-      <c r="O23" s="30"/>
-      <c r="P23" s="30"/>
-      <c r="Q23" s="30"/>
-      <c r="R23" s="30"/>
-      <c r="S23" s="30"/>
-      <c r="T23" s="30"/>
-      <c r="U23" s="30"/>
-      <c r="V23" s="30"/>
-      <c r="W23" s="30"/>
-      <c r="X23" s="30"/>
-      <c r="Y23" s="30"/>
+      <c r="N23" s="32"/>
+      <c r="O23" s="32"/>
+      <c r="P23" s="32"/>
+      <c r="Q23" s="32"/>
+      <c r="R23" s="32"/>
+      <c r="S23" s="32"/>
+      <c r="T23" s="32"/>
+      <c r="U23" s="32"/>
+      <c r="V23" s="32"/>
+      <c r="W23" s="32"/>
+      <c r="X23" s="32"/>
+      <c r="Y23" s="32"/>
       <c r="Z23" s="12" t="s">
         <v>127</v>
       </c>
@@ -2419,26 +2429,26 @@
       <c r="I24" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="J24" s="27" t="s">
+      <c r="J24" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27" t="s">
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="N24" s="27"/>
-      <c r="O24" s="27"/>
-      <c r="P24" s="27"/>
-      <c r="Q24" s="27"/>
-      <c r="R24" s="27"/>
-      <c r="S24" s="27"/>
-      <c r="T24" s="27"/>
-      <c r="U24" s="27"/>
-      <c r="V24" s="27"/>
-      <c r="W24" s="27"/>
-      <c r="X24" s="27"/>
-      <c r="Y24" s="27"/>
+      <c r="N24" s="31"/>
+      <c r="O24" s="31"/>
+      <c r="P24" s="31"/>
+      <c r="Q24" s="31"/>
+      <c r="R24" s="31"/>
+      <c r="S24" s="31"/>
+      <c r="T24" s="31"/>
+      <c r="U24" s="31"/>
+      <c r="V24" s="31"/>
+      <c r="W24" s="31"/>
+      <c r="X24" s="31"/>
+      <c r="Y24" s="31"/>
       <c r="Z24" s="10" t="s">
         <v>130</v>
       </c>
@@ -2450,26 +2460,26 @@
       <c r="I25" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J25" s="32" t="s">
+      <c r="J25" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="K25" s="32"/>
-      <c r="L25" s="32"/>
-      <c r="M25" s="30" t="s">
+      <c r="K25" s="33"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="N25" s="30"/>
-      <c r="O25" s="30"/>
-      <c r="P25" s="30"/>
-      <c r="Q25" s="30"/>
-      <c r="R25" s="30"/>
-      <c r="S25" s="30"/>
-      <c r="T25" s="30"/>
-      <c r="U25" s="30"/>
-      <c r="V25" s="30"/>
-      <c r="W25" s="30"/>
-      <c r="X25" s="30"/>
-      <c r="Y25" s="30"/>
+      <c r="N25" s="32"/>
+      <c r="O25" s="32"/>
+      <c r="P25" s="32"/>
+      <c r="Q25" s="32"/>
+      <c r="R25" s="32"/>
+      <c r="S25" s="32"/>
+      <c r="T25" s="32"/>
+      <c r="U25" s="32"/>
+      <c r="V25" s="32"/>
+      <c r="W25" s="32"/>
+      <c r="X25" s="32"/>
+      <c r="Y25" s="32"/>
       <c r="Z25" s="12" t="s">
         <v>127</v>
       </c>
@@ -2481,26 +2491,26 @@
       <c r="I26" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="J26" s="33" t="s">
+      <c r="J26" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="K26" s="33"/>
-      <c r="L26" s="33"/>
-      <c r="M26" s="27" t="s">
+      <c r="K26" s="34"/>
+      <c r="L26" s="34"/>
+      <c r="M26" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="N26" s="27"/>
-      <c r="O26" s="27"/>
-      <c r="P26" s="27"/>
-      <c r="Q26" s="27"/>
-      <c r="R26" s="27"/>
-      <c r="S26" s="27"/>
-      <c r="T26" s="27"/>
-      <c r="U26" s="27"/>
-      <c r="V26" s="27"/>
-      <c r="W26" s="27"/>
-      <c r="X26" s="27"/>
-      <c r="Y26" s="27"/>
+      <c r="N26" s="31"/>
+      <c r="O26" s="31"/>
+      <c r="P26" s="31"/>
+      <c r="Q26" s="31"/>
+      <c r="R26" s="31"/>
+      <c r="S26" s="31"/>
+      <c r="T26" s="31"/>
+      <c r="U26" s="31"/>
+      <c r="V26" s="31"/>
+      <c r="W26" s="31"/>
+      <c r="X26" s="31"/>
+      <c r="Y26" s="31"/>
       <c r="Z26" s="10" t="s">
         <v>130</v>
       </c>
@@ -2512,26 +2522,26 @@
       <c r="I27" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J27" s="32" t="s">
+      <c r="J27" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="K27" s="32"/>
-      <c r="L27" s="32"/>
-      <c r="M27" s="27" t="s">
+      <c r="K27" s="33"/>
+      <c r="L27" s="33"/>
+      <c r="M27" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="N27" s="27"/>
-      <c r="O27" s="27"/>
-      <c r="P27" s="27"/>
-      <c r="Q27" s="27"/>
-      <c r="R27" s="27"/>
-      <c r="S27" s="27"/>
-      <c r="T27" s="27"/>
-      <c r="U27" s="27"/>
-      <c r="V27" s="27"/>
-      <c r="W27" s="27"/>
-      <c r="X27" s="27"/>
-      <c r="Y27" s="27"/>
+      <c r="N27" s="31"/>
+      <c r="O27" s="31"/>
+      <c r="P27" s="31"/>
+      <c r="Q27" s="31"/>
+      <c r="R27" s="31"/>
+      <c r="S27" s="31"/>
+      <c r="T27" s="31"/>
+      <c r="U27" s="31"/>
+      <c r="V27" s="31"/>
+      <c r="W27" s="31"/>
+      <c r="X27" s="31"/>
+      <c r="Y27" s="31"/>
       <c r="Z27" s="14" t="s">
         <v>126</v>
       </c>
@@ -2543,26 +2553,26 @@
       <c r="I28" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J28" s="32" t="s">
+      <c r="J28" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="K28" s="32"/>
-      <c r="L28" s="32"/>
-      <c r="M28" s="30" t="s">
+      <c r="K28" s="33"/>
+      <c r="L28" s="33"/>
+      <c r="M28" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="N28" s="30"/>
-      <c r="O28" s="30"/>
-      <c r="P28" s="30"/>
-      <c r="Q28" s="30"/>
-      <c r="R28" s="30"/>
-      <c r="S28" s="30"/>
-      <c r="T28" s="30"/>
-      <c r="U28" s="30"/>
-      <c r="V28" s="30"/>
-      <c r="W28" s="30"/>
-      <c r="X28" s="30"/>
-      <c r="Y28" s="30"/>
+      <c r="N28" s="32"/>
+      <c r="O28" s="32"/>
+      <c r="P28" s="32"/>
+      <c r="Q28" s="32"/>
+      <c r="R28" s="32"/>
+      <c r="S28" s="32"/>
+      <c r="T28" s="32"/>
+      <c r="U28" s="32"/>
+      <c r="V28" s="32"/>
+      <c r="W28" s="32"/>
+      <c r="X28" s="32"/>
+      <c r="Y28" s="32"/>
       <c r="Z28" s="12" t="s">
         <v>127</v>
       </c>
@@ -2574,26 +2584,26 @@
       <c r="I29" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="J29" s="33" t="s">
+      <c r="J29" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="K29" s="33"/>
-      <c r="L29" s="33"/>
-      <c r="M29" s="27" t="s">
+      <c r="K29" s="34"/>
+      <c r="L29" s="34"/>
+      <c r="M29" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="N29" s="27"/>
-      <c r="O29" s="27"/>
-      <c r="P29" s="27"/>
-      <c r="Q29" s="27"/>
-      <c r="R29" s="27"/>
-      <c r="S29" s="27"/>
-      <c r="T29" s="27"/>
-      <c r="U29" s="27"/>
-      <c r="V29" s="27"/>
-      <c r="W29" s="27"/>
-      <c r="X29" s="27"/>
-      <c r="Y29" s="27"/>
+      <c r="N29" s="31"/>
+      <c r="O29" s="31"/>
+      <c r="P29" s="31"/>
+      <c r="Q29" s="31"/>
+      <c r="R29" s="31"/>
+      <c r="S29" s="31"/>
+      <c r="T29" s="31"/>
+      <c r="U29" s="31"/>
+      <c r="V29" s="31"/>
+      <c r="W29" s="31"/>
+      <c r="X29" s="31"/>
+      <c r="Y29" s="31"/>
       <c r="Z29" s="10" t="s">
         <v>130</v>
       </c>
@@ -2608,25 +2618,25 @@
       <c r="J30" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K30" s="29" t="s">
+      <c r="K30" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="L30" s="29"/>
-      <c r="M30" s="27" t="s">
+      <c r="L30" s="37"/>
+      <c r="M30" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="N30" s="27"/>
-      <c r="O30" s="27"/>
-      <c r="P30" s="27"/>
-      <c r="Q30" s="27"/>
-      <c r="R30" s="27"/>
-      <c r="S30" s="27"/>
-      <c r="T30" s="27"/>
-      <c r="U30" s="27"/>
-      <c r="V30" s="27"/>
-      <c r="W30" s="27"/>
-      <c r="X30" s="27"/>
-      <c r="Y30" s="27"/>
+      <c r="N30" s="31"/>
+      <c r="O30" s="31"/>
+      <c r="P30" s="31"/>
+      <c r="Q30" s="31"/>
+      <c r="R30" s="31"/>
+      <c r="S30" s="31"/>
+      <c r="T30" s="31"/>
+      <c r="U30" s="31"/>
+      <c r="V30" s="31"/>
+      <c r="W30" s="31"/>
+      <c r="X30" s="31"/>
+      <c r="Y30" s="31"/>
       <c r="Z30" s="14" t="s">
         <v>126</v>
       </c>
@@ -2638,26 +2648,26 @@
       <c r="I31" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J31" s="32" t="s">
+      <c r="J31" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="K31" s="32"/>
-      <c r="L31" s="32"/>
-      <c r="M31" s="30" t="s">
+      <c r="K31" s="33"/>
+      <c r="L31" s="33"/>
+      <c r="M31" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="N31" s="30"/>
-      <c r="O31" s="30"/>
-      <c r="P31" s="30"/>
-      <c r="Q31" s="30"/>
-      <c r="R31" s="30"/>
-      <c r="S31" s="30"/>
-      <c r="T31" s="30"/>
-      <c r="U31" s="30"/>
-      <c r="V31" s="30"/>
-      <c r="W31" s="30"/>
-      <c r="X31" s="30"/>
-      <c r="Y31" s="30"/>
+      <c r="N31" s="32"/>
+      <c r="O31" s="32"/>
+      <c r="P31" s="32"/>
+      <c r="Q31" s="32"/>
+      <c r="R31" s="32"/>
+      <c r="S31" s="32"/>
+      <c r="T31" s="32"/>
+      <c r="U31" s="32"/>
+      <c r="V31" s="32"/>
+      <c r="W31" s="32"/>
+      <c r="X31" s="32"/>
+      <c r="Y31" s="32"/>
       <c r="Z31" s="12" t="s">
         <v>127</v>
       </c>
@@ -2669,26 +2679,26 @@
       <c r="I32" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="J32" s="33" t="s">
+      <c r="J32" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="K32" s="33"/>
-      <c r="L32" s="33"/>
-      <c r="M32" s="27" t="s">
+      <c r="K32" s="34"/>
+      <c r="L32" s="34"/>
+      <c r="M32" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="N32" s="27"/>
-      <c r="O32" s="27"/>
-      <c r="P32" s="27"/>
-      <c r="Q32" s="27"/>
-      <c r="R32" s="27"/>
-      <c r="S32" s="27"/>
-      <c r="T32" s="27"/>
-      <c r="U32" s="27"/>
-      <c r="V32" s="27"/>
-      <c r="W32" s="27"/>
-      <c r="X32" s="27"/>
-      <c r="Y32" s="27"/>
+      <c r="N32" s="31"/>
+      <c r="O32" s="31"/>
+      <c r="P32" s="31"/>
+      <c r="Q32" s="31"/>
+      <c r="R32" s="31"/>
+      <c r="S32" s="31"/>
+      <c r="T32" s="31"/>
+      <c r="U32" s="31"/>
+      <c r="V32" s="31"/>
+      <c r="W32" s="31"/>
+      <c r="X32" s="31"/>
+      <c r="Y32" s="31"/>
       <c r="Z32" s="10" t="s">
         <v>130</v>
       </c>
@@ -2700,26 +2710,26 @@
       <c r="I33" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="J33" s="29" t="s">
+      <c r="J33" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="K33" s="29"/>
-      <c r="L33" s="29"/>
-      <c r="M33" s="30" t="s">
+      <c r="K33" s="37"/>
+      <c r="L33" s="37"/>
+      <c r="M33" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="N33" s="30"/>
-      <c r="O33" s="30"/>
-      <c r="P33" s="30"/>
-      <c r="Q33" s="30"/>
-      <c r="R33" s="30"/>
-      <c r="S33" s="30"/>
-      <c r="T33" s="30"/>
-      <c r="U33" s="30"/>
-      <c r="V33" s="30"/>
-      <c r="W33" s="30"/>
-      <c r="X33" s="30"/>
-      <c r="Y33" s="30"/>
+      <c r="N33" s="32"/>
+      <c r="O33" s="32"/>
+      <c r="P33" s="32"/>
+      <c r="Q33" s="32"/>
+      <c r="R33" s="32"/>
+      <c r="S33" s="32"/>
+      <c r="T33" s="32"/>
+      <c r="U33" s="32"/>
+      <c r="V33" s="32"/>
+      <c r="W33" s="32"/>
+      <c r="X33" s="32"/>
+      <c r="Y33" s="32"/>
       <c r="Z33" s="12" t="s">
         <v>127</v>
       </c>
@@ -2732,26 +2742,26 @@
       <c r="I34" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="J34" s="31" t="s">
+      <c r="J34" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="K34" s="31"/>
-      <c r="L34" s="31"/>
-      <c r="M34" s="27" t="s">
+      <c r="K34" s="36"/>
+      <c r="L34" s="36"/>
+      <c r="M34" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="N34" s="27"/>
-      <c r="O34" s="27"/>
-      <c r="P34" s="27"/>
-      <c r="Q34" s="27"/>
-      <c r="R34" s="27"/>
-      <c r="S34" s="27"/>
-      <c r="T34" s="27"/>
-      <c r="U34" s="27"/>
-      <c r="V34" s="27"/>
-      <c r="W34" s="27"/>
-      <c r="X34" s="27"/>
-      <c r="Y34" s="27"/>
+      <c r="N34" s="31"/>
+      <c r="O34" s="31"/>
+      <c r="P34" s="31"/>
+      <c r="Q34" s="31"/>
+      <c r="R34" s="31"/>
+      <c r="S34" s="31"/>
+      <c r="T34" s="31"/>
+      <c r="U34" s="31"/>
+      <c r="V34" s="31"/>
+      <c r="W34" s="31"/>
+      <c r="X34" s="31"/>
+      <c r="Y34" s="31"/>
       <c r="Z34" s="10" t="s">
         <v>130</v>
       </c>
@@ -2767,26 +2777,26 @@
       <c r="I35" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J35" s="28" t="s">
+      <c r="J35" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="K35" s="28"/>
-      <c r="L35" s="28"/>
-      <c r="M35" s="27" t="s">
+      <c r="K35" s="35"/>
+      <c r="L35" s="35"/>
+      <c r="M35" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="N35" s="27"/>
-      <c r="O35" s="27"/>
-      <c r="P35" s="27"/>
-      <c r="Q35" s="27"/>
-      <c r="R35" s="27"/>
-      <c r="S35" s="27"/>
-      <c r="T35" s="27"/>
-      <c r="U35" s="27"/>
-      <c r="V35" s="27"/>
-      <c r="W35" s="27"/>
-      <c r="X35" s="27"/>
-      <c r="Y35" s="27"/>
+      <c r="N35" s="31"/>
+      <c r="O35" s="31"/>
+      <c r="P35" s="31"/>
+      <c r="Q35" s="31"/>
+      <c r="R35" s="31"/>
+      <c r="S35" s="31"/>
+      <c r="T35" s="31"/>
+      <c r="U35" s="31"/>
+      <c r="V35" s="31"/>
+      <c r="W35" s="31"/>
+      <c r="X35" s="31"/>
+      <c r="Y35" s="31"/>
       <c r="Z35" s="14" t="s">
         <v>126</v>
       </c>
@@ -2802,26 +2812,26 @@
       <c r="I36" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J36" s="28" t="s">
+      <c r="J36" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="K36" s="28"/>
-      <c r="L36" s="28"/>
-      <c r="M36" s="30" t="s">
+      <c r="K36" s="35"/>
+      <c r="L36" s="35"/>
+      <c r="M36" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="N36" s="30"/>
-      <c r="O36" s="30"/>
-      <c r="P36" s="30"/>
-      <c r="Q36" s="30"/>
-      <c r="R36" s="30"/>
-      <c r="S36" s="30"/>
-      <c r="T36" s="30"/>
-      <c r="U36" s="30"/>
-      <c r="V36" s="30"/>
-      <c r="W36" s="30"/>
-      <c r="X36" s="30"/>
-      <c r="Y36" s="30"/>
+      <c r="N36" s="32"/>
+      <c r="O36" s="32"/>
+      <c r="P36" s="32"/>
+      <c r="Q36" s="32"/>
+      <c r="R36" s="32"/>
+      <c r="S36" s="32"/>
+      <c r="T36" s="32"/>
+      <c r="U36" s="32"/>
+      <c r="V36" s="32"/>
+      <c r="W36" s="32"/>
+      <c r="X36" s="32"/>
+      <c r="Y36" s="32"/>
       <c r="Z36" s="12" t="s">
         <v>127</v>
       </c>
@@ -2837,26 +2847,26 @@
       <c r="I37" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="J37" s="27" t="s">
+      <c r="J37" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="K37" s="27"/>
-      <c r="L37" s="27"/>
-      <c r="M37" s="27" t="s">
+      <c r="K37" s="31"/>
+      <c r="L37" s="31"/>
+      <c r="M37" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="N37" s="27"/>
-      <c r="O37" s="27"/>
-      <c r="P37" s="27"/>
-      <c r="Q37" s="27"/>
-      <c r="R37" s="27"/>
-      <c r="S37" s="27"/>
-      <c r="T37" s="27"/>
-      <c r="U37" s="27"/>
-      <c r="V37" s="27"/>
-      <c r="W37" s="27"/>
-      <c r="X37" s="27"/>
-      <c r="Y37" s="27"/>
+      <c r="N37" s="31"/>
+      <c r="O37" s="31"/>
+      <c r="P37" s="31"/>
+      <c r="Q37" s="31"/>
+      <c r="R37" s="31"/>
+      <c r="S37" s="31"/>
+      <c r="T37" s="31"/>
+      <c r="U37" s="31"/>
+      <c r="V37" s="31"/>
+      <c r="W37" s="31"/>
+      <c r="X37" s="31"/>
+      <c r="Y37" s="31"/>
       <c r="Z37" s="10" t="s">
         <v>130</v>
       </c>
@@ -2872,26 +2882,26 @@
       <c r="I38" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J38" s="28" t="s">
+      <c r="J38" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="K38" s="28"/>
-      <c r="L38" s="28"/>
-      <c r="M38" s="27" t="s">
+      <c r="K38" s="35"/>
+      <c r="L38" s="35"/>
+      <c r="M38" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="N38" s="27"/>
-      <c r="O38" s="27"/>
-      <c r="P38" s="27"/>
-      <c r="Q38" s="27"/>
-      <c r="R38" s="27"/>
-      <c r="S38" s="27"/>
-      <c r="T38" s="27"/>
-      <c r="U38" s="27"/>
-      <c r="V38" s="27"/>
-      <c r="W38" s="27"/>
-      <c r="X38" s="27"/>
-      <c r="Y38" s="27"/>
+      <c r="N38" s="31"/>
+      <c r="O38" s="31"/>
+      <c r="P38" s="31"/>
+      <c r="Q38" s="31"/>
+      <c r="R38" s="31"/>
+      <c r="S38" s="31"/>
+      <c r="T38" s="31"/>
+      <c r="U38" s="31"/>
+      <c r="V38" s="31"/>
+      <c r="W38" s="31"/>
+      <c r="X38" s="31"/>
+      <c r="Y38" s="31"/>
       <c r="Z38" s="14" t="s">
         <v>126</v>
       </c>
@@ -2907,26 +2917,26 @@
       <c r="I39" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J39" s="28" t="s">
+      <c r="J39" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="K39" s="28"/>
-      <c r="L39" s="28"/>
-      <c r="M39" s="30" t="s">
+      <c r="K39" s="35"/>
+      <c r="L39" s="35"/>
+      <c r="M39" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="N39" s="30"/>
-      <c r="O39" s="30"/>
-      <c r="P39" s="30"/>
-      <c r="Q39" s="30"/>
-      <c r="R39" s="30"/>
-      <c r="S39" s="30"/>
-      <c r="T39" s="30"/>
-      <c r="U39" s="30"/>
-      <c r="V39" s="30"/>
-      <c r="W39" s="30"/>
-      <c r="X39" s="30"/>
-      <c r="Y39" s="30"/>
+      <c r="N39" s="32"/>
+      <c r="O39" s="32"/>
+      <c r="P39" s="32"/>
+      <c r="Q39" s="32"/>
+      <c r="R39" s="32"/>
+      <c r="S39" s="32"/>
+      <c r="T39" s="32"/>
+      <c r="U39" s="32"/>
+      <c r="V39" s="32"/>
+      <c r="W39" s="32"/>
+      <c r="X39" s="32"/>
+      <c r="Y39" s="32"/>
       <c r="Z39" s="12" t="s">
         <v>127</v>
       </c>
@@ -2942,26 +2952,26 @@
       <c r="I40" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="J40" s="28" t="s">
+      <c r="J40" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="K40" s="28"/>
-      <c r="L40" s="28"/>
-      <c r="M40" s="27" t="s">
+      <c r="K40" s="35"/>
+      <c r="L40" s="35"/>
+      <c r="M40" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="N40" s="27"/>
-      <c r="O40" s="27"/>
-      <c r="P40" s="27"/>
-      <c r="Q40" s="27"/>
-      <c r="R40" s="27"/>
-      <c r="S40" s="27"/>
-      <c r="T40" s="27"/>
-      <c r="U40" s="27"/>
-      <c r="V40" s="27"/>
-      <c r="W40" s="27"/>
-      <c r="X40" s="27"/>
-      <c r="Y40" s="27"/>
+      <c r="N40" s="31"/>
+      <c r="O40" s="31"/>
+      <c r="P40" s="31"/>
+      <c r="Q40" s="31"/>
+      <c r="R40" s="31"/>
+      <c r="S40" s="31"/>
+      <c r="T40" s="31"/>
+      <c r="U40" s="31"/>
+      <c r="V40" s="31"/>
+      <c r="W40" s="31"/>
+      <c r="X40" s="31"/>
+      <c r="Y40" s="31"/>
       <c r="Z40" s="10" t="s">
         <v>130</v>
       </c>
@@ -2977,26 +2987,26 @@
       <c r="I41" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="J41" s="27" t="s">
+      <c r="J41" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="K41" s="27"/>
-      <c r="L41" s="27"/>
-      <c r="M41" s="27" t="s">
+      <c r="K41" s="31"/>
+      <c r="L41" s="31"/>
+      <c r="M41" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="N41" s="27"/>
-      <c r="O41" s="27"/>
-      <c r="P41" s="27"/>
-      <c r="Q41" s="27"/>
-      <c r="R41" s="27"/>
-      <c r="S41" s="27"/>
-      <c r="T41" s="27"/>
-      <c r="U41" s="27"/>
-      <c r="V41" s="27"/>
-      <c r="W41" s="27"/>
-      <c r="X41" s="27"/>
-      <c r="Y41" s="27"/>
+      <c r="N41" s="31"/>
+      <c r="O41" s="31"/>
+      <c r="P41" s="31"/>
+      <c r="Q41" s="31"/>
+      <c r="R41" s="31"/>
+      <c r="S41" s="31"/>
+      <c r="T41" s="31"/>
+      <c r="U41" s="31"/>
+      <c r="V41" s="31"/>
+      <c r="W41" s="31"/>
+      <c r="X41" s="31"/>
+      <c r="Y41" s="31"/>
       <c r="Z41" s="10" t="s">
         <v>129</v>
       </c>
@@ -3012,26 +3022,26 @@
       <c r="I42" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J42" s="28" t="s">
+      <c r="J42" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="K42" s="28"/>
-      <c r="L42" s="28"/>
-      <c r="M42" s="27" t="s">
+      <c r="K42" s="35"/>
+      <c r="L42" s="35"/>
+      <c r="M42" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="N42" s="27"/>
-      <c r="O42" s="27"/>
-      <c r="P42" s="27"/>
-      <c r="Q42" s="27"/>
-      <c r="R42" s="27"/>
-      <c r="S42" s="27"/>
-      <c r="T42" s="27"/>
-      <c r="U42" s="27"/>
-      <c r="V42" s="27"/>
-      <c r="W42" s="27"/>
-      <c r="X42" s="27"/>
-      <c r="Y42" s="27"/>
+      <c r="N42" s="31"/>
+      <c r="O42" s="31"/>
+      <c r="P42" s="31"/>
+      <c r="Q42" s="31"/>
+      <c r="R42" s="31"/>
+      <c r="S42" s="31"/>
+      <c r="T42" s="31"/>
+      <c r="U42" s="31"/>
+      <c r="V42" s="31"/>
+      <c r="W42" s="31"/>
+      <c r="X42" s="31"/>
+      <c r="Y42" s="31"/>
       <c r="Z42" s="14" t="s">
         <v>126</v>
       </c>
@@ -3047,26 +3057,26 @@
       <c r="I43" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J43" s="28" t="s">
+      <c r="J43" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="K43" s="28"/>
-      <c r="L43" s="28"/>
-      <c r="M43" s="30" t="s">
+      <c r="K43" s="35"/>
+      <c r="L43" s="35"/>
+      <c r="M43" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="N43" s="30"/>
-      <c r="O43" s="30"/>
-      <c r="P43" s="30"/>
-      <c r="Q43" s="30"/>
-      <c r="R43" s="30"/>
-      <c r="S43" s="30"/>
-      <c r="T43" s="30"/>
-      <c r="U43" s="30"/>
-      <c r="V43" s="30"/>
-      <c r="W43" s="30"/>
-      <c r="X43" s="30"/>
-      <c r="Y43" s="30"/>
+      <c r="N43" s="32"/>
+      <c r="O43" s="32"/>
+      <c r="P43" s="32"/>
+      <c r="Q43" s="32"/>
+      <c r="R43" s="32"/>
+      <c r="S43" s="32"/>
+      <c r="T43" s="32"/>
+      <c r="U43" s="32"/>
+      <c r="V43" s="32"/>
+      <c r="W43" s="32"/>
+      <c r="X43" s="32"/>
+      <c r="Y43" s="32"/>
       <c r="Z43" s="12" t="s">
         <v>127</v>
       </c>
@@ -3082,26 +3092,26 @@
       <c r="I44" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="J44" s="28" t="s">
+      <c r="J44" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="K44" s="28"/>
-      <c r="L44" s="28"/>
-      <c r="M44" s="27" t="s">
+      <c r="K44" s="35"/>
+      <c r="L44" s="35"/>
+      <c r="M44" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="N44" s="27"/>
-      <c r="O44" s="27"/>
-      <c r="P44" s="27"/>
-      <c r="Q44" s="27"/>
-      <c r="R44" s="27"/>
-      <c r="S44" s="27"/>
-      <c r="T44" s="27"/>
-      <c r="U44" s="27"/>
-      <c r="V44" s="27"/>
-      <c r="W44" s="27"/>
-      <c r="X44" s="27"/>
-      <c r="Y44" s="27"/>
+      <c r="N44" s="31"/>
+      <c r="O44" s="31"/>
+      <c r="P44" s="31"/>
+      <c r="Q44" s="31"/>
+      <c r="R44" s="31"/>
+      <c r="S44" s="31"/>
+      <c r="T44" s="31"/>
+      <c r="U44" s="31"/>
+      <c r="V44" s="31"/>
+      <c r="W44" s="31"/>
+      <c r="X44" s="31"/>
+      <c r="Y44" s="31"/>
       <c r="Z44" s="10" t="s">
         <v>130</v>
       </c>
@@ -3117,26 +3127,26 @@
       <c r="I45" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="J45" s="28" t="s">
+      <c r="J45" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="K45" s="28"/>
-      <c r="L45" s="28"/>
-      <c r="M45" s="27" t="s">
+      <c r="K45" s="35"/>
+      <c r="L45" s="35"/>
+      <c r="M45" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="N45" s="27"/>
-      <c r="O45" s="27"/>
-      <c r="P45" s="27"/>
-      <c r="Q45" s="27"/>
-      <c r="R45" s="27"/>
-      <c r="S45" s="27"/>
-      <c r="T45" s="27"/>
-      <c r="U45" s="27"/>
-      <c r="V45" s="27"/>
-      <c r="W45" s="27"/>
-      <c r="X45" s="27"/>
-      <c r="Y45" s="27"/>
+      <c r="N45" s="31"/>
+      <c r="O45" s="31"/>
+      <c r="P45" s="31"/>
+      <c r="Q45" s="31"/>
+      <c r="R45" s="31"/>
+      <c r="S45" s="31"/>
+      <c r="T45" s="31"/>
+      <c r="U45" s="31"/>
+      <c r="V45" s="31"/>
+      <c r="W45" s="31"/>
+      <c r="X45" s="31"/>
+      <c r="Y45" s="31"/>
       <c r="Z45" s="10" t="s">
         <v>129</v>
       </c>
@@ -3152,50 +3162,77 @@
       <c r="I46" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="J46" s="27" t="s">
+      <c r="J46" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="K46" s="27"/>
-      <c r="L46" s="27"/>
-      <c r="M46" s="27" t="s">
+      <c r="K46" s="31"/>
+      <c r="L46" s="31"/>
+      <c r="M46" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="N46" s="27"/>
-      <c r="O46" s="27"/>
-      <c r="P46" s="27"/>
-      <c r="Q46" s="27"/>
-      <c r="R46" s="27"/>
-      <c r="S46" s="27"/>
-      <c r="T46" s="27"/>
-      <c r="U46" s="27"/>
-      <c r="V46" s="27"/>
-      <c r="W46" s="27"/>
-      <c r="X46" s="27"/>
-      <c r="Y46" s="27"/>
+      <c r="N46" s="31"/>
+      <c r="O46" s="31"/>
+      <c r="P46" s="31"/>
+      <c r="Q46" s="31"/>
+      <c r="R46" s="31"/>
+      <c r="S46" s="31"/>
+      <c r="T46" s="31"/>
+      <c r="U46" s="31"/>
+      <c r="V46" s="31"/>
+      <c r="W46" s="31"/>
+      <c r="X46" s="31"/>
+      <c r="Y46" s="31"/>
       <c r="Z46" s="10" t="s">
         <v>128</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="79">
-    <mergeCell ref="Z10:Z12"/>
-    <mergeCell ref="M17:Y17"/>
-    <mergeCell ref="M20:Y20"/>
-    <mergeCell ref="M22:Y22"/>
-    <mergeCell ref="M16:Y16"/>
-    <mergeCell ref="M18:Y18"/>
-    <mergeCell ref="M19:Y19"/>
-    <mergeCell ref="M21:Y21"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="M13:Y13"/>
-    <mergeCell ref="M14:Y14"/>
-    <mergeCell ref="M10:Y12"/>
-    <mergeCell ref="M15:Y15"/>
-    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J46:L46"/>
+    <mergeCell ref="J40:L40"/>
+    <mergeCell ref="J41:L41"/>
+    <mergeCell ref="J42:L42"/>
+    <mergeCell ref="J43:L43"/>
+    <mergeCell ref="J44:L44"/>
+    <mergeCell ref="J45:L45"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="M33:Y33"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="J34:L34"/>
+    <mergeCell ref="M34:Y34"/>
+    <mergeCell ref="M46:Y46"/>
+    <mergeCell ref="M43:Y43"/>
+    <mergeCell ref="M40:Y40"/>
+    <mergeCell ref="M39:Y39"/>
+    <mergeCell ref="M38:Y38"/>
+    <mergeCell ref="M42:Y42"/>
+    <mergeCell ref="M44:Y44"/>
+    <mergeCell ref="M41:Y41"/>
+    <mergeCell ref="M45:Y45"/>
+    <mergeCell ref="M23:Y23"/>
+    <mergeCell ref="M24:Y24"/>
+    <mergeCell ref="M26:Y26"/>
+    <mergeCell ref="M29:Y29"/>
+    <mergeCell ref="M32:Y32"/>
+    <mergeCell ref="M25:Y25"/>
+    <mergeCell ref="M28:Y28"/>
+    <mergeCell ref="M31:Y31"/>
+    <mergeCell ref="M27:Y27"/>
+    <mergeCell ref="M30:Y30"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="J37:L37"/>
+    <mergeCell ref="J38:L38"/>
+    <mergeCell ref="J39:L39"/>
+    <mergeCell ref="M37:Y37"/>
+    <mergeCell ref="J31:L31"/>
+    <mergeCell ref="M36:Y36"/>
+    <mergeCell ref="M35:Y35"/>
     <mergeCell ref="I10:I12"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="J32:L32"/>
@@ -3212,51 +3249,24 @@
     <mergeCell ref="J17:K17"/>
     <mergeCell ref="K22:L22"/>
     <mergeCell ref="J16:L16"/>
-    <mergeCell ref="J37:L37"/>
-    <mergeCell ref="J38:L38"/>
-    <mergeCell ref="J39:L39"/>
-    <mergeCell ref="M37:Y37"/>
-    <mergeCell ref="J31:L31"/>
-    <mergeCell ref="M36:Y36"/>
-    <mergeCell ref="M35:Y35"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="M23:Y23"/>
-    <mergeCell ref="M24:Y24"/>
-    <mergeCell ref="M26:Y26"/>
-    <mergeCell ref="M29:Y29"/>
-    <mergeCell ref="M32:Y32"/>
-    <mergeCell ref="M25:Y25"/>
-    <mergeCell ref="M28:Y28"/>
-    <mergeCell ref="M31:Y31"/>
-    <mergeCell ref="M27:Y27"/>
-    <mergeCell ref="M30:Y30"/>
-    <mergeCell ref="M46:Y46"/>
-    <mergeCell ref="M43:Y43"/>
-    <mergeCell ref="M40:Y40"/>
-    <mergeCell ref="M39:Y39"/>
-    <mergeCell ref="M38:Y38"/>
-    <mergeCell ref="M42:Y42"/>
-    <mergeCell ref="M44:Y44"/>
-    <mergeCell ref="M41:Y41"/>
-    <mergeCell ref="M45:Y45"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="M33:Y33"/>
-    <mergeCell ref="J33:L33"/>
-    <mergeCell ref="J34:L34"/>
-    <mergeCell ref="M34:Y34"/>
-    <mergeCell ref="J46:L46"/>
-    <mergeCell ref="J40:L40"/>
-    <mergeCell ref="J41:L41"/>
-    <mergeCell ref="J42:L42"/>
-    <mergeCell ref="J43:L43"/>
-    <mergeCell ref="J44:L44"/>
-    <mergeCell ref="J45:L45"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="M13:Y13"/>
+    <mergeCell ref="M14:Y14"/>
+    <mergeCell ref="M10:Y12"/>
+    <mergeCell ref="M15:Y15"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="Z10:Z12"/>
+    <mergeCell ref="M17:Y17"/>
+    <mergeCell ref="M20:Y20"/>
+    <mergeCell ref="M22:Y22"/>
+    <mergeCell ref="M16:Y16"/>
+    <mergeCell ref="M18:Y18"/>
+    <mergeCell ref="M19:Y19"/>
+    <mergeCell ref="M21:Y21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3298,28 +3308,28 @@
       <c r="H2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
       <c r="L2" s="9" t="s">
         <v>59</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="N2" s="32" t="s">
+      <c r="N2" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32" t="s">
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
       <c r="U2" s="9" t="s">
         <v>63</v>
       </c>
@@ -3409,11 +3419,11 @@
       <c r="H9" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="I9" s="27" t="s">
+      <c r="I9" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
       <c r="L9" s="9" t="s">
         <v>2</v>
       </c>
@@ -3461,30 +3471,30 @@
       <c r="B10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H10" s="30" t="s">
+      <c r="H10" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="I10" s="27" t="s">
+      <c r="I10" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="30" t="s">
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
-      <c r="O10" s="30"/>
-      <c r="P10" s="30"/>
-      <c r="Q10" s="30"/>
-      <c r="R10" s="30"/>
-      <c r="S10" s="30"/>
-      <c r="T10" s="30"/>
-      <c r="U10" s="30"/>
-      <c r="V10" s="30"/>
-      <c r="W10" s="30"/>
-      <c r="X10" s="30"/>
-      <c r="Y10" s="34" t="s">
+      <c r="M10" s="32"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="32"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="32"/>
+      <c r="R10" s="32"/>
+      <c r="S10" s="32"/>
+      <c r="T10" s="32"/>
+      <c r="U10" s="32"/>
+      <c r="V10" s="32"/>
+      <c r="W10" s="32"/>
+      <c r="X10" s="32"/>
+      <c r="Y10" s="30" t="s">
         <v>125</v>
       </c>
     </row>
@@ -3492,334 +3502,334 @@
       <c r="B11" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="30"/>
-      <c r="I11" s="33" t="s">
+      <c r="H11" s="32"/>
+      <c r="I11" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="30"/>
-      <c r="O11" s="30"/>
-      <c r="P11" s="30"/>
-      <c r="Q11" s="30"/>
-      <c r="R11" s="30"/>
-      <c r="S11" s="30"/>
-      <c r="T11" s="30"/>
-      <c r="U11" s="30"/>
-      <c r="V11" s="30"/>
-      <c r="W11" s="30"/>
-      <c r="X11" s="30"/>
-      <c r="Y11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="32"/>
+      <c r="Q11" s="32"/>
+      <c r="R11" s="32"/>
+      <c r="S11" s="32"/>
+      <c r="T11" s="32"/>
+      <c r="U11" s="32"/>
+      <c r="V11" s="32"/>
+      <c r="W11" s="32"/>
+      <c r="X11" s="32"/>
+      <c r="Y11" s="30"/>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>4</v>
       </c>
-      <c r="H12" s="30"/>
-      <c r="I12" s="28" t="s">
+      <c r="H12" s="32"/>
+      <c r="I12" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="J12" s="27"/>
+      <c r="J12" s="31"/>
       <c r="K12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="L12" s="30"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="30"/>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="30"/>
-      <c r="R12" s="30"/>
-      <c r="S12" s="30"/>
-      <c r="T12" s="30"/>
-      <c r="U12" s="30"/>
-      <c r="V12" s="30"/>
-      <c r="W12" s="30"/>
-      <c r="X12" s="30"/>
-      <c r="Y12" s="34"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="32"/>
+      <c r="O12" s="32"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="32"/>
+      <c r="R12" s="32"/>
+      <c r="S12" s="32"/>
+      <c r="T12" s="32"/>
+      <c r="U12" s="32"/>
+      <c r="V12" s="32"/>
+      <c r="W12" s="32"/>
+      <c r="X12" s="32"/>
+      <c r="Y12" s="30"/>
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>90</v>
       </c>
       <c r="C13" s="6"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="27" t="s">
+      <c r="H13" s="32"/>
+      <c r="I13" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="30"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="30"/>
-      <c r="P13" s="30"/>
-      <c r="Q13" s="30"/>
-      <c r="R13" s="30"/>
-      <c r="S13" s="30"/>
-      <c r="T13" s="30"/>
-      <c r="U13" s="30"/>
-      <c r="V13" s="30"/>
-      <c r="W13" s="30"/>
-      <c r="X13" s="30"/>
-      <c r="Y13" s="34"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="32"/>
+      <c r="O13" s="32"/>
+      <c r="P13" s="32"/>
+      <c r="Q13" s="32"/>
+      <c r="R13" s="32"/>
+      <c r="S13" s="32"/>
+      <c r="T13" s="32"/>
+      <c r="U13" s="32"/>
+      <c r="V13" s="32"/>
+      <c r="W13" s="32"/>
+      <c r="X13" s="32"/>
+      <c r="Y13" s="30"/>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>78</v>
       </c>
-      <c r="H14" s="30"/>
-      <c r="I14" s="33" t="s">
+      <c r="H14" s="32"/>
+      <c r="I14" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="J14" s="33"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="30"/>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="30"/>
-      <c r="R14" s="30"/>
-      <c r="S14" s="30"/>
-      <c r="T14" s="30"/>
-      <c r="U14" s="30"/>
-      <c r="V14" s="30"/>
-      <c r="W14" s="30"/>
-      <c r="X14" s="30"/>
-      <c r="Y14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="32"/>
+      <c r="N14" s="32"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="32"/>
+      <c r="R14" s="32"/>
+      <c r="S14" s="32"/>
+      <c r="T14" s="32"/>
+      <c r="U14" s="32"/>
+      <c r="V14" s="32"/>
+      <c r="W14" s="32"/>
+      <c r="X14" s="32"/>
+      <c r="Y14" s="30"/>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>5</v>
       </c>
-      <c r="H15" s="30"/>
-      <c r="I15" s="32" t="s">
+      <c r="H15" s="32"/>
+      <c r="I15" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="30"/>
-      <c r="P15" s="30"/>
-      <c r="Q15" s="30"/>
-      <c r="R15" s="30"/>
-      <c r="S15" s="30"/>
-      <c r="T15" s="30"/>
-      <c r="U15" s="30"/>
-      <c r="V15" s="30"/>
-      <c r="W15" s="30"/>
-      <c r="X15" s="30"/>
-      <c r="Y15" s="34"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="32"/>
+      <c r="N15" s="32"/>
+      <c r="O15" s="32"/>
+      <c r="P15" s="32"/>
+      <c r="Q15" s="32"/>
+      <c r="R15" s="32"/>
+      <c r="S15" s="32"/>
+      <c r="T15" s="32"/>
+      <c r="U15" s="32"/>
+      <c r="V15" s="32"/>
+      <c r="W15" s="32"/>
+      <c r="X15" s="32"/>
+      <c r="Y15" s="30"/>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>79</v>
       </c>
-      <c r="H16" s="30"/>
-      <c r="I16" s="33" t="s">
+      <c r="H16" s="32"/>
+      <c r="I16" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="J16" s="33"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="30"/>
-      <c r="M16" s="30"/>
-      <c r="N16" s="30"/>
-      <c r="O16" s="30"/>
-      <c r="P16" s="30"/>
-      <c r="Q16" s="30"/>
-      <c r="R16" s="30"/>
-      <c r="S16" s="30"/>
-      <c r="T16" s="30"/>
-      <c r="U16" s="30"/>
-      <c r="V16" s="30"/>
-      <c r="W16" s="30"/>
-      <c r="X16" s="30"/>
-      <c r="Y16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="32"/>
+      <c r="Q16" s="32"/>
+      <c r="R16" s="32"/>
+      <c r="S16" s="32"/>
+      <c r="T16" s="32"/>
+      <c r="U16" s="32"/>
+      <c r="V16" s="32"/>
+      <c r="W16" s="32"/>
+      <c r="X16" s="32"/>
+      <c r="Y16" s="30"/>
     </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="30"/>
-      <c r="I17" s="32" t="s">
+      <c r="H17" s="32"/>
+      <c r="I17" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="J17" s="32"/>
+      <c r="J17" s="33"/>
       <c r="K17" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="L17" s="30"/>
-      <c r="M17" s="30"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="30"/>
-      <c r="P17" s="30"/>
-      <c r="Q17" s="30"/>
-      <c r="R17" s="30"/>
-      <c r="S17" s="30"/>
-      <c r="T17" s="30"/>
-      <c r="U17" s="30"/>
-      <c r="V17" s="30"/>
-      <c r="W17" s="30"/>
-      <c r="X17" s="30"/>
-      <c r="Y17" s="34"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="32"/>
+      <c r="N17" s="32"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="32"/>
+      <c r="Q17" s="32"/>
+      <c r="R17" s="32"/>
+      <c r="S17" s="32"/>
+      <c r="T17" s="32"/>
+      <c r="U17" s="32"/>
+      <c r="V17" s="32"/>
+      <c r="W17" s="32"/>
+      <c r="X17" s="32"/>
+      <c r="Y17" s="30"/>
     </row>
     <row r="18" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>80</v>
       </c>
-      <c r="H18" s="30"/>
-      <c r="I18" s="33" t="s">
+      <c r="H18" s="32"/>
+      <c r="I18" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="J18" s="33"/>
-      <c r="K18" s="33"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="30"/>
-      <c r="P18" s="30"/>
-      <c r="Q18" s="30"/>
-      <c r="R18" s="30"/>
-      <c r="S18" s="30"/>
-      <c r="T18" s="30"/>
-      <c r="U18" s="30"/>
-      <c r="V18" s="30"/>
-      <c r="W18" s="30"/>
-      <c r="X18" s="30"/>
-      <c r="Y18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="32"/>
+      <c r="N18" s="32"/>
+      <c r="O18" s="32"/>
+      <c r="P18" s="32"/>
+      <c r="Q18" s="32"/>
+      <c r="R18" s="32"/>
+      <c r="S18" s="32"/>
+      <c r="T18" s="32"/>
+      <c r="U18" s="32"/>
+      <c r="V18" s="32"/>
+      <c r="W18" s="32"/>
+      <c r="X18" s="32"/>
+      <c r="Y18" s="30"/>
     </row>
     <row r="19" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
         <v>91</v>
       </c>
       <c r="C19" s="6"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="31" t="s">
+      <c r="H19" s="32"/>
+      <c r="I19" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="J19" s="31"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="30"/>
-      <c r="M19" s="30"/>
-      <c r="N19" s="30"/>
-      <c r="O19" s="30"/>
-      <c r="P19" s="30"/>
-      <c r="Q19" s="30"/>
-      <c r="R19" s="30"/>
-      <c r="S19" s="30"/>
-      <c r="T19" s="30"/>
-      <c r="U19" s="30"/>
-      <c r="V19" s="30"/>
-      <c r="W19" s="30"/>
-      <c r="X19" s="30"/>
-      <c r="Y19" s="34"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="32"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="32"/>
+      <c r="O19" s="32"/>
+      <c r="P19" s="32"/>
+      <c r="Q19" s="32"/>
+      <c r="R19" s="32"/>
+      <c r="S19" s="32"/>
+      <c r="T19" s="32"/>
+      <c r="U19" s="32"/>
+      <c r="V19" s="32"/>
+      <c r="W19" s="32"/>
+      <c r="X19" s="32"/>
+      <c r="Y19" s="30"/>
     </row>
     <row r="20" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>7</v>
       </c>
-      <c r="H20" s="30"/>
-      <c r="I20" s="32" t="s">
+      <c r="H20" s="32"/>
+      <c r="I20" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="J20" s="32"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="30"/>
-      <c r="M20" s="30"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="30"/>
-      <c r="P20" s="30"/>
-      <c r="Q20" s="30"/>
-      <c r="R20" s="30"/>
-      <c r="S20" s="30"/>
-      <c r="T20" s="30"/>
-      <c r="U20" s="30"/>
-      <c r="V20" s="30"/>
-      <c r="W20" s="30"/>
-      <c r="X20" s="30"/>
-      <c r="Y20" s="34"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="32"/>
+      <c r="N20" s="32"/>
+      <c r="O20" s="32"/>
+      <c r="P20" s="32"/>
+      <c r="Q20" s="32"/>
+      <c r="R20" s="32"/>
+      <c r="S20" s="32"/>
+      <c r="T20" s="32"/>
+      <c r="U20" s="32"/>
+      <c r="V20" s="32"/>
+      <c r="W20" s="32"/>
+      <c r="X20" s="32"/>
+      <c r="Y20" s="30"/>
     </row>
     <row r="21" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>81</v>
       </c>
-      <c r="H21" s="30"/>
-      <c r="I21" s="33" t="s">
+      <c r="H21" s="32"/>
+      <c r="I21" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="30"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="30"/>
-      <c r="O21" s="30"/>
-      <c r="P21" s="30"/>
-      <c r="Q21" s="30"/>
-      <c r="R21" s="30"/>
-      <c r="S21" s="30"/>
-      <c r="T21" s="30"/>
-      <c r="U21" s="30"/>
-      <c r="V21" s="30"/>
-      <c r="W21" s="30"/>
-      <c r="X21" s="30"/>
-      <c r="Y21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="32"/>
+      <c r="O21" s="32"/>
+      <c r="P21" s="32"/>
+      <c r="Q21" s="32"/>
+      <c r="R21" s="32"/>
+      <c r="S21" s="32"/>
+      <c r="T21" s="32"/>
+      <c r="U21" s="32"/>
+      <c r="V21" s="32"/>
+      <c r="W21" s="32"/>
+      <c r="X21" s="32"/>
+      <c r="Y21" s="30"/>
     </row>
     <row r="22" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>11</v>
       </c>
-      <c r="H22" s="30"/>
+      <c r="H22" s="32"/>
       <c r="I22" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="J22" s="32" t="s">
+      <c r="J22" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="K22" s="32"/>
-      <c r="L22" s="30"/>
-      <c r="M22" s="30"/>
-      <c r="N22" s="30"/>
-      <c r="O22" s="30"/>
-      <c r="P22" s="30"/>
-      <c r="Q22" s="30"/>
-      <c r="R22" s="30"/>
-      <c r="S22" s="30"/>
-      <c r="T22" s="30"/>
-      <c r="U22" s="30"/>
-      <c r="V22" s="30"/>
-      <c r="W22" s="30"/>
-      <c r="X22" s="30"/>
-      <c r="Y22" s="34"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="32"/>
+      <c r="O22" s="32"/>
+      <c r="P22" s="32"/>
+      <c r="Q22" s="32"/>
+      <c r="R22" s="32"/>
+      <c r="S22" s="32"/>
+      <c r="T22" s="32"/>
+      <c r="U22" s="32"/>
+      <c r="V22" s="32"/>
+      <c r="W22" s="32"/>
+      <c r="X22" s="32"/>
+      <c r="Y22" s="30"/>
     </row>
     <row r="23" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C23" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H23" s="30"/>
-      <c r="I23" s="28" t="s">
+      <c r="H23" s="32"/>
+      <c r="I23" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="J23" s="28"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="30"/>
-      <c r="M23" s="30"/>
-      <c r="N23" s="30"/>
-      <c r="O23" s="30"/>
-      <c r="P23" s="30"/>
-      <c r="Q23" s="30"/>
-      <c r="R23" s="30"/>
-      <c r="S23" s="30"/>
-      <c r="T23" s="30"/>
-      <c r="U23" s="30"/>
-      <c r="V23" s="30"/>
-      <c r="W23" s="30"/>
-      <c r="X23" s="30"/>
-      <c r="Y23" s="34"/>
+      <c r="J23" s="35"/>
+      <c r="K23" s="35"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="32"/>
+      <c r="N23" s="32"/>
+      <c r="O23" s="32"/>
+      <c r="P23" s="32"/>
+      <c r="Q23" s="32"/>
+      <c r="R23" s="32"/>
+      <c r="S23" s="32"/>
+      <c r="T23" s="32"/>
+      <c r="U23" s="32"/>
+      <c r="V23" s="32"/>
+      <c r="W23" s="32"/>
+      <c r="X23" s="32"/>
+      <c r="Y23" s="30"/>
     </row>
     <row r="24" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
@@ -3827,280 +3837,280 @@
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="27" t="s">
+      <c r="H24" s="32"/>
+      <c r="I24" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="30"/>
-      <c r="M24" s="30"/>
-      <c r="N24" s="30"/>
-      <c r="O24" s="30"/>
-      <c r="P24" s="30"/>
-      <c r="Q24" s="30"/>
-      <c r="R24" s="30"/>
-      <c r="S24" s="30"/>
-      <c r="T24" s="30"/>
-      <c r="U24" s="30"/>
-      <c r="V24" s="30"/>
-      <c r="W24" s="30"/>
-      <c r="X24" s="30"/>
-      <c r="Y24" s="34"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="32"/>
+      <c r="N24" s="32"/>
+      <c r="O24" s="32"/>
+      <c r="P24" s="32"/>
+      <c r="Q24" s="32"/>
+      <c r="R24" s="32"/>
+      <c r="S24" s="32"/>
+      <c r="T24" s="32"/>
+      <c r="U24" s="32"/>
+      <c r="V24" s="32"/>
+      <c r="W24" s="32"/>
+      <c r="X24" s="32"/>
+      <c r="Y24" s="30"/>
     </row>
     <row r="25" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>20</v>
       </c>
-      <c r="H25" s="30"/>
-      <c r="I25" s="32" t="s">
+      <c r="H25" s="32"/>
+      <c r="I25" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="J25" s="32"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="30"/>
-      <c r="M25" s="30"/>
-      <c r="N25" s="30"/>
-      <c r="O25" s="30"/>
-      <c r="P25" s="30"/>
-      <c r="Q25" s="30"/>
-      <c r="R25" s="30"/>
-      <c r="S25" s="30"/>
-      <c r="T25" s="30"/>
-      <c r="U25" s="30"/>
-      <c r="V25" s="30"/>
-      <c r="W25" s="30"/>
-      <c r="X25" s="30"/>
-      <c r="Y25" s="34"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="32"/>
+      <c r="O25" s="32"/>
+      <c r="P25" s="32"/>
+      <c r="Q25" s="32"/>
+      <c r="R25" s="32"/>
+      <c r="S25" s="32"/>
+      <c r="T25" s="32"/>
+      <c r="U25" s="32"/>
+      <c r="V25" s="32"/>
+      <c r="W25" s="32"/>
+      <c r="X25" s="32"/>
+      <c r="Y25" s="30"/>
     </row>
     <row r="26" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>82</v>
       </c>
-      <c r="H26" s="30"/>
-      <c r="I26" s="33" t="s">
+      <c r="H26" s="32"/>
+      <c r="I26" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="J26" s="33"/>
-      <c r="K26" s="33"/>
-      <c r="L26" s="30"/>
-      <c r="M26" s="30"/>
-      <c r="N26" s="30"/>
-      <c r="O26" s="30"/>
-      <c r="P26" s="30"/>
-      <c r="Q26" s="30"/>
-      <c r="R26" s="30"/>
-      <c r="S26" s="30"/>
-      <c r="T26" s="30"/>
-      <c r="U26" s="30"/>
-      <c r="V26" s="30"/>
-      <c r="W26" s="30"/>
-      <c r="X26" s="30"/>
-      <c r="Y26" s="34"/>
+      <c r="J26" s="34"/>
+      <c r="K26" s="34"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="32"/>
+      <c r="N26" s="32"/>
+      <c r="O26" s="32"/>
+      <c r="P26" s="32"/>
+      <c r="Q26" s="32"/>
+      <c r="R26" s="32"/>
+      <c r="S26" s="32"/>
+      <c r="T26" s="32"/>
+      <c r="U26" s="32"/>
+      <c r="V26" s="32"/>
+      <c r="W26" s="32"/>
+      <c r="X26" s="32"/>
+      <c r="Y26" s="30"/>
     </row>
     <row r="27" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>12</v>
       </c>
-      <c r="H27" s="30"/>
-      <c r="I27" s="32" t="s">
+      <c r="H27" s="32"/>
+      <c r="I27" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="J27" s="32"/>
-      <c r="K27" s="32"/>
-      <c r="L27" s="30"/>
-      <c r="M27" s="30"/>
-      <c r="N27" s="30"/>
-      <c r="O27" s="30"/>
-      <c r="P27" s="30"/>
-      <c r="Q27" s="30"/>
-      <c r="R27" s="30"/>
-      <c r="S27" s="30"/>
-      <c r="T27" s="30"/>
-      <c r="U27" s="30"/>
-      <c r="V27" s="30"/>
-      <c r="W27" s="30"/>
-      <c r="X27" s="30"/>
-      <c r="Y27" s="34"/>
+      <c r="J27" s="33"/>
+      <c r="K27" s="33"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="32"/>
+      <c r="N27" s="32"/>
+      <c r="O27" s="32"/>
+      <c r="P27" s="32"/>
+      <c r="Q27" s="32"/>
+      <c r="R27" s="32"/>
+      <c r="S27" s="32"/>
+      <c r="T27" s="32"/>
+      <c r="U27" s="32"/>
+      <c r="V27" s="32"/>
+      <c r="W27" s="32"/>
+      <c r="X27" s="32"/>
+      <c r="Y27" s="30"/>
     </row>
     <row r="28" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>9</v>
       </c>
-      <c r="H28" s="30"/>
-      <c r="I28" s="32" t="s">
+      <c r="H28" s="32"/>
+      <c r="I28" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="J28" s="32"/>
-      <c r="K28" s="32"/>
-      <c r="L28" s="30"/>
-      <c r="M28" s="30"/>
-      <c r="N28" s="30"/>
-      <c r="O28" s="30"/>
-      <c r="P28" s="30"/>
-      <c r="Q28" s="30"/>
-      <c r="R28" s="30"/>
-      <c r="S28" s="30"/>
-      <c r="T28" s="30"/>
-      <c r="U28" s="30"/>
-      <c r="V28" s="30"/>
-      <c r="W28" s="30"/>
-      <c r="X28" s="30"/>
-      <c r="Y28" s="34"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="32"/>
+      <c r="M28" s="32"/>
+      <c r="N28" s="32"/>
+      <c r="O28" s="32"/>
+      <c r="P28" s="32"/>
+      <c r="Q28" s="32"/>
+      <c r="R28" s="32"/>
+      <c r="S28" s="32"/>
+      <c r="T28" s="32"/>
+      <c r="U28" s="32"/>
+      <c r="V28" s="32"/>
+      <c r="W28" s="32"/>
+      <c r="X28" s="32"/>
+      <c r="Y28" s="30"/>
     </row>
     <row r="29" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>83</v>
       </c>
-      <c r="H29" s="30"/>
-      <c r="I29" s="33" t="s">
+      <c r="H29" s="32"/>
+      <c r="I29" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="J29" s="33"/>
-      <c r="K29" s="33"/>
-      <c r="L29" s="30"/>
-      <c r="M29" s="30"/>
-      <c r="N29" s="30"/>
-      <c r="O29" s="30"/>
-      <c r="P29" s="30"/>
-      <c r="Q29" s="30"/>
-      <c r="R29" s="30"/>
-      <c r="S29" s="30"/>
-      <c r="T29" s="30"/>
-      <c r="U29" s="30"/>
-      <c r="V29" s="30"/>
-      <c r="W29" s="30"/>
-      <c r="X29" s="30"/>
-      <c r="Y29" s="34"/>
+      <c r="J29" s="34"/>
+      <c r="K29" s="34"/>
+      <c r="L29" s="32"/>
+      <c r="M29" s="32"/>
+      <c r="N29" s="32"/>
+      <c r="O29" s="32"/>
+      <c r="P29" s="32"/>
+      <c r="Q29" s="32"/>
+      <c r="R29" s="32"/>
+      <c r="S29" s="32"/>
+      <c r="T29" s="32"/>
+      <c r="U29" s="32"/>
+      <c r="V29" s="32"/>
+      <c r="W29" s="32"/>
+      <c r="X29" s="32"/>
+      <c r="Y29" s="30"/>
     </row>
     <row r="30" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>13</v>
       </c>
-      <c r="H30" s="30"/>
+      <c r="H30" s="32"/>
       <c r="I30" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J30" s="29" t="s">
+      <c r="J30" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="K30" s="29"/>
-      <c r="L30" s="30"/>
-      <c r="M30" s="30"/>
-      <c r="N30" s="30"/>
-      <c r="O30" s="30"/>
-      <c r="P30" s="30"/>
-      <c r="Q30" s="30"/>
-      <c r="R30" s="30"/>
-      <c r="S30" s="30"/>
-      <c r="T30" s="30"/>
-      <c r="U30" s="30"/>
-      <c r="V30" s="30"/>
-      <c r="W30" s="30"/>
-      <c r="X30" s="30"/>
-      <c r="Y30" s="34"/>
+      <c r="K30" s="37"/>
+      <c r="L30" s="32"/>
+      <c r="M30" s="32"/>
+      <c r="N30" s="32"/>
+      <c r="O30" s="32"/>
+      <c r="P30" s="32"/>
+      <c r="Q30" s="32"/>
+      <c r="R30" s="32"/>
+      <c r="S30" s="32"/>
+      <c r="T30" s="32"/>
+      <c r="U30" s="32"/>
+      <c r="V30" s="32"/>
+      <c r="W30" s="32"/>
+      <c r="X30" s="32"/>
+      <c r="Y30" s="30"/>
     </row>
     <row r="31" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>19</v>
       </c>
-      <c r="H31" s="30"/>
-      <c r="I31" s="32" t="s">
+      <c r="H31" s="32"/>
+      <c r="I31" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="J31" s="32"/>
-      <c r="K31" s="32"/>
-      <c r="L31" s="30"/>
-      <c r="M31" s="30"/>
-      <c r="N31" s="30"/>
-      <c r="O31" s="30"/>
-      <c r="P31" s="30"/>
-      <c r="Q31" s="30"/>
-      <c r="R31" s="30"/>
-      <c r="S31" s="30"/>
-      <c r="T31" s="30"/>
-      <c r="U31" s="30"/>
-      <c r="V31" s="30"/>
-      <c r="W31" s="30"/>
-      <c r="X31" s="30"/>
-      <c r="Y31" s="34"/>
+      <c r="J31" s="33"/>
+      <c r="K31" s="33"/>
+      <c r="L31" s="32"/>
+      <c r="M31" s="32"/>
+      <c r="N31" s="32"/>
+      <c r="O31" s="32"/>
+      <c r="P31" s="32"/>
+      <c r="Q31" s="32"/>
+      <c r="R31" s="32"/>
+      <c r="S31" s="32"/>
+      <c r="T31" s="32"/>
+      <c r="U31" s="32"/>
+      <c r="V31" s="32"/>
+      <c r="W31" s="32"/>
+      <c r="X31" s="32"/>
+      <c r="Y31" s="30"/>
     </row>
     <row r="32" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>85</v>
       </c>
-      <c r="H32" s="30"/>
-      <c r="I32" s="33" t="s">
+      <c r="H32" s="32"/>
+      <c r="I32" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="J32" s="33"/>
-      <c r="K32" s="33"/>
-      <c r="L32" s="30"/>
-      <c r="M32" s="30"/>
-      <c r="N32" s="30"/>
-      <c r="O32" s="30"/>
-      <c r="P32" s="30"/>
-      <c r="Q32" s="30"/>
-      <c r="R32" s="30"/>
-      <c r="S32" s="30"/>
-      <c r="T32" s="30"/>
-      <c r="U32" s="30"/>
-      <c r="V32" s="30"/>
-      <c r="W32" s="30"/>
-      <c r="X32" s="30"/>
-      <c r="Y32" s="34"/>
+      <c r="J32" s="34"/>
+      <c r="K32" s="34"/>
+      <c r="L32" s="32"/>
+      <c r="M32" s="32"/>
+      <c r="N32" s="32"/>
+      <c r="O32" s="32"/>
+      <c r="P32" s="32"/>
+      <c r="Q32" s="32"/>
+      <c r="R32" s="32"/>
+      <c r="S32" s="32"/>
+      <c r="T32" s="32"/>
+      <c r="U32" s="32"/>
+      <c r="V32" s="32"/>
+      <c r="W32" s="32"/>
+      <c r="X32" s="32"/>
+      <c r="Y32" s="30"/>
     </row>
     <row r="33" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
         <v>84</v>
       </c>
       <c r="C33" s="6"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="29" t="s">
+      <c r="H33" s="32"/>
+      <c r="I33" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="J33" s="29"/>
-      <c r="K33" s="29"/>
-      <c r="L33" s="30"/>
-      <c r="M33" s="30"/>
-      <c r="N33" s="30"/>
-      <c r="O33" s="30"/>
-      <c r="P33" s="30"/>
-      <c r="Q33" s="30"/>
-      <c r="R33" s="30"/>
-      <c r="S33" s="30"/>
-      <c r="T33" s="30"/>
-      <c r="U33" s="30"/>
-      <c r="V33" s="30"/>
-      <c r="W33" s="30"/>
-      <c r="X33" s="30"/>
-      <c r="Y33" s="34"/>
+      <c r="J33" s="37"/>
+      <c r="K33" s="37"/>
+      <c r="L33" s="32"/>
+      <c r="M33" s="32"/>
+      <c r="N33" s="32"/>
+      <c r="O33" s="32"/>
+      <c r="P33" s="32"/>
+      <c r="Q33" s="32"/>
+      <c r="R33" s="32"/>
+      <c r="S33" s="32"/>
+      <c r="T33" s="32"/>
+      <c r="U33" s="32"/>
+      <c r="V33" s="32"/>
+      <c r="W33" s="32"/>
+      <c r="X33" s="32"/>
+      <c r="Y33" s="30"/>
     </row>
     <row r="34" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="s">
         <v>118</v>
       </c>
       <c r="C34" s="6"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="31" t="s">
+      <c r="H34" s="32"/>
+      <c r="I34" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="J34" s="31"/>
-      <c r="K34" s="31"/>
-      <c r="L34" s="30"/>
-      <c r="M34" s="30"/>
-      <c r="N34" s="30"/>
-      <c r="O34" s="30"/>
-      <c r="P34" s="30"/>
-      <c r="Q34" s="30"/>
-      <c r="R34" s="30"/>
-      <c r="S34" s="30"/>
-      <c r="T34" s="30"/>
-      <c r="U34" s="30"/>
-      <c r="V34" s="30"/>
-      <c r="W34" s="30"/>
-      <c r="X34" s="30"/>
-      <c r="Y34" s="34"/>
+      <c r="J34" s="36"/>
+      <c r="K34" s="36"/>
+      <c r="L34" s="32"/>
+      <c r="M34" s="32"/>
+      <c r="N34" s="32"/>
+      <c r="O34" s="32"/>
+      <c r="P34" s="32"/>
+      <c r="Q34" s="32"/>
+      <c r="R34" s="32"/>
+      <c r="S34" s="32"/>
+      <c r="T34" s="32"/>
+      <c r="U34" s="32"/>
+      <c r="V34" s="32"/>
+      <c r="W34" s="32"/>
+      <c r="X34" s="32"/>
+      <c r="Y34" s="30"/>
     </row>
     <row r="35" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
@@ -4109,26 +4119,26 @@
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="28" t="s">
+      <c r="H35" s="32"/>
+      <c r="I35" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="J35" s="28"/>
-      <c r="K35" s="28"/>
-      <c r="L35" s="30"/>
-      <c r="M35" s="30"/>
-      <c r="N35" s="30"/>
-      <c r="O35" s="30"/>
-      <c r="P35" s="30"/>
-      <c r="Q35" s="30"/>
-      <c r="R35" s="30"/>
-      <c r="S35" s="30"/>
-      <c r="T35" s="30"/>
-      <c r="U35" s="30"/>
-      <c r="V35" s="30"/>
-      <c r="W35" s="30"/>
-      <c r="X35" s="30"/>
-      <c r="Y35" s="34"/>
+      <c r="J35" s="35"/>
+      <c r="K35" s="35"/>
+      <c r="L35" s="32"/>
+      <c r="M35" s="32"/>
+      <c r="N35" s="32"/>
+      <c r="O35" s="32"/>
+      <c r="P35" s="32"/>
+      <c r="Q35" s="32"/>
+      <c r="R35" s="32"/>
+      <c r="S35" s="32"/>
+      <c r="T35" s="32"/>
+      <c r="U35" s="32"/>
+      <c r="V35" s="32"/>
+      <c r="W35" s="32"/>
+      <c r="X35" s="32"/>
+      <c r="Y35" s="30"/>
     </row>
     <row r="36" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B36" s="6"/>
@@ -4137,26 +4147,26 @@
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
-      <c r="H36" s="30"/>
-      <c r="I36" s="28" t="s">
+      <c r="H36" s="32"/>
+      <c r="I36" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="J36" s="28"/>
-      <c r="K36" s="28"/>
-      <c r="L36" s="30"/>
-      <c r="M36" s="30"/>
-      <c r="N36" s="30"/>
-      <c r="O36" s="30"/>
-      <c r="P36" s="30"/>
-      <c r="Q36" s="30"/>
-      <c r="R36" s="30"/>
-      <c r="S36" s="30"/>
-      <c r="T36" s="30"/>
-      <c r="U36" s="30"/>
-      <c r="V36" s="30"/>
-      <c r="W36" s="30"/>
-      <c r="X36" s="30"/>
-      <c r="Y36" s="34"/>
+      <c r="J36" s="35"/>
+      <c r="K36" s="35"/>
+      <c r="L36" s="32"/>
+      <c r="M36" s="32"/>
+      <c r="N36" s="32"/>
+      <c r="O36" s="32"/>
+      <c r="P36" s="32"/>
+      <c r="Q36" s="32"/>
+      <c r="R36" s="32"/>
+      <c r="S36" s="32"/>
+      <c r="T36" s="32"/>
+      <c r="U36" s="32"/>
+      <c r="V36" s="32"/>
+      <c r="W36" s="32"/>
+      <c r="X36" s="32"/>
+      <c r="Y36" s="30"/>
     </row>
     <row r="37" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
@@ -4165,26 +4175,26 @@
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
-      <c r="H37" s="30"/>
-      <c r="I37" s="27" t="s">
+      <c r="H37" s="32"/>
+      <c r="I37" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="J37" s="27"/>
-      <c r="K37" s="27"/>
-      <c r="L37" s="30"/>
-      <c r="M37" s="30"/>
-      <c r="N37" s="30"/>
-      <c r="O37" s="30"/>
-      <c r="P37" s="30"/>
-      <c r="Q37" s="30"/>
-      <c r="R37" s="30"/>
-      <c r="S37" s="30"/>
-      <c r="T37" s="30"/>
-      <c r="U37" s="30"/>
-      <c r="V37" s="30"/>
-      <c r="W37" s="30"/>
-      <c r="X37" s="30"/>
-      <c r="Y37" s="34"/>
+      <c r="J37" s="31"/>
+      <c r="K37" s="31"/>
+      <c r="L37" s="32"/>
+      <c r="M37" s="32"/>
+      <c r="N37" s="32"/>
+      <c r="O37" s="32"/>
+      <c r="P37" s="32"/>
+      <c r="Q37" s="32"/>
+      <c r="R37" s="32"/>
+      <c r="S37" s="32"/>
+      <c r="T37" s="32"/>
+      <c r="U37" s="32"/>
+      <c r="V37" s="32"/>
+      <c r="W37" s="32"/>
+      <c r="X37" s="32"/>
+      <c r="Y37" s="30"/>
     </row>
     <row r="38" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
@@ -4193,26 +4203,26 @@
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
-      <c r="H38" s="30"/>
-      <c r="I38" s="28" t="s">
+      <c r="H38" s="32"/>
+      <c r="I38" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="J38" s="28"/>
-      <c r="K38" s="28"/>
-      <c r="L38" s="30"/>
-      <c r="M38" s="30"/>
-      <c r="N38" s="30"/>
-      <c r="O38" s="30"/>
-      <c r="P38" s="30"/>
-      <c r="Q38" s="30"/>
-      <c r="R38" s="30"/>
-      <c r="S38" s="30"/>
-      <c r="T38" s="30"/>
-      <c r="U38" s="30"/>
-      <c r="V38" s="30"/>
-      <c r="W38" s="30"/>
-      <c r="X38" s="30"/>
-      <c r="Y38" s="34"/>
+      <c r="J38" s="35"/>
+      <c r="K38" s="35"/>
+      <c r="L38" s="32"/>
+      <c r="M38" s="32"/>
+      <c r="N38" s="32"/>
+      <c r="O38" s="32"/>
+      <c r="P38" s="32"/>
+      <c r="Q38" s="32"/>
+      <c r="R38" s="32"/>
+      <c r="S38" s="32"/>
+      <c r="T38" s="32"/>
+      <c r="U38" s="32"/>
+      <c r="V38" s="32"/>
+      <c r="W38" s="32"/>
+      <c r="X38" s="32"/>
+      <c r="Y38" s="30"/>
     </row>
     <row r="39" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B39" s="6"/>
@@ -4221,26 +4231,26 @@
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
-      <c r="H39" s="30"/>
-      <c r="I39" s="28" t="s">
+      <c r="H39" s="32"/>
+      <c r="I39" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="J39" s="28"/>
-      <c r="K39" s="28"/>
-      <c r="L39" s="30"/>
-      <c r="M39" s="30"/>
-      <c r="N39" s="30"/>
-      <c r="O39" s="30"/>
-      <c r="P39" s="30"/>
-      <c r="Q39" s="30"/>
-      <c r="R39" s="30"/>
-      <c r="S39" s="30"/>
-      <c r="T39" s="30"/>
-      <c r="U39" s="30"/>
-      <c r="V39" s="30"/>
-      <c r="W39" s="30"/>
-      <c r="X39" s="30"/>
-      <c r="Y39" s="34"/>
+      <c r="J39" s="35"/>
+      <c r="K39" s="35"/>
+      <c r="L39" s="32"/>
+      <c r="M39" s="32"/>
+      <c r="N39" s="32"/>
+      <c r="O39" s="32"/>
+      <c r="P39" s="32"/>
+      <c r="Q39" s="32"/>
+      <c r="R39" s="32"/>
+      <c r="S39" s="32"/>
+      <c r="T39" s="32"/>
+      <c r="U39" s="32"/>
+      <c r="V39" s="32"/>
+      <c r="W39" s="32"/>
+      <c r="X39" s="32"/>
+      <c r="Y39" s="30"/>
     </row>
     <row r="40" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B40" s="6"/>
@@ -4249,26 +4259,26 @@
         <v>9</v>
       </c>
       <c r="E40" s="6"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="28" t="s">
+      <c r="H40" s="32"/>
+      <c r="I40" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="J40" s="28"/>
-      <c r="K40" s="28"/>
-      <c r="L40" s="30"/>
-      <c r="M40" s="30"/>
-      <c r="N40" s="30"/>
-      <c r="O40" s="30"/>
-      <c r="P40" s="30"/>
-      <c r="Q40" s="30"/>
-      <c r="R40" s="30"/>
-      <c r="S40" s="30"/>
-      <c r="T40" s="30"/>
-      <c r="U40" s="30"/>
-      <c r="V40" s="30"/>
-      <c r="W40" s="30"/>
-      <c r="X40" s="30"/>
-      <c r="Y40" s="34"/>
+      <c r="J40" s="35"/>
+      <c r="K40" s="35"/>
+      <c r="L40" s="32"/>
+      <c r="M40" s="32"/>
+      <c r="N40" s="32"/>
+      <c r="O40" s="32"/>
+      <c r="P40" s="32"/>
+      <c r="Q40" s="32"/>
+      <c r="R40" s="32"/>
+      <c r="S40" s="32"/>
+      <c r="T40" s="32"/>
+      <c r="U40" s="32"/>
+      <c r="V40" s="32"/>
+      <c r="W40" s="32"/>
+      <c r="X40" s="32"/>
+      <c r="Y40" s="30"/>
     </row>
     <row r="41" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
@@ -4277,26 +4287,26 @@
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
-      <c r="H41" s="30"/>
-      <c r="I41" s="27" t="s">
+      <c r="H41" s="32"/>
+      <c r="I41" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="J41" s="27"/>
-      <c r="K41" s="27"/>
-      <c r="L41" s="30"/>
-      <c r="M41" s="30"/>
-      <c r="N41" s="30"/>
-      <c r="O41" s="30"/>
-      <c r="P41" s="30"/>
-      <c r="Q41" s="30"/>
-      <c r="R41" s="30"/>
-      <c r="S41" s="30"/>
-      <c r="T41" s="30"/>
-      <c r="U41" s="30"/>
-      <c r="V41" s="30"/>
-      <c r="W41" s="30"/>
-      <c r="X41" s="30"/>
-      <c r="Y41" s="34"/>
+      <c r="J41" s="31"/>
+      <c r="K41" s="31"/>
+      <c r="L41" s="32"/>
+      <c r="M41" s="32"/>
+      <c r="N41" s="32"/>
+      <c r="O41" s="32"/>
+      <c r="P41" s="32"/>
+      <c r="Q41" s="32"/>
+      <c r="R41" s="32"/>
+      <c r="S41" s="32"/>
+      <c r="T41" s="32"/>
+      <c r="U41" s="32"/>
+      <c r="V41" s="32"/>
+      <c r="W41" s="32"/>
+      <c r="X41" s="32"/>
+      <c r="Y41" s="30"/>
     </row>
     <row r="42" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
@@ -4305,26 +4315,26 @@
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
-      <c r="H42" s="30"/>
-      <c r="I42" s="28" t="s">
+      <c r="H42" s="32"/>
+      <c r="I42" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="J42" s="28"/>
-      <c r="K42" s="28"/>
-      <c r="L42" s="30"/>
-      <c r="M42" s="30"/>
-      <c r="N42" s="30"/>
-      <c r="O42" s="30"/>
-      <c r="P42" s="30"/>
-      <c r="Q42" s="30"/>
-      <c r="R42" s="30"/>
-      <c r="S42" s="30"/>
-      <c r="T42" s="30"/>
-      <c r="U42" s="30"/>
-      <c r="V42" s="30"/>
-      <c r="W42" s="30"/>
-      <c r="X42" s="30"/>
-      <c r="Y42" s="34"/>
+      <c r="J42" s="35"/>
+      <c r="K42" s="35"/>
+      <c r="L42" s="32"/>
+      <c r="M42" s="32"/>
+      <c r="N42" s="32"/>
+      <c r="O42" s="32"/>
+      <c r="P42" s="32"/>
+      <c r="Q42" s="32"/>
+      <c r="R42" s="32"/>
+      <c r="S42" s="32"/>
+      <c r="T42" s="32"/>
+      <c r="U42" s="32"/>
+      <c r="V42" s="32"/>
+      <c r="W42" s="32"/>
+      <c r="X42" s="32"/>
+      <c r="Y42" s="30"/>
     </row>
     <row r="43" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
@@ -4333,26 +4343,26 @@
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
-      <c r="H43" s="30"/>
-      <c r="I43" s="28" t="s">
+      <c r="H43" s="32"/>
+      <c r="I43" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="J43" s="28"/>
-      <c r="K43" s="28"/>
-      <c r="L43" s="30"/>
-      <c r="M43" s="30"/>
-      <c r="N43" s="30"/>
-      <c r="O43" s="30"/>
-      <c r="P43" s="30"/>
-      <c r="Q43" s="30"/>
-      <c r="R43" s="30"/>
-      <c r="S43" s="30"/>
-      <c r="T43" s="30"/>
-      <c r="U43" s="30"/>
-      <c r="V43" s="30"/>
-      <c r="W43" s="30"/>
-      <c r="X43" s="30"/>
-      <c r="Y43" s="34"/>
+      <c r="J43" s="35"/>
+      <c r="K43" s="35"/>
+      <c r="L43" s="32"/>
+      <c r="M43" s="32"/>
+      <c r="N43" s="32"/>
+      <c r="O43" s="32"/>
+      <c r="P43" s="32"/>
+      <c r="Q43" s="32"/>
+      <c r="R43" s="32"/>
+      <c r="S43" s="32"/>
+      <c r="T43" s="32"/>
+      <c r="U43" s="32"/>
+      <c r="V43" s="32"/>
+      <c r="W43" s="32"/>
+      <c r="X43" s="32"/>
+      <c r="Y43" s="30"/>
     </row>
     <row r="44" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B44" s="6"/>
@@ -4361,26 +4371,26 @@
         <v>9</v>
       </c>
       <c r="E44" s="6"/>
-      <c r="H44" s="30"/>
-      <c r="I44" s="28" t="s">
+      <c r="H44" s="32"/>
+      <c r="I44" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="J44" s="28"/>
-      <c r="K44" s="28"/>
-      <c r="L44" s="30"/>
-      <c r="M44" s="30"/>
-      <c r="N44" s="30"/>
-      <c r="O44" s="30"/>
-      <c r="P44" s="30"/>
-      <c r="Q44" s="30"/>
-      <c r="R44" s="30"/>
-      <c r="S44" s="30"/>
-      <c r="T44" s="30"/>
-      <c r="U44" s="30"/>
-      <c r="V44" s="30"/>
-      <c r="W44" s="30"/>
-      <c r="X44" s="30"/>
-      <c r="Y44" s="34"/>
+      <c r="J44" s="35"/>
+      <c r="K44" s="35"/>
+      <c r="L44" s="32"/>
+      <c r="M44" s="32"/>
+      <c r="N44" s="32"/>
+      <c r="O44" s="32"/>
+      <c r="P44" s="32"/>
+      <c r="Q44" s="32"/>
+      <c r="R44" s="32"/>
+      <c r="S44" s="32"/>
+      <c r="T44" s="32"/>
+      <c r="U44" s="32"/>
+      <c r="V44" s="32"/>
+      <c r="W44" s="32"/>
+      <c r="X44" s="32"/>
+      <c r="Y44" s="30"/>
     </row>
     <row r="45" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B45" s="6"/>
@@ -4389,26 +4399,26 @@
       <c r="E45" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H45" s="30"/>
-      <c r="I45" s="28" t="s">
+      <c r="H45" s="32"/>
+      <c r="I45" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="J45" s="28"/>
-      <c r="K45" s="28"/>
-      <c r="L45" s="30"/>
-      <c r="M45" s="30"/>
-      <c r="N45" s="30"/>
-      <c r="O45" s="30"/>
-      <c r="P45" s="30"/>
-      <c r="Q45" s="30"/>
-      <c r="R45" s="30"/>
-      <c r="S45" s="30"/>
-      <c r="T45" s="30"/>
-      <c r="U45" s="30"/>
-      <c r="V45" s="30"/>
-      <c r="W45" s="30"/>
-      <c r="X45" s="30"/>
-      <c r="Y45" s="34"/>
+      <c r="J45" s="35"/>
+      <c r="K45" s="35"/>
+      <c r="L45" s="32"/>
+      <c r="M45" s="32"/>
+      <c r="N45" s="32"/>
+      <c r="O45" s="32"/>
+      <c r="P45" s="32"/>
+      <c r="Q45" s="32"/>
+      <c r="R45" s="32"/>
+      <c r="S45" s="32"/>
+      <c r="T45" s="32"/>
+      <c r="U45" s="32"/>
+      <c r="V45" s="32"/>
+      <c r="W45" s="32"/>
+      <c r="X45" s="32"/>
+      <c r="Y45" s="30"/>
     </row>
     <row r="46" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B46" s="6" t="s">
@@ -4417,29 +4427,57 @@
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
-      <c r="H46" s="30"/>
-      <c r="I46" s="27" t="s">
+      <c r="H46" s="32"/>
+      <c r="I46" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="J46" s="27"/>
-      <c r="K46" s="27"/>
-      <c r="L46" s="30"/>
-      <c r="M46" s="30"/>
-      <c r="N46" s="30"/>
-      <c r="O46" s="30"/>
-      <c r="P46" s="30"/>
-      <c r="Q46" s="30"/>
-      <c r="R46" s="30"/>
-      <c r="S46" s="30"/>
-      <c r="T46" s="30"/>
-      <c r="U46" s="30"/>
-      <c r="V46" s="30"/>
-      <c r="W46" s="30"/>
-      <c r="X46" s="30"/>
-      <c r="Y46" s="34"/>
+      <c r="J46" s="31"/>
+      <c r="K46" s="31"/>
+      <c r="L46" s="32"/>
+      <c r="M46" s="32"/>
+      <c r="N46" s="32"/>
+      <c r="O46" s="32"/>
+      <c r="P46" s="32"/>
+      <c r="Q46" s="32"/>
+      <c r="R46" s="32"/>
+      <c r="S46" s="32"/>
+      <c r="T46" s="32"/>
+      <c r="U46" s="32"/>
+      <c r="V46" s="32"/>
+      <c r="W46" s="32"/>
+      <c r="X46" s="32"/>
+      <c r="Y46" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="Y10:Y46"/>
+    <mergeCell ref="L10:X46"/>
+    <mergeCell ref="I44:K44"/>
+    <mergeCell ref="I45:K45"/>
+    <mergeCell ref="I46:K46"/>
+    <mergeCell ref="I41:K41"/>
+    <mergeCell ref="I42:K42"/>
+    <mergeCell ref="I43:K43"/>
+    <mergeCell ref="I38:K38"/>
+    <mergeCell ref="I39:K39"/>
+    <mergeCell ref="I40:K40"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="I36:K36"/>
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I24:K24"/>
     <mergeCell ref="H10:H46"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="I9:K9"/>
@@ -4456,34 +4494,6 @@
     <mergeCell ref="I21:K21"/>
     <mergeCell ref="I16:K16"/>
     <mergeCell ref="I17:J17"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="Y10:Y46"/>
-    <mergeCell ref="L10:X46"/>
-    <mergeCell ref="I44:K44"/>
-    <mergeCell ref="I45:K45"/>
-    <mergeCell ref="I46:K46"/>
-    <mergeCell ref="I41:K41"/>
-    <mergeCell ref="I42:K42"/>
-    <mergeCell ref="I43:K43"/>
-    <mergeCell ref="I38:K38"/>
-    <mergeCell ref="I39:K39"/>
-    <mergeCell ref="I40:K40"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="I36:K36"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="I31:K31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4527,28 +4537,28 @@
       <c r="H2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
       <c r="L2" s="9" t="s">
         <v>59</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="N2" s="32" t="s">
+      <c r="N2" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32" t="s">
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
       <c r="U2" s="9" t="s">
         <v>63</v>
       </c>
@@ -4638,11 +4648,11 @@
       <c r="H9" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="I9" s="27" t="s">
+      <c r="I9" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
       <c r="L9" s="9" t="s">
         <v>93</v>
       </c>
@@ -4690,30 +4700,30 @@
       <c r="B10" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="H10" s="30" t="s">
+      <c r="H10" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="I10" s="27" t="s">
+      <c r="I10" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="30" t="s">
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
-      <c r="O10" s="30"/>
-      <c r="P10" s="30"/>
-      <c r="Q10" s="30"/>
-      <c r="R10" s="30"/>
-      <c r="S10" s="30"/>
-      <c r="T10" s="30"/>
-      <c r="U10" s="30"/>
-      <c r="V10" s="30"/>
-      <c r="W10" s="30"/>
-      <c r="X10" s="30"/>
-      <c r="Y10" s="34" t="s">
+      <c r="M10" s="32"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="32"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="32"/>
+      <c r="R10" s="32"/>
+      <c r="S10" s="32"/>
+      <c r="T10" s="32"/>
+      <c r="U10" s="32"/>
+      <c r="V10" s="32"/>
+      <c r="W10" s="32"/>
+      <c r="X10" s="32"/>
+      <c r="Y10" s="30" t="s">
         <v>125</v>
       </c>
     </row>
@@ -4721,76 +4731,76 @@
       <c r="B11" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="H11" s="30"/>
-      <c r="I11" s="28" t="s">
+      <c r="H11" s="32"/>
+      <c r="I11" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="30"/>
-      <c r="O11" s="30"/>
-      <c r="P11" s="30"/>
-      <c r="Q11" s="30"/>
-      <c r="R11" s="30"/>
-      <c r="S11" s="30"/>
-      <c r="T11" s="30"/>
-      <c r="U11" s="30"/>
-      <c r="V11" s="30"/>
-      <c r="W11" s="30"/>
-      <c r="X11" s="30"/>
-      <c r="Y11" s="34"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="32"/>
+      <c r="Q11" s="32"/>
+      <c r="R11" s="32"/>
+      <c r="S11" s="32"/>
+      <c r="T11" s="32"/>
+      <c r="U11" s="32"/>
+      <c r="V11" s="32"/>
+      <c r="W11" s="32"/>
+      <c r="X11" s="32"/>
+      <c r="Y11" s="30"/>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="H12" s="30"/>
-      <c r="I12" s="28" t="s">
+      <c r="H12" s="32"/>
+      <c r="I12" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="30"/>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="30"/>
-      <c r="R12" s="30"/>
-      <c r="S12" s="30"/>
-      <c r="T12" s="30"/>
-      <c r="U12" s="30"/>
-      <c r="V12" s="30"/>
-      <c r="W12" s="30"/>
-      <c r="X12" s="30"/>
-      <c r="Y12" s="34"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="32"/>
+      <c r="O12" s="32"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="32"/>
+      <c r="R12" s="32"/>
+      <c r="S12" s="32"/>
+      <c r="T12" s="32"/>
+      <c r="U12" s="32"/>
+      <c r="V12" s="32"/>
+      <c r="W12" s="32"/>
+      <c r="X12" s="32"/>
+      <c r="Y12" s="30"/>
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="H13" s="30"/>
-      <c r="I13" s="28" t="s">
+      <c r="H13" s="32"/>
+      <c r="I13" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="30"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="30"/>
-      <c r="P13" s="30"/>
-      <c r="Q13" s="30"/>
-      <c r="R13" s="30"/>
-      <c r="S13" s="30"/>
-      <c r="T13" s="30"/>
-      <c r="U13" s="30"/>
-      <c r="V13" s="30"/>
-      <c r="W13" s="30"/>
-      <c r="X13" s="30"/>
-      <c r="Y13" s="34"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="32"/>
+      <c r="O13" s="32"/>
+      <c r="P13" s="32"/>
+      <c r="Q13" s="32"/>
+      <c r="R13" s="32"/>
+      <c r="S13" s="32"/>
+      <c r="T13" s="32"/>
+      <c r="U13" s="32"/>
+      <c r="V13" s="32"/>
+      <c r="W13" s="32"/>
+      <c r="X13" s="32"/>
+      <c r="Y13" s="30"/>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
@@ -4799,212 +4809,219 @@
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="28" t="s">
+      <c r="H14" s="32"/>
+      <c r="I14" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="30"/>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="30"/>
-      <c r="R14" s="30"/>
-      <c r="S14" s="30"/>
-      <c r="T14" s="30"/>
-      <c r="U14" s="30"/>
-      <c r="V14" s="30"/>
-      <c r="W14" s="30"/>
-      <c r="X14" s="30"/>
-      <c r="Y14" s="34"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="32"/>
+      <c r="N14" s="32"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="32"/>
+      <c r="R14" s="32"/>
+      <c r="S14" s="32"/>
+      <c r="T14" s="32"/>
+      <c r="U14" s="32"/>
+      <c r="V14" s="32"/>
+      <c r="W14" s="32"/>
+      <c r="X14" s="32"/>
+      <c r="Y14" s="30"/>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B15" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="H15" s="30"/>
-      <c r="I15" s="33" t="s">
+      <c r="H15" s="32"/>
+      <c r="I15" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="J15" s="33"/>
-      <c r="K15" s="33"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="30"/>
-      <c r="P15" s="30"/>
-      <c r="Q15" s="30"/>
-      <c r="R15" s="30"/>
-      <c r="S15" s="30"/>
-      <c r="T15" s="30"/>
-      <c r="U15" s="30"/>
-      <c r="V15" s="30"/>
-      <c r="W15" s="30"/>
-      <c r="X15" s="30"/>
-      <c r="Y15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="32"/>
+      <c r="N15" s="32"/>
+      <c r="O15" s="32"/>
+      <c r="P15" s="32"/>
+      <c r="Q15" s="32"/>
+      <c r="R15" s="32"/>
+      <c r="S15" s="32"/>
+      <c r="T15" s="32"/>
+      <c r="U15" s="32"/>
+      <c r="V15" s="32"/>
+      <c r="W15" s="32"/>
+      <c r="X15" s="32"/>
+      <c r="Y15" s="30"/>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B16" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="H16" s="30"/>
-      <c r="I16" s="33" t="s">
+      <c r="H16" s="32"/>
+      <c r="I16" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="J16" s="33"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="30"/>
-      <c r="M16" s="30"/>
-      <c r="N16" s="30"/>
-      <c r="O16" s="30"/>
-      <c r="P16" s="30"/>
-      <c r="Q16" s="30"/>
-      <c r="R16" s="30"/>
-      <c r="S16" s="30"/>
-      <c r="T16" s="30"/>
-      <c r="U16" s="30"/>
-      <c r="V16" s="30"/>
-      <c r="W16" s="30"/>
-      <c r="X16" s="30"/>
-      <c r="Y16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="32"/>
+      <c r="Q16" s="32"/>
+      <c r="R16" s="32"/>
+      <c r="S16" s="32"/>
+      <c r="T16" s="32"/>
+      <c r="U16" s="32"/>
+      <c r="V16" s="32"/>
+      <c r="W16" s="32"/>
+      <c r="X16" s="32"/>
+      <c r="Y16" s="30"/>
     </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B17" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="H17" s="30"/>
-      <c r="I17" s="33" t="s">
+      <c r="H17" s="32"/>
+      <c r="I17" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="J17" s="33"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="30"/>
-      <c r="M17" s="30"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="30"/>
-      <c r="P17" s="30"/>
-      <c r="Q17" s="30"/>
-      <c r="R17" s="30"/>
-      <c r="S17" s="30"/>
-      <c r="T17" s="30"/>
-      <c r="U17" s="30"/>
-      <c r="V17" s="30"/>
-      <c r="W17" s="30"/>
-      <c r="X17" s="30"/>
-      <c r="Y17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="32"/>
+      <c r="N17" s="32"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="32"/>
+      <c r="Q17" s="32"/>
+      <c r="R17" s="32"/>
+      <c r="S17" s="32"/>
+      <c r="T17" s="32"/>
+      <c r="U17" s="32"/>
+      <c r="V17" s="32"/>
+      <c r="W17" s="32"/>
+      <c r="X17" s="32"/>
+      <c r="Y17" s="30"/>
     </row>
     <row r="18" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>4</v>
       </c>
-      <c r="H18" s="30"/>
-      <c r="I18" s="28" t="s">
+      <c r="H18" s="32"/>
+      <c r="I18" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="J18" s="27"/>
+      <c r="J18" s="31"/>
       <c r="K18" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="L18" s="30"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="30"/>
-      <c r="P18" s="30"/>
-      <c r="Q18" s="30"/>
-      <c r="R18" s="30"/>
-      <c r="S18" s="30"/>
-      <c r="T18" s="30"/>
-      <c r="U18" s="30"/>
-      <c r="V18" s="30"/>
-      <c r="W18" s="30"/>
-      <c r="X18" s="30"/>
-      <c r="Y18" s="34"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="32"/>
+      <c r="N18" s="32"/>
+      <c r="O18" s="32"/>
+      <c r="P18" s="32"/>
+      <c r="Q18" s="32"/>
+      <c r="R18" s="32"/>
+      <c r="S18" s="32"/>
+      <c r="T18" s="32"/>
+      <c r="U18" s="32"/>
+      <c r="V18" s="32"/>
+      <c r="W18" s="32"/>
+      <c r="X18" s="32"/>
+      <c r="Y18" s="30"/>
     </row>
     <row r="19" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>6</v>
       </c>
-      <c r="H19" s="30"/>
-      <c r="I19" s="32" t="s">
+      <c r="H19" s="32"/>
+      <c r="I19" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="J19" s="32"/>
+      <c r="J19" s="33"/>
       <c r="K19" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="L19" s="30"/>
-      <c r="M19" s="30"/>
-      <c r="N19" s="30"/>
-      <c r="O19" s="30"/>
-      <c r="P19" s="30"/>
-      <c r="Q19" s="30"/>
-      <c r="R19" s="30"/>
-      <c r="S19" s="30"/>
-      <c r="T19" s="30"/>
-      <c r="U19" s="30"/>
-      <c r="V19" s="30"/>
-      <c r="W19" s="30"/>
-      <c r="X19" s="30"/>
-      <c r="Y19" s="34"/>
+      <c r="L19" s="32"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="32"/>
+      <c r="O19" s="32"/>
+      <c r="P19" s="32"/>
+      <c r="Q19" s="32"/>
+      <c r="R19" s="32"/>
+      <c r="S19" s="32"/>
+      <c r="T19" s="32"/>
+      <c r="U19" s="32"/>
+      <c r="V19" s="32"/>
+      <c r="W19" s="32"/>
+      <c r="X19" s="32"/>
+      <c r="Y19" s="30"/>
     </row>
     <row r="20" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="30"/>
+      <c r="H20" s="32"/>
       <c r="I20" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="J20" s="32" t="s">
+      <c r="J20" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="K20" s="32"/>
-      <c r="L20" s="30"/>
-      <c r="M20" s="30"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="30"/>
-      <c r="P20" s="30"/>
-      <c r="Q20" s="30"/>
-      <c r="R20" s="30"/>
-      <c r="S20" s="30"/>
-      <c r="T20" s="30"/>
-      <c r="U20" s="30"/>
-      <c r="V20" s="30"/>
-      <c r="W20" s="30"/>
-      <c r="X20" s="30"/>
-      <c r="Y20" s="34"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="32"/>
+      <c r="N20" s="32"/>
+      <c r="O20" s="32"/>
+      <c r="P20" s="32"/>
+      <c r="Q20" s="32"/>
+      <c r="R20" s="32"/>
+      <c r="S20" s="32"/>
+      <c r="T20" s="32"/>
+      <c r="U20" s="32"/>
+      <c r="V20" s="32"/>
+      <c r="W20" s="32"/>
+      <c r="X20" s="32"/>
+      <c r="Y20" s="30"/>
     </row>
     <row r="21" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>13</v>
       </c>
-      <c r="H21" s="30"/>
+      <c r="H21" s="32"/>
       <c r="I21" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="J21" s="29" t="s">
+      <c r="J21" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="K21" s="29"/>
-      <c r="L21" s="30"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="30"/>
-      <c r="O21" s="30"/>
-      <c r="P21" s="30"/>
-      <c r="Q21" s="30"/>
-      <c r="R21" s="30"/>
-      <c r="S21" s="30"/>
-      <c r="T21" s="30"/>
-      <c r="U21" s="30"/>
-      <c r="V21" s="30"/>
-      <c r="W21" s="30"/>
-      <c r="X21" s="30"/>
-      <c r="Y21" s="34"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="32"/>
+      <c r="O21" s="32"/>
+      <c r="P21" s="32"/>
+      <c r="Q21" s="32"/>
+      <c r="R21" s="32"/>
+      <c r="S21" s="32"/>
+      <c r="T21" s="32"/>
+      <c r="U21" s="32"/>
+      <c r="V21" s="32"/>
+      <c r="W21" s="32"/>
+      <c r="X21" s="32"/>
+      <c r="Y21" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="Y10:Y21"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I19:J19"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:T2"/>
@@ -5017,13 +5034,6 @@
     <mergeCell ref="I12:K12"/>
     <mergeCell ref="I13:K13"/>
     <mergeCell ref="J21:K21"/>
-    <mergeCell ref="Y10:Y21"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I19:J19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5149,10 +5159,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B8:Q17"/>
+  <dimension ref="B8:R17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5164,46 +5174,49 @@
     <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17" style="20" customWidth="1"/>
     <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" style="20"/>
-    <col min="15" max="15" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" style="26" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="20"/>
+    <col min="16" max="16" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="F8" s="35" t="s">
+    <row r="8" spans="2:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="F8" s="38" t="s">
         <v>191</v>
       </c>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
       <c r="J8" s="24"/>
-      <c r="K8" s="35" t="s">
+      <c r="K8" s="38" t="s">
         <v>192</v>
       </c>
-      <c r="L8" s="35"/>
-      <c r="M8" s="35"/>
-      <c r="N8" s="35"/>
-      <c r="O8" s="35"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="24" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="K9" s="32" t="s">
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="38"/>
+      <c r="P8" s="38"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="24" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="K9" s="33" t="s">
         <v>193</v>
       </c>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="22"/>
-      <c r="O9" t="s">
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="33"/>
+      <c r="O9" s="22"/>
+      <c r="P9" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="G10" s="18" t="s">
         <v>182</v>
       </c>
@@ -5211,7 +5224,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="D11" s="18" t="s">
         <v>185</v>
       </c>
@@ -5230,31 +5243,34 @@
       </c>
       <c r="J11" s="22"/>
       <c r="K11" s="22" t="s">
-        <v>197</v>
-      </c>
-      <c r="L11" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="L11" s="28" t="s">
+        <v>202</v>
+      </c>
+      <c r="M11" s="22" t="s">
         <v>195</v>
       </c>
-      <c r="M11" s="22" t="s">
+      <c r="N11" s="22" t="s">
         <v>196</v>
       </c>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22" t="s">
-        <v>199</v>
-      </c>
-      <c r="Q11" s="18" t="s">
+      <c r="O11" s="22"/>
+      <c r="P11" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="R11" s="18" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" s="18" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B14" s="18"/>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
         <v>0</v>
       </c>
@@ -5271,47 +5287,51 @@
         <v>56</v>
       </c>
       <c r="J15" s="23"/>
-      <c r="K15" s="27" t="s">
+      <c r="K15" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="L15" s="27"/>
-      <c r="M15" s="27"/>
-      <c r="O15" s="30" t="s">
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="31"/>
+      <c r="P15" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="Q15" s="11" t="s">
+      <c r="R15" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>184</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H16" s="19" t="s">
         <v>181</v>
       </c>
       <c r="I16" s="21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J16" s="21"/>
       <c r="K16" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="L16" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="L16" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="M16" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="M16" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="N16" s="21"/>
-      <c r="O16" s="30"/>
-      <c r="Q16" s="21" t="s">
+      <c r="N16" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="O16" s="21"/>
+      <c r="P16" s="32"/>
+      <c r="R16" s="21" t="s">
         <v>125</v>
       </c>
     </row>
@@ -5321,10 +5341,10 @@
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="F8:I8"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="K8:O8"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="K8:P8"/>
+    <mergeCell ref="K15:N15"/>
+    <mergeCell ref="P15:P16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>